<commit_message>
More changes on Jan 28, 2019
</commit_message>
<xml_diff>
--- a/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
+++ b/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/503096727/Documents/workspace-sts-3.9.6.RELEASE/my_java_projects/java-projects/DataStructures/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599FAFDA-3C90-0841-B067-6D0F574BF18C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07167C0-5F3D-AF4A-8884-7AA44F6DDFCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33200" windowHeight="17660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="278">
   <si>
     <t>Data Structure</t>
   </si>
@@ -1433,6 +1433,42 @@
 4) Before we return the node, call this method recursively, once with argument: data, start, mid-1, assign that result to leftNode variable of type Node and then with argument data, mid+1, end and assign that resule to rightNode variable.
 5) Above wil allow each node of left and right subtree to be populated and we return root  of main BST formed via newNode variabe.
 6) Outside the if loop, return null since start was sent as more than end, so we can't do anything.</t>
+  </si>
+  <si>
+    <t>LinkedList</t>
+  </si>
+  <si>
+    <t>removeDuplicates()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) If root is null or LinkedList has only one element (i.e., root.getNextNode() == null), log and return since no duplicate data is possible there.
+2) Define three variables of Node type, current = head.getNextNode(), previous =  head and runner = null.
+3) Start a while loop with condition as while (current != null) and in that set runner to head as first thing since we want to start with that in every iteration.
+4) Start another while loop with condition as runner != current. We are going to compare every node from head to previous with current to know if there is any duplicate data from head to current or not. 
+5) In this while loop, have an if condition to check if runner became same as current (runner.getData() == current.getData()).
+6) If true on #5 above, delete the current node by setting the next node for previous to the next node of current, setting previous to current and current to the node that was next node for current earlier. Once done, don't forget to add break statement there so internal while loop ends and next iteration for outer while loop start when you reset the runner to head and start comparing it with new node that now current points to.
+7) If false on #5 above, this means we need to compare next element after runner to current now, so do runner = runner.getNextNode().
+8) When while loop finishes, check if runner could reach all the way to current, so runner == current will work here, if so, move the previous and current both by a node and you're done! </t>
+  </si>
+  <si>
+    <t>reverse()</t>
+  </si>
+  <si>
+    <t>1) If head is null or head.getNextNode() is null, nothing needs to be done, log and return.
+2) Define two pointers of Node type: previous (set to null) and current (set to head).
+3) Start a while loop with condition as current.getNextNode() != null. We want to go until last node of the list and save that to make the new head so current != null condition won't help here.
+4) First thing in the loop: save the node next to current in a variable, say next.
+5) Set the next node to current as previous so the link reverses at that point.
+6) Set previous to current and current to its next node held by variable next. End the while loop here.
+7) Outside the while loop (don't forget to) set the current which now points to last node of earlier list as new head of the list. You're done!</t>
+  </si>
+  <si>
+    <t>1) Check if that node is null or its next node is null, log and return. You will need next node to delete that node.
+2) Copy the data from next node to this node. n.setData(n.getNextNode().getData()).
+3) Set the next node to given node as the node after next node since both the given node and its next node now has same data. n.setNextNode(n.getNextNode().getNextNode()) and you're done!</t>
+  </si>
+  <si>
+    <t>deleteMiddleNodeWithMiddleNode()  Basically delete a node where you don't have the head. All you have is that node itself.</t>
   </si>
 </sst>
 </file>
@@ -1933,15 +1969,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" customWidth="1"/>
+    <col min="4" max="4" width="38.5" customWidth="1"/>
     <col min="5" max="5" width="72" customWidth="1"/>
     <col min="6" max="6" width="86.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="67.1640625" customWidth="1"/>
@@ -3071,18 +3107,20 @@
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="1:7" ht="137" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="372" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>111</v>
+        <v>271</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E72" s="2"/>
+        <v>272</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>273</v>
+      </c>
       <c r="F72" s="2" t="s">
         <v>114</v>
       </c>
@@ -3090,21 +3128,33 @@
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A73" s="9"/>
       <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
+      <c r="C73" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>275</v>
+      </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A74" s="9"/>
       <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
+      <c r="C74" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
     </row>
@@ -3117,11 +3167,15 @@
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" s="9"/>
       <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
+      <c r="C76" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>

</xml_diff>

<commit_message>
changes made on Jan 29, 2019
</commit_message>
<xml_diff>
--- a/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
+++ b/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/503096727/Documents/workspace-sts-3.9.6.RELEASE/my_java_projects/java-projects/DataStructures/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07167C0-5F3D-AF4A-8884-7AA44F6DDFCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14790C5A-F1A9-D441-8C18-1E7225F87725}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33200" windowHeight="17660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="37780" windowHeight="18360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="306">
   <si>
     <t>Data Structure</t>
   </si>
@@ -416,13 +416,6 @@
 Sum the numbers and have them represented same way as above. </t>
   </si>
   <si>
-    <t xml:space="preserve">1) Create arrays from 2 lists with elements as data from nodes.
-2) Read arrays from end, add data from last idex, mod 10000 (%) will give data for last node of result list. And division (/) by 10000 will give overflow (carryover).
-3) Save the overflow in a variable outside of for loop for array indexes left to current.
-4) Create a new node and set data in it from the result of modulo (above). If Head of result list is null, make this as head, else set this node's nextNode to head of result list. Then make this node the new head of result list.
-5) </t>
-  </si>
-  <si>
     <t>Palindrome</t>
   </si>
   <si>
@@ -717,10 +710,6 @@
     <t>BinarySearchTree</t>
   </si>
   <si>
-    <t>Height of a BST
-(Minimum Height of a Tree?)</t>
-  </si>
-  <si>
     <t>** This approach will work for any Binary Tree and not just for Binary Search Tree. A variation of this could be to find the minimum height of a tree where all we need to do is on the Step 4) where we return the result, get Math.min instead of Math.max and we will be done!</t>
   </si>
   <si>
@@ -749,17 +738,6 @@
   </si>
   <si>
     <t>MaxPathSum</t>
-  </si>
-  <si>
-    <t>Get sum of all the nodes</t>
-  </si>
-  <si>
-    <t>1) Do it via recursive function sum(Node n)
-2) Call the function with root node as argument
-3) Breaking condition: if n is null, return 0
-4) Declare two variables: leftSum and rightSum initialized to 0
-5) Do leftSum = sum(n.getLeftNode()) and rightSum = sum(n.getRightNode())
-6) return leftSum + rightSum() + n.getData();</t>
   </si>
   <si>
     <t>Note: This is similar to print all nodes, except that here we need to return sum and there we just had to print the nodes</t>
@@ -1468,7 +1446,134 @@
 3) Set the next node to given node as the node after next node since both the given node and its next node now has same data. n.setNextNode(n.getNextNode().getNextNode()) and you're done!</t>
   </si>
   <si>
-    <t>deleteMiddleNodeWithMiddleNode()  Basically delete a node where you don't have the head. All you have is that node itself.</t>
+    <t>isCyclic()</t>
+  </si>
+  <si>
+    <t>1) Check if head is null, log and return.
+2) Define two pointers of type Node: slow and fast. Also define result = false.
+3) Start a while loop with condition as fast != null &amp;&amp; fast.getNextNode() != null. The reason is, in this loop we are going to move fast twice.
+4) Move slow once and fast twice. In each iteration, check if slow becomes equal to fast. If so, set result to true and break from loop.
+5) Outside the while loop, return result.
+Note*** If you define an integer counter and increment that each time, you can know the node number where this loop starts getting into a loop.</t>
+  </si>
+  <si>
+    <t>CircularQueue</t>
+  </si>
+  <si>
+    <t>Queues</t>
+  </si>
+  <si>
+    <t>findElementIndexInCircularArray()</t>
+  </si>
+  <si>
+    <t>Remove nodes with duplicate data in a Singly LinkedList.</t>
+  </si>
+  <si>
+    <t>Reverse the nodes of a linked list. Existing Tail becomes new Head and vice versa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deleteMiddleNodeWithMiddleNode() </t>
+  </si>
+  <si>
+    <t>Delete a node where you don't have the head and that node is middle of the node. All you have is that node itself.</t>
+  </si>
+  <si>
+    <t>Detect if a LinkedList is cyclic.</t>
+  </si>
+  <si>
+    <t>Find the height of a tree</t>
+  </si>
+  <si>
+    <t>Height of a BST</t>
+  </si>
+  <si>
+    <t>Search for a given data in a BST.</t>
+  </si>
+  <si>
+    <t>Insert given data in a BST.</t>
+  </si>
+  <si>
+    <t>Print all nodes of a BST inOrder, which gives sorted results.</t>
+  </si>
+  <si>
+    <t>Find mimimum and maximum nodes of a BST.</t>
+  </si>
+  <si>
+    <t>Delete root node of a BST.</t>
+  </si>
+  <si>
+    <t>Find if a node in BST is a leaf node or not.</t>
+  </si>
+  <si>
+    <t>Count number of nodes in a BST.</t>
+  </si>
+  <si>
+    <t>If you are given an array which is already sorted. How can you most add the data to a BST in a most effifient way?</t>
+  </si>
+  <si>
+    <t>Create a Queue from a Circular Array</t>
+  </si>
+  <si>
+    <t>Create a queue using circular arrays and define following operations there:
+1) size(): returns the size
+2) enqueue(int data): adds new data to queue
+3) dequeue(): takes off a data from queue
+4) Queue should never get full. (Hint: resize it if it does)
+5) toString(): prints all elements of the queue.</t>
+  </si>
+  <si>
+    <t>Circular Arrays are arrays which is sorted by the lowest data (called "pivot point") need not be on index 0, it can be pushed to anywhere in the array depending on how many times array is sorted. We can implement a queue using a circular array where new data will always be enqueued on head and data will be dequeued from tail.
+1) Start with an array of say, int type. Define variables, head, tail and capacity variables. Initialize them using constructor where array is created of capacity sent and head and tail are initialized to zero.
+2) size() method: Compute the size of queue by size=(capacity - head + tail) % capacity. Modulo on capacity ensures we never get ArrayOutOfBounds exception since we will be moving head and tail both.
+3) enqueue(int data): 
+3a) Before we add an element, we need to check if size is not full and if so, we will have to resize the array to its double capacity and copy existing data to it. So check for if (tail + 1) % == head { resize(); }
+3b) We will add the data to tail and then increment the tail. Just ensure to mod the incremented tail by capacity and then assign it back to tail.
+4) dequeue():
+4a) We can't dequeue if the size of the queue is zero. So just check for that using the size() method we already coded and if it is zero, log and return.
+4b) We will take an element from head since queue are of FIFO types. So we will return arr[head] and then increment head by ensuring to take mod by capacity in case head falls on the extreme end of the array.
+5) resize():
+5a) create variables newCapaciy (2 * capacity), newArr (if type int and size as newCapacity), pos (if type int, initial value as zero, this will serve as indez when we populate the new array.
+5b) We need to now copy all the data in existing array beginning from head to one index before tail. So start a while loop with condition as head != tail and in this loop, do newArr[pos] = arr[head].
+5c) Then do head = (head + 1) %capacity. With this, end the while loop.
+5d) Once while loop is done, assign newCapacity to capacity, head to zero, tail to pos and arr to newArr and you're done!</t>
+  </si>
+  <si>
+    <t>sum()</t>
+  </si>
+  <si>
+    <t>Get sum of all nodes.</t>
+  </si>
+  <si>
+    <t>Similar to print(), maintain a variable and keep on getting the sum in that variable.</t>
+  </si>
+  <si>
+    <t>Stacks</t>
+  </si>
+  <si>
+    <t>RemoveRedundantBrackets</t>
+  </si>
+  <si>
+    <t>removeParantheses()</t>
+  </si>
+  <si>
+    <t>StackWithDoublyEndedLinkedList</t>
+  </si>
+  <si>
+    <t>Create a stack using double ended linked list.</t>
+  </si>
+  <si>
+    <t>Create a stack using double ended linked list and provide following operations there:
+1) getSize()
+2) push: adds an element to stack
+3) pop(): returns last inserted element and removes it from stack
+4) peek(): returns last inserted element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Define variables of type DoublyEndedLinkedList (custom type or can use a Deque), top and size of types int.
+2) Use constructor to initialize them. DBLyEndedLinkedList to new object, top to -1 and size to zero.
+3) For size(), just return the current size.
+4) push(int data): insert the data at the head using insertAtHead() already coded at DBLyEndedLinkedList and increment size and top.
+5) pop(): </t>
   </si>
 </sst>
 </file>
@@ -1967,10 +2072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="C87" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1978,8 +2083,8 @@
     <col min="1" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.5" customWidth="1"/>
-    <col min="5" max="5" width="72" customWidth="1"/>
-    <col min="6" max="6" width="86.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.33203125" customWidth="1"/>
+    <col min="6" max="6" width="105.1640625" customWidth="1"/>
     <col min="7" max="7" width="67.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1999,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
@@ -2008,24 +2113,24 @@
         <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -2035,23 +2140,23 @@
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="340" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>8</v>
@@ -2067,7 +2172,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>14</v>
@@ -2086,10 +2191,10 @@
         <v>17</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -2097,19 +2202,19 @@
       <c r="A7" s="9"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -2262,34 +2367,34 @@
       <c r="A18" s="9"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="255" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -2303,7 +2408,7 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>11</v>
@@ -2313,16 +2418,16 @@
       <c r="A21" s="9"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G21" s="2"/>
     </row>
@@ -2330,19 +2435,19 @@
       <c r="A22" s="9"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2355,7 +2460,7 @@
         <v>17</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>19</v>
@@ -2368,38 +2473,38 @@
       <c r="A24" s="9"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="255" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -2426,7 +2531,7 @@
         <v>24</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -2444,10 +2549,10 @@
         <v>29</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>27</v>
@@ -2463,7 +2568,7 @@
         <v>36</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>37</v>
@@ -2521,16 +2626,16 @@
       <c r="A33" s="9"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G33" s="2"/>
     </row>
@@ -2540,54 +2645,54 @@
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="E35" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="323" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G36" s="2"/>
     </row>
@@ -2595,31 +2700,31 @@
       <c r="A37" s="9"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G38" s="2"/>
     </row>
@@ -2633,10 +2738,10 @@
         <v>61</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="G39" s="2"/>
     </row>
@@ -2664,19 +2769,19 @@
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="238" x14ac:dyDescent="0.2">
@@ -2685,16 +2790,16 @@
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="F43" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G43" s="2"/>
     </row>
@@ -2702,19 +2807,19 @@
       <c r="A44" s="9"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -2732,16 +2837,16 @@
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="G46" s="2"/>
     </row>
@@ -2751,16 +2856,16 @@
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="G47" s="2"/>
     </row>
@@ -2776,10 +2881,10 @@
         <v>46</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G48" s="2"/>
     </row>
@@ -2789,16 +2894,16 @@
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G49" s="2"/>
     </row>
@@ -2808,19 +2913,19 @@
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="4" customFormat="1" ht="272" x14ac:dyDescent="0.2">
@@ -2829,16 +2934,16 @@
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G51" s="3"/>
     </row>
@@ -2848,16 +2953,16 @@
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G52" s="2"/>
     </row>
@@ -2876,7 +2981,7 @@
         <v>40</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>40</v>
@@ -2892,10 +2997,10 @@
         <v>43</v>
       </c>
       <c r="E54" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="G54" s="2"/>
     </row>
@@ -2903,16 +3008,16 @@
       <c r="A55" s="9"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G55" s="2"/>
     </row>
@@ -2926,7 +3031,7 @@
         <v>47</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>49</v>
@@ -2937,16 +3042,16 @@
       <c r="A57" s="9"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G57" s="2"/>
     </row>
@@ -3048,7 +3153,7 @@
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>106</v>
@@ -3107,67 +3212,79 @@
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="1:7" ht="372" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="323" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>114</v>
+        <v>269</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A73" s="9"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="F73" s="2"/>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A74" s="9"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="F74" s="2"/>
+        <v>281</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>272</v>
+      </c>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A75" s="9"/>
       <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
+      <c r="C75" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>274</v>
+      </c>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A76" s="9"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
@@ -3180,171 +3297,201 @@
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="G77" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="G77" s="2"/>
     </row>
     <row r="78" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A78" s="9"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F78" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>256</v>
+      </c>
       <c r="G78" s="2"/>
     </row>
-    <row r="79" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A79" s="9"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F79" s="2"/>
+        <v>286</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="G79" s="2"/>
     </row>
-    <row r="80" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A80" s="9"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="F80" s="2"/>
+        <v>287</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>263</v>
+      </c>
       <c r="G80" s="2"/>
     </row>
     <row r="81" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A81" s="9"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D81" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G81" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G81" s="2"/>
-    </row>
-    <row r="82" spans="1:7" s="4" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:7" s="4" customFormat="1" ht="356" x14ac:dyDescent="0.2">
       <c r="A82" s="9"/>
       <c r="B82" s="3"/>
       <c r="C82" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="F82" s="3"/>
+        <v>289</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>258</v>
+      </c>
       <c r="G82" s="3"/>
     </row>
-    <row r="83" spans="1:7" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="9"/>
       <c r="B83" s="3"/>
       <c r="C83" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="F83" s="3"/>
+        <v>290</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>260</v>
+      </c>
       <c r="G83" s="3"/>
     </row>
     <row r="84" spans="1:7" s="4" customFormat="1" ht="170" x14ac:dyDescent="0.2">
       <c r="A84" s="9"/>
       <c r="B84" s="3"/>
       <c r="C84" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="F84" s="3"/>
+        <v>291</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>262</v>
+      </c>
       <c r="G84" s="3"/>
     </row>
-    <row r="85" spans="1:7" s="4" customFormat="1" ht="238" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" s="4" customFormat="1" ht="204" x14ac:dyDescent="0.2">
       <c r="A85" s="9"/>
       <c r="B85" s="3"/>
       <c r="C85" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="F85" s="3"/>
+        <v>292</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>266</v>
+      </c>
       <c r="G85" s="3"/>
     </row>
-    <row r="86" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="9"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>194</v>
+        <v>296</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>195</v>
+        <v>297</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G86" s="2"/>
-    </row>
-    <row r="87" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A87" s="9"/>
+        <v>298</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="9" t="s">
+        <v>276</v>
+      </c>
       <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
+      <c r="C87" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="G87" s="2"/>
     </row>
     <row r="88" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -3365,48 +3512,64 @@
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
     </row>
-    <row r="90" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A90" s="9"/>
+    <row r="90" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A90" s="9" t="s">
+        <v>299</v>
+      </c>
       <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
+      <c r="C90" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>305</v>
+      </c>
       <c r="G90" s="2"/>
     </row>
     <row r="91" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A91" s="9"/>
       <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
+      <c r="C91" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>301</v>
+      </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
     </row>
-    <row r="92" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A92" s="9" t="s">
+    <row r="92" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A92" s="9"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+    </row>
+    <row r="93" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="A93" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2" t="s">
+      <c r="B93" s="2"/>
+      <c r="C93" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="D93" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2" t="s">
+      <c r="E93" s="2"/>
+      <c r="F93" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G92" s="2"/>
-    </row>
-    <row r="93" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A93" s="9"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
       <c r="G93" s="2"/>
     </row>
     <row r="94" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -3427,55 +3590,53 @@
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
     </row>
-    <row r="96" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A96" s="9" t="s">
+    <row r="96" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A96" s="9"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+    </row>
+    <row r="97" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A97" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E96" s="2"/>
-      <c r="F96" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A97" s="9"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2" t="s">
-        <v>216</v>
+        <v>101</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A98" s="9"/>
       <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
+      <c r="C98" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-    </row>
-    <row r="99" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A99" s="9" t="s">
-        <v>130</v>
-      </c>
+      <c r="F98" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A99" s="9"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -3483,8 +3644,10 @@
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
     </row>
-    <row r="100" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A100" s="9"/>
+    <row r="100" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="A100" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -3492,16 +3655,25 @@
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
     </row>
-    <row r="101" spans="1:7" ht="40" x14ac:dyDescent="0.2">
-      <c r="A101" s="9" t="s">
-        <v>131</v>
-      </c>
+    <row r="101" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A101" s="9"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
+    </row>
+    <row r="102" spans="1:7" ht="40" x14ac:dyDescent="0.2">
+      <c r="A102" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Some maintenance on existing algos
</commit_message>
<xml_diff>
--- a/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
+++ b/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/503096727/Documents/workspace-sts-3.9.6.RELEASE/my_java_projects/java-projects/DataStructures/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asheshsingh/Documents/workspace-sts-3.9.6.RELEASE/java-projects/DataStructures/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14790C5A-F1A9-D441-8C18-1E7225F87725}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA332CB3-7036-7E4D-A3B1-993C55C8F42C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="37780" windowHeight="18360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -674,21 +674,6 @@
   </si>
   <si>
     <t>largestCommonSubstringOptimized1(String str1, String str2)</t>
-  </si>
-  <si>
-    <t>Here, time complexity will be of O(n). We need a storage of 256
-  * characters but that should not be the big deal
-  * Solution: 
-  * a) Define an int array of size 256. It can be 128 if pure ascii is contained by strings 
-  * b) Initialize array by -1 for each elements. You can avoid this step if can come with
-  *    special index for index 0 for str1 
-  * c) loop through each chars of str1 and store their indices in array. Index of array will
-  *    be ascii values of str1 chars 
-  * d) Loop through str2 chars, check if a char is present in str1, if not continue checking
-  * e) If chars match, save the position of char position and define another variable to check subsequent substrings 
-  * f) Do a while loop to keep checking how far we can go, i.e., how large of substring is common from position we saved 
-  * g) when while loop exits, check length of substring found, get to max one
-  *    and store the resulting string to return</t>
   </si>
   <si>
     <t>Find out if String has duplicate chars and also remove them.</t>
@@ -1574,6 +1559,17 @@
 3) For size(), just return the current size.
 4) push(int data): insert the data at the head using insertAtHead() already coded at DBLyEndedLinkedList and increment size and top.
 5) pop(): </t>
+  </si>
+  <si>
+    <t>Here, time complexity will be of O(n). We need a storage of 256 characters but that should not be the big deal
+ * Solution: 
+ a) Define an int array of size 256. It can be 128 if pure ascii is contained by strings 
+ b) Initialize array by -1 for each elements. You can avoid this step if can come with special index for index 0 for str1 
+ c) loop through each chars of str1 and store their indices in array. Index of array will be ascii values of str1 chars 
+ d) Loop through str2 chars, check if a char is present in str1, if not continue checking
+ e) If chars match, save the position of char position and define another variable to check subsequent substrings 
+ f) Do a while loop to keep checking how far we can go, i.e., how large of substring is common from position we saved 
+ g) when while loop exits, check length of substring found, get to max one and store the resulting string to return</t>
   </si>
 </sst>
 </file>
@@ -1747,13 +1743,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2074,8 +2070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C87" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2089,15 +2085,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2144,7 +2140,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="340" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>138</v>
@@ -2156,14 +2152,14 @@
         <v>157</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="83" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>12</v>
@@ -2182,7 +2178,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="83" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>16</v>
@@ -2191,15 +2187,15 @@
         <v>17</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="238" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>153</v>
@@ -2218,7 +2214,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>65</v>
@@ -2235,7 +2231,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
@@ -2248,7 +2244,7 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -2261,7 +2257,7 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -2276,7 +2272,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
@@ -2291,7 +2287,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
@@ -2306,7 +2302,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
@@ -2321,7 +2317,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
         <v>85</v>
@@ -2336,7 +2332,7 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
         <v>88</v>
@@ -2349,7 +2345,7 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>90</v>
@@ -2364,7 +2360,7 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
         <v>121</v>
@@ -2381,7 +2377,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="255" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
         <v>125</v>
@@ -2398,7 +2394,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
         <v>9</v>
@@ -2415,7 +2411,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="238" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
         <v>142</v>
@@ -2427,31 +2423,31 @@
         <v>146</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="272" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>249</v>
-      </c>
     </row>
     <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
         <v>16</v>
@@ -2470,7 +2466,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
         <v>150</v>
@@ -2482,33 +2478,33 @@
         <v>149</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="255" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>234</v>
-      </c>
     </row>
     <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
         <v>20</v>
@@ -2525,7 +2521,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
         <v>24</v>
@@ -2540,7 +2536,7 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="299" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
+      <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
         <v>28</v>
@@ -2559,7 +2555,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="293" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
+      <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
         <v>34</v>
@@ -2578,7 +2574,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
+      <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
         <v>53</v>
@@ -2593,7 +2589,7 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
         <v>54</v>
@@ -2608,7 +2604,7 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
         <v>55</v>
@@ -2623,7 +2619,7 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
+      <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
         <v>131</v>
@@ -2632,15 +2628,15 @@
         <v>132</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="2"/>
@@ -2661,7 +2657,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
+      <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
         <v>121</v>
@@ -2679,8 +2675,8 @@
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="323" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
+    <row r="36" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
         <v>178</v>
@@ -2689,15 +2685,15 @@
         <v>179</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>180</v>
+        <v>305</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
+      <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
         <v>114</v>
@@ -2714,7 +2710,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
+      <c r="A38" s="8"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
         <v>118</v>
@@ -2729,7 +2725,7 @@
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" ht="372" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
+      <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
         <v>60</v>
@@ -2738,15 +2734,15 @@
         <v>61</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
+      <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2755,7 +2751,7 @@
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
+      <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2764,12 +2760,12 @@
       <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" ht="340" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>32</v>
@@ -2778,33 +2774,33 @@
         <v>158</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="238" x14ac:dyDescent="0.2">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A44" s="9"/>
+      <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
         <v>163</v>
@@ -2823,7 +2819,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A45" s="9"/>
+      <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2831,46 +2827,46 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A46" s="9" t="s">
+    <row r="46" spans="1:7" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="G46" s="2"/>
     </row>
     <row r="47" spans="1:7" ht="323" x14ac:dyDescent="0.2">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>241</v>
-      </c>
       <c r="F47" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G47" s="2"/>
     </row>
     <row r="48" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B48" s="2"/>
@@ -2881,93 +2877,93 @@
         <v>46</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" ht="323" x14ac:dyDescent="0.2">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
+    <row r="50" spans="1:7" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A50" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>222</v>
-      </c>
     </row>
     <row r="51" spans="1:7" s="4" customFormat="1" ht="272" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E51" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>225</v>
-      </c>
       <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" ht="221" x14ac:dyDescent="0.2">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="G52" s="2"/>
     </row>
     <row r="53" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B53" s="2"/>
@@ -2988,7 +2984,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="121" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="9"/>
+      <c r="A54" s="8"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
         <v>42</v>
@@ -3005,24 +3001,24 @@
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="1:7" ht="215" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="9"/>
+      <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F55" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="G55" s="2"/>
     </row>
     <row r="56" spans="1:7" ht="170" x14ac:dyDescent="0.2">
-      <c r="A56" s="9"/>
+      <c r="A56" s="8"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
         <v>48</v>
@@ -3031,7 +3027,7 @@
         <v>47</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>49</v>
@@ -3039,24 +3035,24 @@
       <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:7" ht="204" x14ac:dyDescent="0.2">
-      <c r="A57" s="9"/>
+      <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F57" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="G57" s="2"/>
     </row>
     <row r="58" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A58" s="9"/>
+      <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
         <v>50</v>
@@ -3070,8 +3066,8 @@
       </c>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A59" s="9"/>
+    <row r="59" spans="1:7" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
         <v>57</v>
@@ -3086,11 +3082,11 @@
       <c r="G59" s="2"/>
     </row>
     <row r="60" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A60" s="10"/>
+      <c r="A60" s="9"/>
       <c r="G60" s="2"/>
     </row>
     <row r="61" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A61" s="9"/>
+      <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -3099,7 +3095,7 @@
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A62" s="9"/>
+      <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -3108,7 +3104,7 @@
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A63" s="9"/>
+      <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -3117,7 +3113,7 @@
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A64" s="9"/>
+      <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -3126,7 +3122,7 @@
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A65" s="9" t="s">
+      <c r="A65" s="8" t="s">
         <v>93</v>
       </c>
       <c r="B65" s="2"/>
@@ -3143,7 +3139,7 @@
       <c r="G65" s="2"/>
     </row>
     <row r="66" spans="1:7" ht="289" x14ac:dyDescent="0.2">
-      <c r="A66" s="9"/>
+      <c r="A66" s="8"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
         <v>97</v>
@@ -3153,14 +3149,14 @@
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A67" s="9"/>
+      <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
         <v>99</v>
@@ -3171,7 +3167,7 @@
       <c r="G67" s="2"/>
     </row>
     <row r="68" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A68" s="9"/>
+      <c r="A68" s="8"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
         <v>107</v>
@@ -3186,7 +3182,7 @@
       <c r="G68" s="2"/>
     </row>
     <row r="69" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A69" s="9"/>
+      <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -3195,7 +3191,7 @@
       <c r="G69" s="2"/>
     </row>
     <row r="70" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A70" s="9"/>
+      <c r="A70" s="8"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -3204,7 +3200,7 @@
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A71" s="9"/>
+      <c r="A71" s="8"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
@@ -3213,79 +3209,79 @@
       <c r="G71" s="2"/>
     </row>
     <row r="72" spans="1:7" ht="323" x14ac:dyDescent="0.2">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="8" t="s">
         <v>110</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="E72" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A73" s="9"/>
+      <c r="A73" s="8"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D73" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="G73" s="2"/>
     </row>
     <row r="74" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A74" s="9"/>
+      <c r="A74" s="8"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D74" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E74" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="F74" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G74" s="2"/>
     </row>
     <row r="75" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A75" s="9"/>
+      <c r="A75" s="8"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D75" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E75" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="G75" s="2"/>
     </row>
     <row r="76" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A76" s="9"/>
+      <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
         <v>111</v>
@@ -3298,204 +3294,204 @@
       <c r="G76" s="2"/>
     </row>
     <row r="77" spans="1:7" ht="136" x14ac:dyDescent="0.2">
-      <c r="A77" s="9" t="s">
-        <v>183</v>
+      <c r="A77" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="G77" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="78" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A78" s="9"/>
+      <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D78" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E78" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="G78" s="2"/>
     </row>
     <row r="79" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A79" s="9"/>
+      <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G79" s="2"/>
     </row>
     <row r="80" spans="1:7" ht="170" x14ac:dyDescent="0.2">
-      <c r="A80" s="9"/>
+      <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G80" s="2"/>
     </row>
     <row r="81" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A81" s="9"/>
+      <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D81" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="F81" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="G81" s="2" t="s">
-        <v>189</v>
-      </c>
     </row>
     <row r="82" spans="1:7" s="4" customFormat="1" ht="356" x14ac:dyDescent="0.2">
-      <c r="A82" s="9"/>
+      <c r="A82" s="8"/>
       <c r="B82" s="3"/>
       <c r="C82" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G82" s="3"/>
     </row>
     <row r="83" spans="1:7" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A83" s="9"/>
+      <c r="A83" s="8"/>
       <c r="B83" s="3"/>
       <c r="C83" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D83" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="E83" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>260</v>
-      </c>
       <c r="G83" s="3"/>
     </row>
     <row r="84" spans="1:7" s="4" customFormat="1" ht="170" x14ac:dyDescent="0.2">
-      <c r="A84" s="9"/>
+      <c r="A84" s="8"/>
       <c r="B84" s="3"/>
       <c r="C84" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D84" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="F84" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="E84" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>262</v>
-      </c>
       <c r="G84" s="3"/>
     </row>
     <row r="85" spans="1:7" s="4" customFormat="1" ht="204" x14ac:dyDescent="0.2">
-      <c r="A85" s="9"/>
+      <c r="A85" s="8"/>
       <c r="B85" s="3"/>
       <c r="C85" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D85" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="F85" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="E85" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>266</v>
-      </c>
       <c r="G85" s="3"/>
     </row>
     <row r="86" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="9"/>
+      <c r="A86" s="8"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G86" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>192</v>
-      </c>
     </row>
     <row r="87" spans="1:7" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="9" t="s">
-        <v>276</v>
+      <c r="A87" s="8" t="s">
+        <v>275</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D87" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="F87" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="F87" s="2" t="s">
-        <v>295</v>
-      </c>
       <c r="G87" s="2"/>
     </row>
     <row r="88" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A88" s="9"/>
+      <c r="A88" s="8"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
@@ -3504,7 +3500,7 @@
       <c r="G88" s="2"/>
     </row>
     <row r="89" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A89" s="9"/>
+      <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
@@ -3513,50 +3509,50 @@
       <c r="G89" s="2"/>
     </row>
     <row r="90" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A90" s="9" t="s">
-        <v>299</v>
+      <c r="A90" s="8" t="s">
+        <v>298</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="E90" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="E90" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F90" s="2" t="s">
-        <v>305</v>
-      </c>
       <c r="G90" s="2"/>
     </row>
     <row r="91" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A91" s="9"/>
+      <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D91" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
     </row>
     <row r="92" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A92" s="9"/>
+      <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
     </row>
     <row r="93" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A93" s="9" t="s">
+      <c r="A93" s="8" t="s">
         <v>62</v>
       </c>
       <c r="B93" s="2"/>
@@ -3573,7 +3569,7 @@
       <c r="G93" s="2"/>
     </row>
     <row r="94" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A94" s="9"/>
+      <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
@@ -3582,7 +3578,7 @@
       <c r="G94" s="2"/>
     </row>
     <row r="95" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A95" s="9"/>
+      <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
@@ -3591,7 +3587,7 @@
       <c r="G95" s="2"/>
     </row>
     <row r="96" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A96" s="9"/>
+      <c r="A96" s="8"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
@@ -3600,7 +3596,7 @@
       <c r="G96" s="2"/>
     </row>
     <row r="97" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A97" s="9" t="s">
+      <c r="A97" s="8" t="s">
         <v>102</v>
       </c>
       <c r="B97" s="2"/>
@@ -3619,7 +3615,7 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A98" s="9"/>
+      <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2" t="s">
         <v>104</v>
@@ -3629,14 +3625,14 @@
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G98" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="G98" s="2" t="s">
-        <v>213</v>
-      </c>
     </row>
     <row r="99" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A99" s="9"/>
+      <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
@@ -3645,7 +3641,7 @@
       <c r="G99" s="2"/>
     </row>
     <row r="100" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A100" s="9" t="s">
+      <c r="A100" s="8" t="s">
         <v>129</v>
       </c>
       <c r="B100" s="2"/>
@@ -3656,7 +3652,7 @@
       <c r="G100" s="2"/>
     </row>
     <row r="101" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A101" s="9"/>
+      <c r="A101" s="8"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
@@ -3665,7 +3661,7 @@
       <c r="G101" s="2"/>
     </row>
     <row r="102" spans="1:7" ht="40" x14ac:dyDescent="0.2">
-      <c r="A102" s="9" t="s">
+      <c r="A102" s="8" t="s">
         <v>130</v>
       </c>
       <c r="B102" s="2"/>

</xml_diff>

<commit_message>
Added TopK Elements MinHeap Algo
</commit_message>
<xml_diff>
--- a/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
+++ b/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asheshsingh/Documents/workspace-sts-3.9.6.RELEASE/java-projects/DataStructures/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA332CB3-7036-7E4D-A3B1-993C55C8F42C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87A1A5D-E281-7246-A710-4BFA26EFB6BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3680" yWindow="460" windowWidth="33600" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1564,12 +1564,13 @@
     <t>Here, time complexity will be of O(n). We need a storage of 256 characters but that should not be the big deal
  * Solution: 
  a) Define an int array of size 256. It can be 128 if pure ascii is contained by strings 
- b) Initialize array by -1 for each elements. You can avoid this step if can come with special index for index 0 for str1 
- c) loop through each chars of str1 and store their indices in array. Index of array will be ascii values of str1 chars 
- d) Loop through str2 chars, check if a char is present in str1, if not continue checking
- e) If chars match, save the position of char position and define another variable to check subsequent substrings 
- f) Do a while loop to keep checking how far we can go, i.e., how large of substring is common from position we saved 
- g) when while loop exits, check length of substring found, get to max one and store the resulting string to return</t>
+ b) Initialize first element of this array by -1. Rest of them by default will have 0 and we are good with them.
+ c) loop through each chars of str1 and store their indices in array. Index of array will be ascii values of str1 chars: 
+     arr[str1.charAt(i)] = i
+ d) Loop through str2 chars, check if a char is present in str1 by checking arr[ch] &lt;= 0, if not continue checking.
+ e) If chars match, save the position of char position and define another variable (beginIndex = j) to check subsequent substrings. Define a new variable endIndex as beginIndex + 1. 
+ f) Do a while loop with condition as endIndex should be &lt;= length of str2 to keep checking if str1 contans the substring from str2 begining from beginIndex to endIndex and each time this true, increment the endIndex. See how far we can go, i.e., how large of substring is common from position we saved earlier as beginIndex. Break from while loop whenever there is no match.
+ g) when while loop exits, check length of substring found, compare the maxLength of the result we got so far, same the new max, if bigger one is found and store the resulting string to return finally.</t>
   </si>
 </sst>
 </file>
@@ -2675,7 +2676,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">

</xml_diff>

<commit_message>
Updated Practice Also sheet and some refactoring
</commit_message>
<xml_diff>
--- a/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
+++ b/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asheshsingh/Documents/workspace-sts-3.9.6.RELEASE/java-projects/DataStructures/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87A1A5D-E281-7246-A710-4BFA26EFB6BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF23F0B-FC26-FF47-9330-A3A137101B20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="460" windowWidth="33600" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="320">
   <si>
     <t>Data Structure</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>findPairsWithGivenSum(int[] array, int sum)</t>
-  </si>
-  <si>
-    <t>This approach can be used to find all the 3 some numbers too which have sum as given sum. For this take I, k, j indexes where k=mid point. In while loop, move k first depending on sum &gt; or &lt; given sum. Once reach first or last element, then increment I or decrement j (depending on which one k touches, recompute k as new mid point and repeat the steps.</t>
   </si>
   <si>
     <t>BalancedParantheses</t>
@@ -192,10 +189,6 @@
     <t>ReverseIntegerClient - two classes</t>
   </si>
   <si>
-    <t>Method 1: Have a for loop, do modulo everytime, extract last digit and append to a string. Then convert this string to integer by above method on Row # 3, class Algorithms. Take care of boundary conditions and save a boolean as isNegative, convert number as positive and use that at the end to convert the integer back to negative before returning.
-Method 2: Optimized one, as this does not need temporary storage of reverse of number. This directly converts number to reverse number. Underlying theory is, say you have a number 23, how will you add an extra digit at the end, say 4? You'll multiply it by 10 (i.e., promote the current unit digit to 10th place) and then add the new digit to it. That'll be 23 * 10 + 4 = 234! So basically, define a variable as result = 0, in while loop (till num == 0), get modulo and do result = (result * 10 + modulo) everytime in the loop. Finally return the result.</t>
-  </si>
-  <si>
     <t>SwapTwoNumbers</t>
   </si>
   <si>
@@ -214,9 +207,6 @@
   </si>
   <si>
     <t>TopPageVisitedSquence</t>
-  </si>
-  <si>
-    <t>Check STS DataStructures project for approach.</t>
   </si>
   <si>
     <t>BitManupulation</t>
@@ -527,9 +517,6 @@
     <t>Tips to Remember / Future Notes</t>
   </si>
   <si>
-    <t>Find count of triplets in an array with given Sum</t>
-  </si>
-  <si>
     <t>Given strings like these, find if parantheses are balanced or not: "[(5+6)*{6*7}[(7+9)]]"</t>
   </si>
   <si>
@@ -748,22 +735,6 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">Brute Force Solution:
-1. For every number, move to right, look for first greater number, append to result, if they do, else append ", _". 
-2) For last number simply append ", _".
-Better Solution:
-    a) Create a stack, push first element to it. Iterate from 2nd element and call that one "next"
-    b) pop from stack, call that "element", compare next to element, if next is bigger, send "element -&gt; next" to result collection (or print),
-    c) Keep popping from stack and comparing to next and send to output till next is smaller,
-    d) If stack gets empty in between, break and stop comparing,
-    e) Send the "element" which turns to be bigger than 'next' back to stack,
-    f) Push next to stack before an iteration ends so its current array element (next's) pair can also be found,
-    g) Once loop finishes, check if stack is not empty, those elements don't have next bigger element, so 
-        print them as "element -&gt; -1"
-(Note** Per Geeksforgeeks, later solution is O(N), more optimized but I found this to be taking more time than above. May be due to stack operation overhead? Find out more!
-</t>
-  </si>
-  <si>
     <t>Reverse a given integer.</t>
   </si>
   <si>
@@ -771,38 +742,10 @@
 Example: A = {1, 2, 3}, B = {2, 4, 4}, C = {1, 2, 4}, targetSum = 5, Result = [[1, 2, 2], [2, 2, 1]]</t>
   </si>
   <si>
-    <t>BigO: O(n^2):
-1) Interate through smaller array and inside that iterate through next bigger array, for each element combinations of both, find the diffrence of their sum with given sum. Then do a binary search on 3rd (largest size) array to check if they have a number equal to the difference we computed in nested for loops. If so, mark that 3-some for one of your results. Proceed with rest of elements of first 2 arrays.</t>
-  </si>
-  <si>
     <t>CircularArrayNumRotation</t>
   </si>
   <si>
     <t>CircularArraySearch</t>
-  </si>
-  <si>
-    <t>Do binary search. In the while (low &lt;= high), once we check that mid element is not what we are looking for, we will have following cases there:
-Case 1: If array between low and high indexes is not circular a this point, i.e., everything is sorted,
-Case 1.a: Move high to right before mid or low to right after mid depending on how num compares with A[mid].
-Case 2: if left array is sorted. This will allow us to check if num lies in that sub array. 
-Case 2.a: if num lies between two ends of left sub array, move high to right before mid, OR 
-Case 2.b: num has to be on right sub array, move low to right after mid.
-Case 3: if right array is sorted, we will be able to check if num is present there 
-Case 3.a: if num lies between two ends of right sub array, move low to right after mid, OR 
-Case 3.b: if num has to be on left sub array, move high to right before mid.</t>
-  </si>
-  <si>
-    <t>1) CircularArrays are sorted arrays with min element need not be the 0th element. Min element is called "Pivot Element" and its distance from 0th element tells us how many times this circular array is rotated.
-2) in rotated array, to find previous index, we should subtract 1, add the array length and then get a modulo with array length. This will help if index was 0, then (0 - 1 + length) % length will give us length - 1 as resulting index, which will be the last index of array, which makes perfect sense in case of rotated array. This will help us avoid ArrayOutOfBounds Exception.
-3) Same as above, next index = (current index + 1) % array length.
-4) Keeping above properties in mind, do a binary search using a while loop with while loop as (low &lt;= high) condition. If mid is pivot, return mid index. If not, decrement high to mid-1 or increase low to mid+1.
-5) At the beginning of while loop, make sure to check for this and return low if array is already sorted:
-// If first element is lower then last element of this (sub) array, first index is the pivot
-   if (array[low] &lt;= array[high]) {
-    result = low;
-    return result;
-}
-6) just take care to use &lt;= or &gt;= during checks above, else you might miss a corner case getting to result.</t>
   </si>
   <si>
     <t>search(int[] A, int num) {</t>
@@ -895,17 +838,6 @@
   </si>
   <si>
     <t>Find common elements in 3 sorted arrays</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Solution:
-1) Do one while loop with condition as no array should not go out of bounds.
-2) Grab elements from 3 arrays at their corresponding indices as e1 = arr1[i], e2 = arr2[j], etc.
-3) We now have following cases here:
-   a) All elements are same: (e1 == e2 &amp;&amp; e2 == e3). Add this element to result list.
-   b) e1 &gt; e2 -&gt; increase j and within this check if e2 &gt; e3 -&gt; increase k. if e2 &lt; e3 -&gt; increase j.
-   c) e1 &lt; e2 -&gt; increase i and within this check if e2 &lt; e3 -&gt; increase j. if e2 &gt; e3 -&gt; increase k.
-Note** With above, there is no need to check e1 with e3 since that is taken care in above conditions. if e1 &gt; e2 &amp;&amp; e2 &gt; e3, then e1 &gt; e3.
-Note** For &gt; or &lt; comparisons, don't rely on doing else only, add the conditions explicitly like e1 &gt; e2 else e2 &gt; e1. This will help not increment the indices when elements are equal and then capture them as part of your result with case a) above!</t>
   </si>
   <si>
     <t>CommonElementsFromSortedArray</t>
@@ -1118,31 +1050,508 @@
 of consecutive elements.</t>
   </si>
   <si>
+    <t>In this the key is, we need consecutive integers at any index but in the forward direction.</t>
+  </si>
+  <si>
+    <t>RemoveDuplicatesIntArray</t>
+  </si>
+  <si>
+    <t>removeDuplicatesIntArray(int [] A)</t>
+  </si>
+  <si>
+    <t>Remove duplicates from an int array without using any extra storage (map, etc). The algorithm needs to be very efficient.</t>
+  </si>
+  <si>
+    <t>Print2DArraySnakeOrder</t>
+  </si>
+  <si>
+    <t>print2DArraySnakeOrderHorizontal(int[][] A, int m, int n),
+print2DArraySnakeOrderVertical(int[][] A, int m, int n)</t>
+  </si>
+  <si>
+    <t>For a 2D Array, print the elements in "snake order horizontal" and then "snake order vertical".
+Example Input:
+A mxn 2D array, 
+A = { 
+   {1, 2, 3}, 
+   {4, 5, 6},
+   {7, 8, 9}, 
+   {10, 11, 12}
+ };
+Output:
+a) Snake order horizontal: 1, 2, 3, 6, 5, 4, 7, 8, 9, 12, 11, 10
+b) Snake order vertical: 1, 4, 7, 10, 11, 8, 5, 2, 3, 6, 9, 12</t>
+  </si>
+  <si>
+    <t>Print 2D Array in Spiral Order.</t>
+  </si>
+  <si>
     <t>Solution:
-1) Create an empty hash.
+A) Snake Horizontal Order:
+1) We basically need to print m rows by varying the direction every time, left to right (to start with) and alternate that
+   every time.
+2) Take a variable k and assign this to -1.
+3) Start first for loop and in that vary i from 0 to m-1.
+4) Inside above loop, do k *= -1 (basically toggle it from -1 to +1 in every loop.
+5) Have 2 variation of inner for-loop based on whether k &gt; 0 or not, vary j from 0 to n-1 or n-1 to 0 and print A[j][j];
+B) Snake Vertical Order:
+1) Do exactly reverse of above. Here we need to print columns from 0 to n by alternating the direction every time.
+2) Take a variable k and assign this to -1.
+3) Start first for loop and in that vary j from 0 to n-1.
+4) Inside above loop, do k *= -1 (basically toggle it from -1 to +1 in every loop.
+5) Have 2 variation of inner for-loop based on whether k &gt; 0 or not, vary i from 0 to m-1 or m-1 to 0 and print A[j][j];</t>
+  </si>
+  <si>
+    <t>1) Define variables like topRow=0, rightCol=n-1, bottomRow=m-1, leftCol=0. Also define a variable as dir, which will indicate directions: 0 for left to right, 1 for top to bottom, 2 for right to left and 3 for bottom to top. Start with dir = 0;
+2) Have a while loop with condition as (leftCol &lt;= rightCol &amp;&amp; topRow &lt;= bottomRow) and inside, check for dir value and accordingly have for loops for what will vary, e.g, for dir == 0, i will vary from leftCol to rightCol but topRow will be fixed for an iteration. Make sure to increment topRow or rightCol after the iteration is over depending on a row or column you are done printing, i.e., say, when i touches rightCol for dir == 0, do topRow++ and when i touches bottomRow for dir==1. This way, same row or column won't print again with you're done with that.
+3) Once all of 4 for loops are done in while loop, change the direction as dir = (dir + 1) % 4. This will take care of boundary condition and dir will rotate between 0 and 3.</t>
+  </si>
+  <si>
+    <t>ArrrayDuplicateElements</t>
+  </si>
+  <si>
+    <t>findDuplicateElementsWithoutAnyStorage(int[] A),
+findDuplicateElementsWithMap(int[] A)</t>
+  </si>
+  <si>
+    <t>Given an integer array, print the duplicate elements including how many times they appear in the array.
+ Variation: Do this without using any extra storage, like Map, Set, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Soluton:
+ A) Using a Map:
+ 1) Fill the map with array elements as key and number of occurrences as value.
+ 2) Iterate through map using forEach((key, value) -&gt; { }) and print the duplicate element with their # of occurrences.
+ B) Without using any map or set:
+ 1) Use "Tail Based Approach" as used in removing duplicates from an array.
+ 2) Define variables, i=1, j=0 and tail = 1.
+ 3) Start a for loop with i = 1 to len-1.
+ 4) In above loop, start another loop with j = 0 to tail - 1 (condition: j &lt; tail).
+ 5) Inside second loop, check if A[j] == A[i], break from this loop.
+ 6) Outside of inside loop (and still inside the outer loop), check if j == tail (i.e. j could reach all the way till tail),
+  increment tail in that case.
+ You're done!</t>
+  </si>
+  <si>
+    <t>Tail based method comes very handy in removing duplicates or finding duplicates when you don't have any extra storage to use. Most time efficient too as I saw so far!
+My tests revealed time taken by Map based method as around 60,032,195 NS (60 Million Nano Seconds) where as with tail based method as just 426,041 Nano Seconds !! This is more than 12x more time that we spend on Map based method plus added storage too! This is why Tail based approach is so AWESOME!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note**: This is not same as LongestCommonSubsequence of DynamicProgramming package. Here it is longest common substring where chars are contiguous. In other one, chars don't need to be together as long as they come after the first char match in the subsequence.
+** Also, StringBuilder does not has clear() method unlike &lt;a collection like list, map&gt;.clear(). You will have to use sb.delete(fromIndex, toIndex) to clear the StringBuffer before filling it in again.
+** One more thing, unlike String's indexOf(char c), StringBuffer's indexOf method takes a string input, so when you read your string, read a string from it or conver the char to a string, like string.subString(i, i+1) or do Character.toString(char). </t>
+  </si>
+  <si>
+    <t>Rotate2DArray</t>
+  </si>
+  <si>
+    <t>rotate2DArray(int[][] A, int n)</t>
+  </si>
+  <si>
+    <t>Rotate n x n 2D Matrix clockwise</t>
+  </si>
+  <si>
+    <t>Solution: Check this video: https://www.youtube.com/watch?v=Jtu6dJ0Cb94
+(This is one of Cracking the Coding Interview Questions)
+1) Start with a 2 x 2 array and see how you need to swap elements to rotate it clockwise. Write exact positions like (0, 0) that needs to be swaped with position, say (0, last) where last = n-1. For corner positions, for 2D matrix, this will suffice:
+swap (0,0) with (0, last), then swap (0, 0) with (last, last), then swap (0, 0) with (last, 0).
+2) You can then generalize above and see how you can create loop(s) to ensure 2D array is taken care, since it will only have corners, no in between elements on rows. Once you can generalize it, apply with 3 x 3 and then with 4 x 4 matrix to test that you don't have a bug. Adjust your "formula" by introducing layer (0 to &lt;n/2) and last - i, for example instead of just last which worked for 2x2 (may not hold good for 3x3 matrix or 4x4 matrix). Also, see if layer = 2, in case of 4x4 or larger matrix, needs any adjustment in your Arrays references in the loop while ensuring that 2x2 matrix that worked good earlier with your loop, still works. For example, you can say (layer, i) now instead of saying (0, 1) since that will be more genaric, for outer layer, layer = 0, so it will be (0, 1) anyway, which will satisfy 2x2 matrix. 
+3) You swap the corners first, then swap element next to corner and go till end of row.
+ Say, A, B, C and D denote 4 corners and you need each of them to move by one position and get to D A B C, then if you swap position of A with B, then again new character at first position (previous position of A) with C, then same with D, with these 3 swaps, you can change the order from A B C D to D A B C. This means one rotation clock wise!
+4) Define a variable as layer which will vary from 0 to (n-1)/2. Your task is to rotate array one layer at a time.
+5) Within a layer, you need to swap elements based on 3) above, once for corner, then position next to that and so on.</t>
+  </si>
+  <si>
+    <t>Find data</t>
+  </si>
+  <si>
+    <t>1) If root is null, log and return.
+2) find(data) can be coded inside the Node class itself.
+3) Inside the find() method, if current node contains the data, return current node.
+4) If data less than data at current node, if left node is null, rerurn null, else find on left node (recursively).
+5) Do the reverse for else condition.</t>
+  </si>
+  <si>
+    <t>1) If root itself is null, create a node and insert it right there.
+2) Assign two new variables as parent and current and initialize the current variable to root
+3) Start a while(true) loop and in that assign parent to current as first thing.
+4) Check if data sent is less than the data on parent node. If so, move current node to its left child. If current becomes null, create the new node with given data and assign it as left child of the parent variable. Break from while (true) loop.
+5) Do the opposite on Else condition.</t>
+  </si>
+  <si>
+    <t>1) If left node to root is not null, new root will be the right most child of left sub tree, else if right node to root is not null, new root will be the left most child of right sub tree.
+2) Do null checks on root, if it is null, tree is empty and nothing needs to be done. Log and return.
+3) Get Left and Right childs of Root, if both are null, simply set the root of bst to null.
+4) If Left Child to Root != null, declare two pointers, parent and current. Assign "parent" the left child to root and make current the right child to parent. 
+5) Now, current can be null and in that case leftNodeToRoot has to be the new root. So with an if condition, check if this is the case. If so, set the left and right child of current root to null and make leftNodeToRoot as new root and return at this point. 
+6) If leftNodeToRoot does has a right child, Do a while loop and go right with condition as current != null &amp;&amp; current.rightNode != null. When this loop comes out, current will have its right child as null. Current will be the new root. parent should be the parent of this node at this point. But we have 2 situations here. A) current might have left child and B) current may not have left child. For A), make the left child of current as new right most node to left sub tree, i.e., assign that as right child of parent. For B, Assign Right child of parent as null. (Its like hey that right most child says: hey parent, I am being promoted to root now, I don't have right child but if I have a left child that now becomes your right child :))
+7) For Else condition, i.e., if (leftChildToRoot == null and rightChildToRoot != null, do the opposite of steps 4, 5 and 6 above.
+8) Finally, after above if-else loops, don't forget to set left and right child of current root to null, assign current as new root of the tree and return.</t>
+  </si>
+  <si>
+    <t>isLeafNode(int data)</t>
+  </si>
+  <si>
+    <t>1) Use find(data) to find the node that has this data, if root not null and if at all data is present in the BST.
+2) If node is found, then check if both of its children are null, if so, return true else, false.</t>
+  </si>
+  <si>
+    <t>Count Leaf Nodes</t>
+  </si>
+  <si>
+    <t>1) Check if root is null, return 0.
+2) Define two methods, isLeaf(Node n) and countLeaves(Node n). isLeaf will check if both the children of a node is null, it will return true, else false.
+3) In countLeaves, first check if n is a leaf node, return 1. We are going to call this method recursively, so this serves as the breaking condition.
+4) Define two variables, numLeftLeafNodes and numRightLeafNodes.
+5) Check if n != null and n.getLeftNode() != null. If so, call the same method with n.getLeftNode() as argument and assign the results to numLeftLeafNodes.
+6) Do the reverse for right node.
+7) Return the sum of numLeftLeafNodes and numRightLeafNodes.</t>
+  </si>
+  <si>
+    <t>1) Recursive approach. print(Node root) method.
+2) Inside this method, call inOrder(n); 
+if (n != null) {
+   inOrder(n.getLeftNode());
+   System.out.println(n.getData());
+   inOrder(n.getRightNode());
+}
+This method will print BST tree in ascending order since it goes to extreme left (shortest element of a BST tree), prints that, then goes to right child of its parent, prints that, goes to parent, prints that, right child of its parents, and so on. This is why it is calld inOrder traversing.</t>
+  </si>
+  <si>
+    <t>1) Take Recursive approach with breaking conditions as
+when we hit a leaf node.
+2) isLeaf can be a function to leverage that will check if a node has both its children as null
+3) The method needs to define two variables, say "left" and "right" to hold the results from two recursive calls, one to get height of left child (if that is not null) and another one for right child.
+4) Then at the end, return Math.max(left, right) + 1. + 1 is needed to account for root node itself.
+5) Outside of this recursive function one should verify if root is null, return 0 and only then call the height() recursive function.</t>
+  </si>
+  <si>
+    <t>Add sorted data to a BST: public Node addSorted(int [] data, int start, int end)</t>
+  </si>
+  <si>
+    <t>1) Create a method addSorted with arguments that take a sorted array, start and end indices. This method returns Node object, which will be the root of the BST formed.
+2) Code everything under a condition if(start &lt;= end). This also serves as breaking condition when this method is called recursively.
+3) Get mid point of start and add that data from array to create root node, call that newNode, which we will return before if loop ends.
+4) Before we return the node, call this method recursively, once with argument: data, start, mid-1, assign that result to leftNode variable of type Node and then with argument data, mid+1, end and assign that resule to rightNode variable.
+5) Above wil allow each node of left and right subtree to be populated and we return root  of main BST formed via newNode variabe.
+6) Outside the if loop, return null since start was sent as more than end, so we can't do anything.</t>
+  </si>
+  <si>
+    <t>LinkedList</t>
+  </si>
+  <si>
+    <t>removeDuplicates()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) If root is null or LinkedList has only one element (i.e., root.getNextNode() == null), log and return since no duplicate data is possible there.
+2) Define three variables of Node type, current = head.getNextNode(), previous =  head and runner = null.
+3) Start a while loop with condition as while (current != null) and in that set runner to head as first thing since we want to start with that in every iteration.
+4) Start another while loop with condition as runner != current. We are going to compare every node from head to previous with current to know if there is any duplicate data from head to current or not. 
+5) In this while loop, have an if condition to check if runner became same as current (runner.getData() == current.getData()).
+6) If true on #5 above, delete the current node by setting the next node for previous to the next node of current, setting previous to current and current to the node that was next node for current earlier. Once done, don't forget to add break statement there so internal while loop ends and next iteration for outer while loop start when you reset the runner to head and start comparing it with new node that now current points to.
+7) If false on #5 above, this means we need to compare next element after runner to current now, so do runner = runner.getNextNode().
+8) When while loop finishes, check if runner could reach all the way to current, so runner == current will work here, if so, move the previous and current both by a node and you're done! </t>
+  </si>
+  <si>
+    <t>reverse()</t>
+  </si>
+  <si>
+    <t>1) If head is null or head.getNextNode() is null, nothing needs to be done, log and return.
+2) Define two pointers of Node type: previous (set to null) and current (set to head).
+3) Start a while loop with condition as current.getNextNode() != null. We want to go until last node of the list and save that to make the new head so current != null condition won't help here.
+4) First thing in the loop: save the node next to current in a variable, say next.
+5) Set the next node to current as previous so the link reverses at that point.
+6) Set previous to current and current to its next node held by variable next. End the while loop here.
+7) Outside the while loop (don't forget to) set the current which now points to last node of earlier list as new head of the list. You're done!</t>
+  </si>
+  <si>
+    <t>1) Check if that node is null or its next node is null, log and return. You will need next node to delete that node.
+2) Copy the data from next node to this node. n.setData(n.getNextNode().getData()).
+3) Set the next node to given node as the node after next node since both the given node and its next node now has same data. n.setNextNode(n.getNextNode().getNextNode()) and you're done!</t>
+  </si>
+  <si>
+    <t>isCyclic()</t>
+  </si>
+  <si>
+    <t>1) Check if head is null, log and return.
+2) Define two pointers of type Node: slow and fast. Also define result = false.
+3) Start a while loop with condition as fast != null &amp;&amp; fast.getNextNode() != null. The reason is, in this loop we are going to move fast twice.
+4) Move slow once and fast twice. In each iteration, check if slow becomes equal to fast. If so, set result to true and break from loop.
+5) Outside the while loop, return result.
+Note*** If you define an integer counter and increment that each time, you can know the node number where this loop starts getting into a loop.</t>
+  </si>
+  <si>
+    <t>CircularQueue</t>
+  </si>
+  <si>
+    <t>Queues</t>
+  </si>
+  <si>
+    <t>findElementIndexInCircularArray()</t>
+  </si>
+  <si>
+    <t>Remove nodes with duplicate data in a Singly LinkedList.</t>
+  </si>
+  <si>
+    <t>Reverse the nodes of a linked list. Existing Tail becomes new Head and vice versa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deleteMiddleNodeWithMiddleNode() </t>
+  </si>
+  <si>
+    <t>Delete a node where you don't have the head and that node is middle of the node. All you have is that node itself.</t>
+  </si>
+  <si>
+    <t>Detect if a LinkedList is cyclic.</t>
+  </si>
+  <si>
+    <t>Find the height of a tree</t>
+  </si>
+  <si>
+    <t>Height of a BST</t>
+  </si>
+  <si>
+    <t>Search for a given data in a BST.</t>
+  </si>
+  <si>
+    <t>Insert given data in a BST.</t>
+  </si>
+  <si>
+    <t>Print all nodes of a BST inOrder, which gives sorted results.</t>
+  </si>
+  <si>
+    <t>Find mimimum and maximum nodes of a BST.</t>
+  </si>
+  <si>
+    <t>Delete root node of a BST.</t>
+  </si>
+  <si>
+    <t>Find if a node in BST is a leaf node or not.</t>
+  </si>
+  <si>
+    <t>Count number of nodes in a BST.</t>
+  </si>
+  <si>
+    <t>If you are given an array which is already sorted. How can you most add the data to a BST in a most effifient way?</t>
+  </si>
+  <si>
+    <t>Create a Queue from a Circular Array</t>
+  </si>
+  <si>
+    <t>Create a queue using circular arrays and define following operations there:
+1) size(): returns the size
+2) enqueue(int data): adds new data to queue
+3) dequeue(): takes off a data from queue
+4) Queue should never get full. (Hint: resize it if it does)
+5) toString(): prints all elements of the queue.</t>
+  </si>
+  <si>
+    <t>Circular Arrays are arrays which is sorted by the lowest data (called "pivot point") need not be on index 0, it can be pushed to anywhere in the array depending on how many times array is sorted. We can implement a queue using a circular array where new data will always be enqueued on head and data will be dequeued from tail.
+1) Start with an array of say, int type. Define variables, head, tail and capacity variables. Initialize them using constructor where array is created of capacity sent and head and tail are initialized to zero.
+2) size() method: Compute the size of queue by size=(capacity - head + tail) % capacity. Modulo on capacity ensures we never get ArrayOutOfBounds exception since we will be moving head and tail both.
+3) enqueue(int data): 
+3a) Before we add an element, we need to check if size is not full and if so, we will have to resize the array to its double capacity and copy existing data to it. So check for if (tail + 1) % == head { resize(); }
+3b) We will add the data to tail and then increment the tail. Just ensure to mod the incremented tail by capacity and then assign it back to tail.
+4) dequeue():
+4a) We can't dequeue if the size of the queue is zero. So just check for that using the size() method we already coded and if it is zero, log and return.
+4b) We will take an element from head since queue are of FIFO types. So we will return arr[head] and then increment head by ensuring to take mod by capacity in case head falls on the extreme end of the array.
+5) resize():
+5a) create variables newCapaciy (2 * capacity), newArr (if type int and size as newCapacity), pos (if type int, initial value as zero, this will serve as indez when we populate the new array.
+5b) We need to now copy all the data in existing array beginning from head to one index before tail. So start a while loop with condition as head != tail and in this loop, do newArr[pos] = arr[head].
+5c) Then do head = (head + 1) %capacity. With this, end the while loop.
+5d) Once while loop is done, assign newCapacity to capacity, head to zero, tail to pos and arr to newArr and you're done!</t>
+  </si>
+  <si>
+    <t>sum()</t>
+  </si>
+  <si>
+    <t>Get sum of all nodes.</t>
+  </si>
+  <si>
+    <t>Similar to print(), maintain a variable and keep on getting the sum in that variable.</t>
+  </si>
+  <si>
+    <t>Stacks</t>
+  </si>
+  <si>
+    <t>RemoveRedundantBrackets</t>
+  </si>
+  <si>
+    <t>removeParantheses()</t>
+  </si>
+  <si>
+    <t>StackWithDoublyEndedLinkedList</t>
+  </si>
+  <si>
+    <t>Create a stack using double ended linked list.</t>
+  </si>
+  <si>
+    <t>Create a stack using double ended linked list and provide following operations there:
+1) getSize()
+2) push: adds an element to stack
+3) pop(): returns last inserted element and removes it from stack
+4) peek(): returns last inserted element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Define variables of type DoublyEndedLinkedList (custom type or can use a Deque), top and size of types int.
+2) Use constructor to initialize them. DBLyEndedLinkedList to new object, top to -1 and size to zero.
+3) For size(), just return the current size.
+4) push(int data): insert the data at the head using insertAtHead() already coded at DBLyEndedLinkedList and increment size and top.
+5) pop(): </t>
+  </si>
+  <si>
+    <t>Here, time complexity will be of O(n). We need a storage of 256 characters but that should not be the big deal
+ * Solution: 
+ a) Define an int array of size 256. It can be 128 if pure ascii is contained by strings 
+ b) Initialize first element of this array by -1. Rest of them by default will have 0 and we are good with them.
+ c) loop through each chars of str1 and store their indices in array. Index of array will be ascii values of str1 chars: 
+     arr[str1.charAt(i)] = i
+ d) Loop through str2 chars, check if a char is present in str1 by checking arr[ch] &lt;= 0, if not continue checking.
+ e) If chars match, save the position of char position and define another variable (beginIndex = j) to check subsequent substrings. Define a new variable endIndex as beginIndex + 1. 
+ f) Do a while loop with condition as endIndex should be &lt;= length of str2 to keep checking if str1 contans the substring from str2 begining from beginIndex to endIndex and each time this true, increment the endIndex. See how far we can go, i.e., how large of substring is common from position we saved earlier as beginIndex. Break from while loop whenever there is no match.
+ g) when while loop exits, check length of substring found, compare the maxLength of the result we got so far, same the new max, if bigger one is found and store the resulting string to return finally.</t>
+  </si>
+  <si>
+    <t>ArrayCommonElements</t>
+  </si>
+  <si>
+    <t>getCommonElementsAlgo1(int[] arr1, int[] arr2)
+getCommonElementsAlgo2(int[] arr1, int[] arr2)
+getCommonElementsIterativeMethod(int[] arr1, int[] arr2)</t>
+  </si>
+  <si>
+    <t>Given two arrays, find the common elements among them.</t>
+  </si>
+  <si>
+    <t>Soluton:
+1) Brute Force: iterate through both arrays in two nested loop and find the common elements. Big 0(n^2)!
+2) Use a HashTable (or HashMap), add elements from Arrays 1 to it, then iterate through Array2, elements which are also in HashTable will be common elements. Create a resulting list and then convert the list by .toArrayMethod passing an empty array of same type as data in list and size of resulting list.
+3) Create ArrayLists from two input arrays and use the List interface method: list1.retainAll(list2) where Java removes the elements from list1 which are not contained in list2. Finally, convert list1 to array by method .toArray() passing an empty array with data type and size same as list1 and return it.</t>
+  </si>
+  <si>
+    <t>Given an array, find pair(s) of elements with given sum.</t>
+  </si>
+  <si>
+    <t>This approach can be used to find all the 3 some numbers too which have sum as given sum. For this take i, k, j indexes where k=mid point. In while loop, move k first depending on sum &gt; or &lt; given sum. Once reach first or last element, then increment I or decrement j (depending on which one k touches, recompute k as new mid point and repeat the steps.</t>
+  </si>
+  <si>
+    <t>Find count of triplets in an array whose sum is less than the given Sum</t>
+  </si>
+  <si>
+    <t>1) CircularArrays are sorted arrays with min element need not be the 0th element. Min element is called "Pivot Element" and its distance from 0th element tells us how many times this circular array is rotated.
+2) in rotated array, to find previous index, we should subtract 1, add the array length and then get a modulo with array length. This will help if index was 0, then (0 - 1 + length) % length will give us length - 1 as resulting index, which will be the last index of array, which makes perfect sense in case of rotated array. This will help us avoid ArrayOutOfBounds Exception.
+3) Same as above, next index = (current index + 1) % array length.
+4) Another very important property with Rotated Arrays is that one side of the pivot element is sorted and the other side is not. The side which is not sorted is where the pivot is located (due to its property that it is lower than its both the neighbors, it does not allow that side to be sorted).
+5) Keeping above properties in mind, do a binary search using a while loop with while loop as (low &lt;= high) condition. If mid is pivot, return mid index. If not, 
+6) Check which side of mid is sorted and accordingly do either low = next or high = previous in elseif and else conditions. Remember, pivot will always be on the side which is not sorted, i.e, !(A[low] &lt;= A[mid]) for pivot to be between low and mid (inclusive)!
+7) At the beginning of while loop, make sure to check for this and return low if array is already sorted:
+// If first element is lower then last element of this (sub) array, first index is the pivot
+   if (array[low] &lt;= array[high]) {
+    result = low;
+    return result;
+}
+8) just take care to use &lt;= or &gt;= during checks above, else you might miss a corner case getting to result.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Do binary search. In the while (low &lt;= high), once we check that mid element is not what we are looking for, we will have following cases there:
+Case 1: If array between low and high indexes sorted (numRotation == 0) at this point, i.e., everything is sorted, 
+mid is compared to high and low here!
+Case 1.a: Move high to right before mid or low to right after mid depending on how num compares with A[mid].
+Case 2: if left array is sorted, i.e., A[low] &lt;= A[prev]. This will allow us to check if num lies in that sub array. 
+Case 2.a: if num lies between two ends of left sub array, i.e., num &lt;= A[prev] move high to right before mid, i.e., high = prev. 
+Case 2.b: num has to be on right sub array, move low to right after mid, i.e, low = next.
+Case 3: if right array is sorted, i.e., A[next] &lt;= A[high], we will be able to check if num is present there 
+Case 3.a: if num lies between two ends of right sub array, , i.e., num &gt;= A[next], move low to right after mid, i.e., low = next.
+Case 3.b: if num has to be on left sub array, move high to right before mid.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Since this is a circular array, make sure to compute prev = (mid - 1 + len) % len and next = (mid + 1) % len and then use these variables instead of directly doing mid-1 or mid+1 which might give you ArrayIndexOutOfBounds otherwise!</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Solution:
+1) Do one while loop with condition as no array should not go out of bounds: while (i&lt;A.len &amp;&amp; j&lt;B.len &amp;&amp; k&lt;C.len).
+2) Grab elements from 3 arrays at their corresponding indices as e1 = arr1[i], e2 = arr2[j], etc.
+3) We now have following cases here:
+   a) All elements are same: (e1 == e2 &amp;&amp; e2 == e3). Add this element to result list.
+   b) e1 &gt; e2 -&gt; increase j and within this check if e2 &gt; e3 -&gt; increase k. if e2 &lt; e3 -&gt; increase j.
+   c) e1 &lt; e2 -&gt; increase i and within this check if e2 &lt; e3 -&gt; increase j. if e2 &gt; e3 -&gt; increase k.
+Note** With above, there is no need to check e1 with e3 since that is taken care in above conditions. if e1 &gt; e2 &amp;&amp; e2 &gt; e3, then e1 &gt; e3.
+Note** For &gt; or &lt; comparisons, don't rely on doing else only, add the conditions explicitly like e1 &gt; e2 else e2 &gt; e1. This will help not increment the indices when elements are equal and then capture them as part of your result with case a) above!</t>
+  </si>
+  <si>
+    <t>LargestSubsequenceIncreasingOrder</t>
+  </si>
+  <si>
+    <t>largestSubsequence(int[] arr)</t>
+  </si>
+  <si>
+    <t>Given a set of integers, write an algorithm, to find the largest sequence, meaning in increasing order.
+ For example,
+ Input: {1, 9, 3, 10, 4, 20, 2}
+ Output: 2
+ Explanation:
+ 1 -&gt; 9
+ 3 -&gt; 10
+ 4 -&gt; 20
+ So largest subsequence where next element(s) is/are in increasing is 2</t>
+  </si>
+  <si>
+    <t>Solution:
+1) Define an int variable for result and a stack. Push A[0] to stack.
+2) Iterate through array from 1 to len-1.
+3) if element at i is greater than stack.peak(), add the element to stack, else 
+4) Copmpare result with stack.size(), if higher, save new result and do stack.clear().
+5) Once loop is done, return the result.</t>
+  </si>
+  <si>
+    <t>Solution:
+1) Create an empty hash, like a HashSet&lt;Integer&gt;.
 2) Insert all array elements to hash.
 3) Do following for every element arr[i]
-....a) Check if this element is the starting point of a 
+a) Check if this element is the starting point of a 
        subsequence.  To check this, we simply look for
        arr[i] - 1 in hash, if not found, then this is
-       the first element a subsequence.  
-       If this element is a first element, then count 
-       number of elements in the consecutive starting 
-       with this element.
-       If count is more than current res, then update    
-       res.</t>
-  </si>
-  <si>
-    <t>In this the key is, we need consecutive integers at any index but in the forward direction.</t>
-  </si>
-  <si>
-    <t>RemoveDuplicatesIntArray</t>
-  </si>
-  <si>
-    <t>removeDuplicatesIntArray(int [] A)</t>
-  </si>
-  <si>
-    <t>Remove duplicates from an int array without using any extra storage (map, etc). The algorithm needs to be very efficient.</t>
+       the first element a subsequence. So we do if(!hash.contains(A[i] - 1)) { ... }
+       (So, basically don't do anything for elements that are not starting a subsequence)
+b) If this element is a first element, then count number of elements in the consecutive starting with this element. Can use the while loop. while (hash.contains(elem)) -&gt; elem++ and also append elem to a temp stringbuilder if you need elements as well. Finally, elem will be one more than the last elem in the subsequence.
+c) Do elem - A[i] to know the count. Doing + 1 not necessary since elem is already one more than last one when it came out of above while loop. Compare this number with result and if more, save the new max.
+d) Within this if control block itself, clear the previous stringbuilder, add the content of temp stringbuilder to it and once all done, clear the temp stringbuilder too.</t>
+  </si>
+  <si>
+    <t>Brute Force Solution:
+1. For every number, move to right, look for first greater number, append to result, if they do, else append ", _". 
+2) For last number simply append ", _".
+Better Solution:
+    a) Create a stack, push first element to it. Iterate from 2nd element and call that one "next"
+    b) pop from stack, call that "element", compare next to element, if next is bigger, send "element -&gt; next" to result collection (or print),
+    c) Keep popping from stack and comparing to next and send to output till next is smaller,
+    d) If stack gets empty in between, break and stop comparing,
+    e) Send the "element" which turns to be bigger than 'next' back to stack,
+    f) Push next to stack before an iteration ends so its current array element (next's) pair can also be found,
+    g) Once loop finishes, check if stack is not empty, those elements don't have next bigger element, so 
+        print them as "element -&gt; -1"
+(Note** Per Geeksforgeeks, later solution is O(N), more optimized but I found this to be taking more time than above. May be due to stack operation overhead? Find out more!</t>
   </si>
   <si>
     <r>
@@ -1192,12 +1601,13 @@
       <t xml:space="preserve">
  for it. Approach:
  1) Define j and tail, initialize them to 0 and 1 respectively.
- 2) Start a for loop with i from 1 to len-1.
- 3) Inside above loop, start another one with j=0 to j &lt; tail.
- 4) if A[j] == A[i], break from inner loop.
- 5) Outside the inner loop, check if j could go uninterrupted all the way to tail before the inner loop broke.
- 6) If above is true, swap A[tail] with A[i] because A[i] is first no duplicate element after tail position. Increment tail by one.
- 7) Outside of the loop, grab the array elements from A[0] A[tail - 1] and return.
+ 2) Start a for-loop with i from 1 to len-1.
+ 3) Inside above loop, reset j = 0.
+ 4) Start a while loop with condition as j &lt; tail.
+ 5) Inside of while-loop, if A[j] == A[i], break from while loop. Then do j++ (i.e., if loop services this iteration).
+ 6) Outside the whiler loop, check if j could go uninterrupted all the way to tail before the inner loop broke, i.e., if j == tail
+ 7) If above is true, do A[tail] = A[i] because A[i] is first no duplicate element after tail position. Increment tail by one.
+ 8) Outside of the loop, grab the array elements from A[0] A[tail - 1] and return.
  </t>
     </r>
     <r>
@@ -1223,354 +1633,288 @@
     </r>
   </si>
   <si>
-    <t>Print2DArraySnakeOrder</t>
-  </si>
-  <si>
-    <t>print2DArraySnakeOrderHorizontal(int[][] A, int m, int n),
-print2DArraySnakeOrderVertical(int[][] A, int m, int n)</t>
-  </si>
-  <si>
-    <t>For a 2D Array, print the elements in "snake order horizontal" and then "snake order vertical".
-Example Input:
-A mxn 2D array, 
-A = { 
-   {1, 2, 3}, 
-   {4, 5, 6},
-   {7, 8, 9}, 
-   {10, 11, 12}
- };
-Output:
-a) Snake order horizontal: 1, 2, 3, 6, 5, 4, 7, 8, 9, 12, 11, 10
-b) Snake order vertical: 1, 4, 7, 10, 11, 8, 5, 2, 3, 6, 9, 12</t>
-  </si>
-  <si>
-    <t>Print 2D Array in Spiral Order.</t>
-  </si>
-  <si>
-    <t>Solution:
-A) Snake Horizontal Order:
-1) We basically need to print m rows by varying the direction every time, left to right (to start with) and alternate that
-   every time.
-2) Take a variable k and assign this to -1.
-3) Start first for loop and in that vary i from 0 to m-1.
-4) Inside above loop, do k *= -1 (basically toggle it from -1 to +1 in every loop.
-5) Have 2 variation of inner for-loop based on whether k &gt; 0 or not, vary j from 0 to n-1 or n-1 to 0 and print A[j][j];
-B) Snake Vertical Order:
-1) Do exactly reverse of above. Here we need to print columns from 0 to n by alternating the direction every time.
-2) Take a variable k and assign this to -1.
-3) Start first for loop and in that vary j from 0 to n-1.
-4) Inside above loop, do k *= -1 (basically toggle it from -1 to +1 in every loop.
-5) Have 2 variation of inner for-loop based on whether k &gt; 0 or not, vary i from 0 to m-1 or m-1 to 0 and print A[j][j];</t>
-  </si>
-  <si>
-    <t>1) Define variables like topRow=0, rightCol=n-1, bottomRow=m-1, leftCol=0. Also define a variable as dir, which will indicate directions: 0 for left to right, 1 for top to bottom, 2 for right to left and 3 for bottom to top. Start with dir = 0;
-2) Have a while loop with condition as (leftCol &lt;= rightCol &amp;&amp; topRow &lt;= bottomRow) and inside, check for dir value and accordingly have for loops for what will vary, e.g, for dir == 0, i will vary from leftCol to rightCol but topRow will be fixed for an iteration. Make sure to increment topRow or rightCol after the iteration is over depending on a row or column you are done printing, i.e., say, when i touches rightCol for dir == 0, do topRow++ and when i touches bottomRow for dir==1. This way, same row or column won't print again with you're done with that.
-3) Once all of 4 for loops are done in while loop, change the direction as dir = (dir + 1) % 4. This will take care of boundary condition and dir will rotate between 0 and 3.</t>
-  </si>
-  <si>
-    <t>ArrrayDuplicateElements</t>
-  </si>
-  <si>
-    <t>findDuplicateElementsWithoutAnyStorage(int[] A),
-findDuplicateElementsWithMap(int[] A)</t>
-  </si>
-  <si>
-    <t>Given an integer array, print the duplicate elements including how many times they appear in the array.
- Variation: Do this without using any extra storage, like Map, Set, etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Soluton:
- A) Using a Map:
- 1) Fill the map with array elements as key and number of occurrences as value.
- 2) Iterate through map using forEach((key, value) -&gt; { }) and print the duplicate element with their # of occurrences.
- B) Without using any map or set:
- 1) Use "Tail Based Approach" as used in removing duplicates from an array.
- 2) Define variables, i=1, j=0 and tail = 1.
- 3) Start a for loop with i = 1 to len-1.
- 4) In above loop, start another loop with j = 0 to tail - 1 (condition: j &lt; tail).
- 5) Inside second loop, check if A[j] == A[i], break from this loop.
- 6) Outside of inside loop (and still inside the outer loop), check if j == tail (i.e. j could reach all the way till tail),
-  increment tail in that case.
- You're done!</t>
-  </si>
-  <si>
-    <t>Tail based method comes very handy in removing duplicates or finding duplicates when you don't have any extra storage to use. Most time efficient too as I saw so far!
-My tests revealed time taken by Map based method as around 60,032,195 NS (60 Million Nano Seconds) where as with tail based method as just 426,041 Nano Seconds !! This is more than 12x more time that we spend on Map based method plus added storage too! This is why Tail based approach is so AWESOME!!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note**: This is not same as LongestCommonSubsequence of DynamicProgramming package. Here it is longest common substring where chars are contiguous. In other one, chars don't need to be together as long as they come after the first char match in the subsequence.
-** Also, StringBuilder does not has clear() method unlike &lt;a collection like list, map&gt;.clear(). You will have to use sb.delete(fromIndex, toIndex) to clear the StringBuffer before filling it in again.
-** One more thing, unlike String's indexOf(char c), StringBuffer's indexOf method takes a string input, so when you read your string, read a string from it or conver the char to a string, like string.subString(i, i+1) or do Character.toString(char). </t>
-  </si>
-  <si>
-    <t>Rotate2DArray</t>
-  </si>
-  <si>
-    <t>rotate2DArray(int[][] A, int n)</t>
-  </si>
-  <si>
-    <t>Rotate n x n 2D Matrix clockwise</t>
-  </si>
-  <si>
-    <t>Solution: Check this video: https://www.youtube.com/watch?v=Jtu6dJ0Cb94
-(This is one of Cracking the Coding Interview Questions)
-1) Start with a 2 x 2 array and see how you need to swap elements to rotate it clockwise. Write exact positions like (0, 0) that needs to be swaped with position, say (0, last) where last = n-1. For corner positions, for 2D matrix, this will suffice:
-swap (0,0) with (0, last), then swap (0, 0) with (last, last), then swap (0, 0) with (last, 0).
-2) You can then generalize above and see how you can create loop(s) to ensure 2D array is taken care, since it will only have corners, no in between elements on rows. Once you can generalize it, apply with 3 x 3 and then with 4 x 4 matrix to test that you don't have a bug. Adjust your "formula" by introducing layer (0 to &lt;n/2) and last - i, for example instead of just last which worked for 2x2 (may not hold good for 3x3 matrix or 4x4 matrix). Also, see if layer = 2, in case of 4x4 or larger matrix, needs any adjustment in your Arrays references in the loop while ensuring that 2x2 matrix that worked good earlier with your loop, still works. For example, you can say (layer, i) now instead of saying (0, 1) since that will be more genaric, for outer layer, layer = 0, so it will be (0, 1) anyway, which will satisfy 2x2 matrix. 
-3) You swap the corners first, then swap element next to corner and go till end of row.
- Say, A, B, C and D denote 4 corners and you need each of them to move by one position and get to D A B C, then if you swap position of A with B, then again new character at first position (previous position of A) with C, then same with D, with these 3 swaps, you can change the order from A B C D to D A B C. This means one rotation clock wise!
-4) Define a variable as layer which will vary from 0 to (n-1)/2. Your task is to rotate array one layer at a time.
-5) Within a layer, you need to swap elements based on 3) above, once for corner, then position next to that and so on.</t>
-  </si>
-  <si>
-    <t>Find data</t>
-  </si>
-  <si>
-    <t>1) If root is null, log and return.
-2) find(data) can be coded inside the Node class itself.
-3) Inside the find() method, if current node contains the data, return current node.
-4) If data less than data at current node, if left node is null, rerurn null, else find on left node (recursively).
-5) Do the reverse for else condition.</t>
-  </si>
-  <si>
-    <t>1) If root itself is null, create a node and insert it right there.
-2) Assign two new variables as parent and current and initialize the current variable to root
-3) Start a while(true) loop and in that assign parent to current as first thing.
-4) Check if data sent is less than the data on parent node. If so, move current node to its left child. If current becomes null, create the new node with given data and assign it as left child of the parent variable. Break from while (true) loop.
-5) Do the opposite on Else condition.</t>
-  </si>
-  <si>
-    <t>1) If left node to root is not null, new root will be the right most child of left sub tree, else if right node to root is not null, new root will be the left most child of right sub tree.
-2) Do null checks on root, if it is null, tree is empty and nothing needs to be done. Log and return.
-3) Get Left and Right childs of Root, if both are null, simply set the root of bst to null.
-4) If Left Child to Root != null, declare two pointers, parent and current. Assign "parent" the left child to root and make current the right child to parent. 
-5) Now, current can be null and in that case leftNodeToRoot has to be the new root. So with an if condition, check if this is the case. If so, set the left and right child of current root to null and make leftNodeToRoot as new root and return at this point. 
-6) If leftNodeToRoot does has a right child, Do a while loop and go right with condition as current != null &amp;&amp; current.rightNode != null. When this loop comes out, current will have its right child as null. Current will be the new root. parent should be the parent of this node at this point. But we have 2 situations here. A) current might have left child and B) current may not have left child. For A), make the left child of current as new right most node to left sub tree, i.e., assign that as right child of parent. For B, Assign Right child of parent as null. (Its like hey that right most child says: hey parent, I am being promoted to root now, I don't have right child but if I have a left child that now becomes your right child :))
-7) For Else condition, i.e., if (leftChildToRoot == null and rightChildToRoot != null, do the opposite of steps 4, 5 and 6 above.
-8) Finally, after above if-else loops, don't forget to set left and right child of current root to null, assign current as new root of the tree and return.</t>
-  </si>
-  <si>
-    <t>isLeafNode(int data)</t>
-  </si>
-  <si>
-    <t>1) Use find(data) to find the node that has this data, if root not null and if at all data is present in the BST.
-2) If node is found, then check if both of its children are null, if so, return true else, false.</t>
-  </si>
-  <si>
-    <t>Count Leaf Nodes</t>
-  </si>
-  <si>
-    <t>1) Check if root is null, return 0.
-2) Define two methods, isLeaf(Node n) and countLeaves(Node n). isLeaf will check if both the children of a node is null, it will return true, else false.
-3) In countLeaves, first check if n is a leaf node, return 1. We are going to call this method recursively, so this serves as the breaking condition.
-4) Define two variables, numLeftLeafNodes and numRightLeafNodes.
-5) Check if n != null and n.getLeftNode() != null. If so, call the same method with n.getLeftNode() as argument and assign the results to numLeftLeafNodes.
-6) Do the reverse for right node.
-7) Return the sum of numLeftLeafNodes and numRightLeafNodes.</t>
-  </si>
-  <si>
-    <t>1) Recursive approach. print(Node root) method.
-2) Inside this method, call inOrder(n); 
-if (n != null) {
-   inOrder(n.getLeftNode());
-   System.out.println(n.getData());
-   inOrder(n.getRightNode());
-}
-This method will print BST tree in ascending order since it goes to extreme left (shortest element of a BST tree), prints that, then goes to right child of its parent, prints that, goes to parent, prints that, right child of its parents, and so on. This is why it is calld inOrder traversing.</t>
-  </si>
-  <si>
-    <t>1) Take Recursive approach with breaking conditions as
-when we hit a leaf node.
-2) isLeaf can be a function to leverage that will check if a node has both its children as null
-3) The method needs to define two variables, say "left" and "right" to hold the results from two recursive calls, one to get height of left child (if that is not null) and another one for right child.
-4) Then at the end, return Math.max(left, right) + 1. + 1 is needed to account for root node itself.
-5) Outside of this recursive function one should verify if root is null, return 0 and only then call the height() recursive function.</t>
-  </si>
-  <si>
-    <t>Add sorted data to a BST: public Node addSorted(int [] data, int start, int end)</t>
-  </si>
-  <si>
-    <t>1) Create a method addSorted with arguments that take a sorted array, start and end indices. This method returns Node object, which will be the root of the BST formed.
-2) Code everything under a condition if(start &lt;= end). This also serves as breaking condition when this method is called recursively.
-3) Get mid point of start and add that data from array to create root node, call that newNode, which we will return before if loop ends.
-4) Before we return the node, call this method recursively, once with argument: data, start, mid-1, assign that result to leftNode variable of type Node and then with argument data, mid+1, end and assign that resule to rightNode variable.
-5) Above wil allow each node of left and right subtree to be populated and we return root  of main BST formed via newNode variabe.
-6) Outside the if loop, return null since start was sent as more than end, so we can't do anything.</t>
-  </si>
-  <si>
-    <t>LinkedList</t>
-  </si>
-  <si>
-    <t>removeDuplicates()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) If root is null or LinkedList has only one element (i.e., root.getNextNode() == null), log and return since no duplicate data is possible there.
-2) Define three variables of Node type, current = head.getNextNode(), previous =  head and runner = null.
-3) Start a while loop with condition as while (current != null) and in that set runner to head as first thing since we want to start with that in every iteration.
-4) Start another while loop with condition as runner != current. We are going to compare every node from head to previous with current to know if there is any duplicate data from head to current or not. 
-5) In this while loop, have an if condition to check if runner became same as current (runner.getData() == current.getData()).
-6) If true on #5 above, delete the current node by setting the next node for previous to the next node of current, setting previous to current and current to the node that was next node for current earlier. Once done, don't forget to add break statement there so internal while loop ends and next iteration for outer while loop start when you reset the runner to head and start comparing it with new node that now current points to.
-7) If false on #5 above, this means we need to compare next element after runner to current now, so do runner = runner.getNextNode().
-8) When while loop finishes, check if runner could reach all the way to current, so runner == current will work here, if so, move the previous and current both by a node and you're done! </t>
-  </si>
-  <si>
-    <t>reverse()</t>
-  </si>
-  <si>
-    <t>1) If head is null or head.getNextNode() is null, nothing needs to be done, log and return.
-2) Define two pointers of Node type: previous (set to null) and current (set to head).
-3) Start a while loop with condition as current.getNextNode() != null. We want to go until last node of the list and save that to make the new head so current != null condition won't help here.
-4) First thing in the loop: save the node next to current in a variable, say next.
-5) Set the next node to current as previous so the link reverses at that point.
-6) Set previous to current and current to its next node held by variable next. End the while loop here.
-7) Outside the while loop (don't forget to) set the current which now points to last node of earlier list as new head of the list. You're done!</t>
-  </si>
-  <si>
-    <t>1) Check if that node is null or its next node is null, log and return. You will need next node to delete that node.
-2) Copy the data from next node to this node. n.setData(n.getNextNode().getData()).
-3) Set the next node to given node as the node after next node since both the given node and its next node now has same data. n.setNextNode(n.getNextNode().getNextNode()) and you're done!</t>
-  </si>
-  <si>
-    <t>isCyclic()</t>
-  </si>
-  <si>
-    <t>1) Check if head is null, log and return.
-2) Define two pointers of type Node: slow and fast. Also define result = false.
-3) Start a while loop with condition as fast != null &amp;&amp; fast.getNextNode() != null. The reason is, in this loop we are going to move fast twice.
-4) Move slow once and fast twice. In each iteration, check if slow becomes equal to fast. If so, set result to true and break from loop.
-5) Outside the while loop, return result.
-Note*** If you define an integer counter and increment that each time, you can know the node number where this loop starts getting into a loop.</t>
-  </si>
-  <si>
-    <t>CircularQueue</t>
-  </si>
-  <si>
-    <t>Queues</t>
-  </si>
-  <si>
-    <t>findElementIndexInCircularArray()</t>
-  </si>
-  <si>
-    <t>Remove nodes with duplicate data in a Singly LinkedList.</t>
-  </si>
-  <si>
-    <t>Reverse the nodes of a linked list. Existing Tail becomes new Head and vice versa.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deleteMiddleNodeWithMiddleNode() </t>
-  </si>
-  <si>
-    <t>Delete a node where you don't have the head and that node is middle of the node. All you have is that node itself.</t>
-  </si>
-  <si>
-    <t>Detect if a LinkedList is cyclic.</t>
-  </si>
-  <si>
-    <t>Find the height of a tree</t>
-  </si>
-  <si>
-    <t>Height of a BST</t>
-  </si>
-  <si>
-    <t>Search for a given data in a BST.</t>
-  </si>
-  <si>
-    <t>Insert given data in a BST.</t>
-  </si>
-  <si>
-    <t>Print all nodes of a BST inOrder, which gives sorted results.</t>
-  </si>
-  <si>
-    <t>Find mimimum and maximum nodes of a BST.</t>
-  </si>
-  <si>
-    <t>Delete root node of a BST.</t>
-  </si>
-  <si>
-    <t>Find if a node in BST is a leaf node or not.</t>
-  </si>
-  <si>
-    <t>Count number of nodes in a BST.</t>
-  </si>
-  <si>
-    <t>If you are given an array which is already sorted. How can you most add the data to a BST in a most effifient way?</t>
-  </si>
-  <si>
-    <t>Create a Queue from a Circular Array</t>
-  </si>
-  <si>
-    <t>Create a queue using circular arrays and define following operations there:
-1) size(): returns the size
-2) enqueue(int data): adds new data to queue
-3) dequeue(): takes off a data from queue
-4) Queue should never get full. (Hint: resize it if it does)
-5) toString(): prints all elements of the queue.</t>
-  </si>
-  <si>
-    <t>Circular Arrays are arrays which is sorted by the lowest data (called "pivot point") need not be on index 0, it can be pushed to anywhere in the array depending on how many times array is sorted. We can implement a queue using a circular array where new data will always be enqueued on head and data will be dequeued from tail.
-1) Start with an array of say, int type. Define variables, head, tail and capacity variables. Initialize them using constructor where array is created of capacity sent and head and tail are initialized to zero.
-2) size() method: Compute the size of queue by size=(capacity - head + tail) % capacity. Modulo on capacity ensures we never get ArrayOutOfBounds exception since we will be moving head and tail both.
-3) enqueue(int data): 
-3a) Before we add an element, we need to check if size is not full and if so, we will have to resize the array to its double capacity and copy existing data to it. So check for if (tail + 1) % == head { resize(); }
-3b) We will add the data to tail and then increment the tail. Just ensure to mod the incremented tail by capacity and then assign it back to tail.
-4) dequeue():
-4a) We can't dequeue if the size of the queue is zero. So just check for that using the size() method we already coded and if it is zero, log and return.
-4b) We will take an element from head since queue are of FIFO types. So we will return arr[head] and then increment head by ensuring to take mod by capacity in case head falls on the extreme end of the array.
-5) resize():
-5a) create variables newCapaciy (2 * capacity), newArr (if type int and size as newCapacity), pos (if type int, initial value as zero, this will serve as indez when we populate the new array.
-5b) We need to now copy all the data in existing array beginning from head to one index before tail. So start a while loop with condition as head != tail and in this loop, do newArr[pos] = arr[head].
-5c) Then do head = (head + 1) %capacity. With this, end the while loop.
-5d) Once while loop is done, assign newCapacity to capacity, head to zero, tail to pos and arr to newArr and you're done!</t>
-  </si>
-  <si>
-    <t>sum()</t>
-  </si>
-  <si>
-    <t>Get sum of all nodes.</t>
-  </si>
-  <si>
-    <t>Similar to print(), maintain a variable and keep on getting the sum in that variable.</t>
-  </si>
-  <si>
-    <t>Stacks</t>
-  </si>
-  <si>
-    <t>RemoveRedundantBrackets</t>
-  </si>
-  <si>
-    <t>removeParantheses()</t>
-  </si>
-  <si>
-    <t>StackWithDoublyEndedLinkedList</t>
-  </si>
-  <si>
-    <t>Create a stack using double ended linked list.</t>
-  </si>
-  <si>
-    <t>Create a stack using double ended linked list and provide following operations there:
-1) getSize()
-2) push: adds an element to stack
-3) pop(): returns last inserted element and removes it from stack
-4) peek(): returns last inserted element</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) Define variables of type DoublyEndedLinkedList (custom type or can use a Deque), top and size of types int.
-2) Use constructor to initialize them. DBLyEndedLinkedList to new object, top to -1 and size to zero.
-3) For size(), just return the current size.
-4) push(int data): insert the data at the head using insertAtHead() already coded at DBLyEndedLinkedList and increment size and top.
-5) pop(): </t>
-  </si>
-  <si>
-    <t>Here, time complexity will be of O(n). We need a storage of 256 characters but that should not be the big deal
- * Solution: 
- a) Define an int array of size 256. It can be 128 if pure ascii is contained by strings 
- b) Initialize first element of this array by -1. Rest of them by default will have 0 and we are good with them.
- c) loop through each chars of str1 and store their indices in array. Index of array will be ascii values of str1 chars: 
-     arr[str1.charAt(i)] = i
- d) Loop through str2 chars, check if a char is present in str1 by checking arr[ch] &lt;= 0, if not continue checking.
- e) If chars match, save the position of char position and define another variable (beginIndex = j) to check subsequent substrings. Define a new variable endIndex as beginIndex + 1. 
- f) Do a while loop with condition as endIndex should be &lt;= length of str2 to keep checking if str1 contans the substring from str2 begining from beginIndex to endIndex and each time this true, increment the endIndex. See how far we can go, i.e., how large of substring is common from position we saved earlier as beginIndex. Break from while loop whenever there is no match.
- g) when while loop exits, check length of substring found, compare the maxLength of the result we got so far, same the new max, if bigger one is found and store the resulting string to return finally.</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Method 1: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Have a for loop, do modulo everytime, extract last digit and append to a string. Then convert this string to integer by above method on Row # 3, class Algorithms. Take care of boundary conditions and save a boolean as isNegative, convert number as positive and use that at the end to convert the integer back to negative before returning. You can also do it via a stack instead of string.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Optimized one</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, as this </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>does not need temporary storage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of reverse of number. This directly converts number to reverse number. Underlying theory is, say you have a number 23, how will you add an extra digit at the end, say 4? You'll multiply it by 10 (i.e., promote the current unit digit to 10th place) and then add the new digit to it. That'll be 23 * 10 + 4 = 234! So basically, define a variable as result = 0, in while loop (till num == 0), get modulo and do result = (result * 10 + modulo) everytime in the loop. Finally return the result.</t>
+    </r>
+  </si>
+  <si>
+    <t>BigO: O(n^2):
+1) Iterate through smaller array and inside that iterate through next bigger array, for each element combinations of both, find the diffrence of their sum with given sum. Then do a binary search on 3rd (largest size) array to check if they have a number equal to the difference we computed in nested for loops. If so, mark that 3-some for one of your results. Proceed with rest of elements of first 2 arrays.</t>
+  </si>
+  <si>
+    <t>Implemented as TopK Problem already</t>
+  </si>
+  <si>
+    <t>This is a TopK Problem. See:
+https://github.com/ashesh1105/java-projects/blob/master/DataStructures/src/main/java/com/datastructures/heaps/TopKHeavyHitters.java
+	   1) Define a Map of String and Integer. Key will be combination of 3 pages visited, like home -&gt; search -&gt; checkout
+	      value will be frequency of them.
+	   2) Populate this map for the time range we are interested. Bigger time ranges will need offline data pipeline.
+	   3) Define a Min PriorityQueue of size k (if k==1, just iterate through map and get the max one.
+	   4) On PriorityQueue, whenever k+1th element comes, pool the queue, which will remove the minimum element from it.</t>
+  </si>
+  <si>
+    <t>Anagram1 / Anagram2 / Anagram3</t>
+  </si>
+  <si>
+    <t>isAnagram(String str1, String str2)</t>
+  </si>
+  <si>
+    <t>Aangrams are strings where by swapping chars in one string, one can form into another one. Given two string, find out if they are anagrams.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Solution 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Most Optimized One!!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) Define an int array of 128 or 256 size (depending on if you're dealing with pure ascii chars or not). Elements get initialized to 0.
+2) Iterate through str1 and increment array elements by using char as index, i.e., arr[ch]++
+3) Iterate through str2, check if arr[ch] == 0, return false. Outside of loop, return true.
+4) You can optimize it further if you can define variables like </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>numUniqueChars</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, populate it while iterating str1 and check everytime arr[ch] != 0 and you decrement it, if then arr[ch] == 0, at this point if </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>numUniqueChars</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> == </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>numCompletedStr2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, we must be at last character of str2 here, i.e., i == len-1 for str2. Meaning you're done checking for all unique chars of str1 including duplicate ones on them (since you checked arr[ch] == 0 here in str2 iteration) and with numUniqueChars == numCompletedStr2, you're still not done with str2!! Return i == str2.length() - 1;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Solution 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) Define a Map of Character and Integer. Iterate through str1 and populate the map with chars and frequency.
+2) Iterate through str2, if any char is not present or not present enough number of times, return false. So, if char is present, keep decrementing the frequncies. Finally, outside of the loop, check if map.size() != 0, return false, else true.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Solution 3:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1) Define two variables, compute sum of ascii values of chars in each string, I call it "hash1" and "hash2", i.e., int hash1 += ch, while iterating a string.
+2) Compare the hashes and return hash1 == hash2.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:: Solution 1 is abiout 16 times faster than 2, about 2.7 times faster than 3 in my code.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2069,10 +2413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2101,7 +2445,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
@@ -2110,24 +2454,24 @@
         <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -2137,23 +2481,23 @@
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="340" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>195</v>
+        <v>310</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>8</v>
@@ -2163,35 +2507,35 @@
       <c r="A5" s="8"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -2199,36 +2543,36 @@
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -2236,11 +2580,11 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G9" s="2"/>
     </row>
@@ -2249,11 +2593,11 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G10" s="2"/>
     </row>
@@ -2262,14 +2606,14 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -2277,14 +2621,14 @@
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="153" x14ac:dyDescent="0.2">
@@ -2292,14 +2636,14 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -2307,28 +2651,28 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G15" s="2"/>
     </row>
@@ -2336,12 +2680,12 @@
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -2349,14 +2693,14 @@
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G17" s="2"/>
     </row>
@@ -2364,34 +2708,34 @@
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="255" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -2403,714 +2747,760 @@
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>299</v>
+      </c>
       <c r="F20" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="238" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>146</v>
+        <v>301</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="272" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>244</v>
+        <v>295</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>245</v>
+        <v>296</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>246</v>
+        <v>297</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>298</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="238" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>16</v>
+        <v>233</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>17</v>
+        <v>234</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>148</v>
+        <v>235</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>19</v>
+        <v>236</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>150</v>
+        <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>205</v>
+        <v>18</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="255" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>229</v>
+        <v>146</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>230</v>
+        <v>32</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>231</v>
+        <v>145</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>20</v>
+        <v>305</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="2"/>
+        <v>306</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>307</v>
+      </c>
       <c r="F26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>308</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="289" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>24</v>
+        <v>220</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E27" s="2"/>
+        <v>221</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>222</v>
+      </c>
       <c r="F27" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" ht="299" customHeight="1" x14ac:dyDescent="0.2">
+        <v>309</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>151</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>152</v>
+        <v>22</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="293" customHeight="1" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>161</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="299" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="F30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="293" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="F31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>197</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>198</v>
+        <v>24</v>
       </c>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
-        <v>4</v>
-      </c>
+    <row r="34" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>170</v>
+        <v>53</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>172</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
+        <v>313</v>
+      </c>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" ht="372" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>179</v>
+        <v>31</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>305</v>
+        <v>154</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>302</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="323" x14ac:dyDescent="0.2">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>114</v>
+        <v>194</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E37" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="F37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
+        <v>303</v>
+      </c>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>168</v>
+      </c>
       <c r="F38" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" ht="372" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="388" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>60</v>
+        <v>316</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>61</v>
+        <v>317</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>180</v>
+        <v>318</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>181</v>
+        <v>319</v>
       </c>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="C40" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="C41" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" ht="340" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
-        <v>31</v>
-      </c>
+    <row r="42" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>199</v>
+        <v>111</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>158</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="E42" s="2"/>
       <c r="F42" s="2" t="s">
-        <v>202</v>
+        <v>114</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="238" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
-        <v>31</v>
-      </c>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>200</v>
+        <v>115</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>204</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E43" s="2"/>
       <c r="F43" s="2" t="s">
-        <v>201</v>
+        <v>117</v>
       </c>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="340" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>163</v>
+        <v>57</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>164</v>
+        <v>58</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A45" s="8"/>
+        <v>177</v>
+      </c>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" ht="372" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="C45" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="323" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>250</v>
+        <v>194</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>251</v>
+        <v>195</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>252</v>
+        <v>196</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>253</v>
+        <v>303</v>
       </c>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" ht="323" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
-        <v>44</v>
-      </c>
+    <row r="47" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>238</v>
+        <v>159</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>239</v>
+        <v>160</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>240</v>
+        <v>161</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" ht="187" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>44</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A48" s="8"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>243</v>
-      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="1:7" ht="323" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="356" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>213</v>
+        <v>239</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>214</v>
+        <v>240</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>215</v>
+        <v>241</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>216</v>
+        <v>242</v>
       </c>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="255" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" s="4" customFormat="1" ht="272" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3" t="s">
-        <v>222</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="G51" s="3"/>
-    </row>
-    <row r="52" spans="1:7" ht="221" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" s="4" customFormat="1" ht="323" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
-        <v>39</v>
+        <v>208</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>41</v>
+        <v>209</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>40</v>
+        <v>210</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="121" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="8"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2" t="s">
-        <v>42</v>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="255" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" spans="1:7" ht="121" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="1:7" ht="215" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="8"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:7" ht="170" x14ac:dyDescent="0.2">
-      <c r="A56" s="8"/>
+    <row r="56" spans="1:7" ht="215" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>196</v>
+        <v>39</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G56" s="2"/>
-    </row>
-    <row r="57" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A57" s="8"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2" t="s">
-        <v>210</v>
+        <v>41</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>207</v>
+        <v>42</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>208</v>
+        <v>164</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>209</v>
+        <v>165</v>
       </c>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>50</v>
+        <v>224</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E58" s="2"/>
+        <v>225</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>226</v>
+      </c>
       <c r="F58" s="2" t="s">
-        <v>52</v>
+        <v>311</v>
       </c>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:7" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A59" s="8"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E59" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="F59" s="2" t="s">
-        <v>59</v>
+        <v>312</v>
       </c>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A60" s="9"/>
+    <row r="60" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A60" s="8"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>304</v>
+      </c>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="C61" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
+      <c r="F61" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
+      <c r="C62" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
+      <c r="F62" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A63" s="8"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
+    <row r="63" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A63" s="9"/>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="1:7" ht="19" x14ac:dyDescent="0.2">
@@ -3122,421 +3512,407 @@
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
     </row>
-    <row r="65" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A65" s="8" t="s">
-        <v>93</v>
-      </c>
+    <row r="65" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A65" s="8"/>
       <c r="B65" s="2"/>
-      <c r="C65" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
       <c r="E65" s="2"/>
-      <c r="F65" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="F65" s="2"/>
       <c r="G65" s="2"/>
     </row>
-    <row r="66" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A66" s="8"/>
       <c r="B66" s="2"/>
-      <c r="C66" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>98</v>
-      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
       <c r="E66" s="2"/>
-      <c r="F66" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
     </row>
     <row r="67" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
-      <c r="C67" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D67" s="7"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="7"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A68" s="8"/>
+    <row r="68" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
+        <v>90</v>
+      </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="2" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="G68" s="2"/>
     </row>
-    <row r="69" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
+      <c r="C69" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
+      <c r="F69" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="70" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
+      <c r="C70" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A71" s="8"/>
       <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
+      <c r="C71" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
+      <c r="F71" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="1:7" ht="323" x14ac:dyDescent="0.2">
-      <c r="A72" s="8" t="s">
-        <v>110</v>
-      </c>
+    <row r="72" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A72" s="8"/>
       <c r="B72" s="2"/>
-      <c r="C72" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
-      <c r="C73" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>270</v>
-      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
-      <c r="C74" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>271</v>
-      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A75" s="8"/>
+    <row r="75" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+      <c r="A75" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="F75" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="G75" s="2"/>
-    </row>
-    <row r="76" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
-        <v>111</v>
+        <v>255</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
+        <v>258</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>259</v>
+      </c>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="1:7" ht="136" x14ac:dyDescent="0.2">
-      <c r="A77" s="8" t="s">
-        <v>182</v>
-      </c>
+    <row r="77" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
-        <v>182</v>
+        <v>255</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+      <c r="G77" s="2"/>
+    </row>
+    <row r="78" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
-        <v>182</v>
+        <v>255</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="G78" s="2"/>
     </row>
-    <row r="79" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
-        <v>182</v>
+        <v>108</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>256</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
       <c r="G79" s="2"/>
     </row>
-    <row r="80" spans="1:7" ht="170" x14ac:dyDescent="0.2">
-      <c r="A80" s="8"/>
+    <row r="80" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A80" s="8" t="s">
+        <v>178</v>
+      </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>185</v>
+        <v>272</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="G80" s="2"/>
-    </row>
-    <row r="81" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G81" s="2"/>
+    </row>
+    <row r="82" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A82" s="8"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G82" s="2"/>
+    </row>
+    <row r="83" spans="1:7" s="4" customFormat="1" ht="170" x14ac:dyDescent="0.2">
+      <c r="A83" s="8"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G83" s="2"/>
+    </row>
+    <row r="84" spans="1:7" s="4" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A84" s="8"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D84" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" s="4" customFormat="1" ht="356" x14ac:dyDescent="0.2">
-      <c r="A82" s="8"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="G82" s="3"/>
-    </row>
-    <row r="83" spans="1:7" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A83" s="8"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="G83" s="3"/>
-    </row>
-    <row r="84" spans="1:7" s="4" customFormat="1" ht="170" x14ac:dyDescent="0.2">
-      <c r="A84" s="8"/>
-      <c r="B84" s="3"/>
-      <c r="C84" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="G84" s="3"/>
-    </row>
-    <row r="85" spans="1:7" s="4" customFormat="1" ht="204" x14ac:dyDescent="0.2">
+      <c r="E84" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="4" customFormat="1" ht="306" x14ac:dyDescent="0.2">
       <c r="A85" s="8"/>
       <c r="B85" s="3"/>
       <c r="C85" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>264</v>
+        <v>178</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="G85" s="3"/>
     </row>
-    <row r="86" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="8"/>
-      <c r="B86" s="2"/>
+      <c r="B86" s="3"/>
       <c r="C86" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="B87" s="2"/>
+        <v>178</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G86" s="3"/>
+    </row>
+    <row r="87" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="8"/>
+      <c r="B87" s="3"/>
       <c r="C87" s="2" t="s">
-        <v>274</v>
+        <v>178</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="G87" s="2"/>
-    </row>
-    <row r="88" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="G87" s="3"/>
+    </row>
+    <row r="88" spans="1:7" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="8"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-    </row>
-    <row r="89" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="B88" s="3"/>
+      <c r="C88" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G88" s="3"/>
+    </row>
+    <row r="89" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-      <c r="G89" s="2"/>
-    </row>
-    <row r="90" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="C89" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
-        <v>298</v>
+        <v>264</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2" t="s">
-        <v>301</v>
+        <v>263</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>304</v>
+        <v>283</v>
       </c>
       <c r="G90" s="2"/>
     </row>
     <row r="91" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
-      <c r="C91" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>300</v>
-      </c>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
@@ -3545,35 +3921,39 @@
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
-      <c r="D92" s="2" t="s">
-        <v>276</v>
-      </c>
+      <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
     </row>
-    <row r="93" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
-        <v>62</v>
+        <v>287</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2" t="s">
-        <v>63</v>
+        <v>290</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E93" s="2"/>
+        <v>291</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="F93" s="2" t="s">
-        <v>64</v>
+        <v>293</v>
       </c>
       <c r="G93" s="2"/>
     </row>
     <row r="94" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
+      <c r="C94" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>289</v>
+      </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -3582,55 +3962,47 @@
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
+      <c r="D95" s="2" t="s">
+        <v>265</v>
+      </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
     </row>
-    <row r="96" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A96" s="8"/>
+    <row r="96" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="A96" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
+      <c r="C96" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="E96" s="2"/>
-      <c r="F96" s="2"/>
+      <c r="F96" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="G96" s="2"/>
     </row>
-    <row r="97" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A97" s="8" t="s">
-        <v>102</v>
-      </c>
+    <row r="97" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A97" s="8"/>
       <c r="B97" s="2"/>
-      <c r="C97" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>100</v>
-      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
       <c r="E97" s="2"/>
-      <c r="F97" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+    </row>
+    <row r="98" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
-      <c r="C98" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D98" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
       <c r="E98" s="2"/>
-      <c r="F98" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>212</v>
-      </c>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
     </row>
     <row r="99" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A99" s="8"/>
@@ -3643,34 +4015,79 @@
     </row>
     <row r="100" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
+      <c r="C100" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-    </row>
-    <row r="101" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="F100" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A101" s="8"/>
       <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
+      <c r="C101" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-    </row>
-    <row r="102" spans="1:7" ht="40" x14ac:dyDescent="0.2">
-      <c r="A102" s="8" t="s">
-        <v>130</v>
-      </c>
+      <c r="F101" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A102" s="8"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
+    </row>
+    <row r="103" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="A103" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+    </row>
+    <row r="104" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="A104" s="8"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+    </row>
+    <row r="105" spans="1:7" ht="40" x14ac:dyDescent="0.2">
+      <c r="A105" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated PracticedAlgorithms sheet and some code refactoring
</commit_message>
<xml_diff>
--- a/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
+++ b/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asheshsingh/Documents/workspace-sts-3.9.6.RELEASE/java-projects/DataStructures/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF23F0B-FC26-FF47-9330-A3A137101B20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80180214-3D4C-154B-90A6-5B2DA7FD466C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3680" yWindow="460" windowWidth="33600" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -629,16 +629,6 @@
     <t>Capitalize a sentence by making first letter in each word capital letter</t>
   </si>
   <si>
-    <t>a) Create a char array from string
-b) Capitalize the first element (if it is not a space)
-c) Iterate through the array from 2nd element, look for character for which there's space on its left of it
-d) Replace that element with its capitalized form
-e) Once all done, create a new String from resulting array as new String(arr) and return it</t>
-  </si>
-  <si>
-    <t>Character.toUpperCase(char)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Given an input string and ordering string, need to return true if the ordering string is present in Input string.
 Example: Input: "hello world!", ordering: "hlo!", result: false, since 'l' comes after o (as well) in string.
 Another example: Input: "hello world!", ordering: "!od", result: false, since "!" appears after 'o' and 'd' in string.
@@ -664,19 +654,6 @@
   </si>
   <si>
     <t>Find out if String has duplicate chars and also remove them.</t>
-  </si>
-  <si>
-    <t>Method 1: Declare an int variable, checker = 0. iterate through string. Get int val = ch - 'a'. Then check if (checker &amp; (1 &lt;&lt; val) == 0) is true, add this char to StringBuffer, else continue. Here with 1 &lt;&lt; val, we are left shifting 0001 by val, say for char c, 1 &lt;&lt; 2 gives 0100, so 3rd bit is set. THis when bit wise anded (&amp;) with checker, must give 0 for c to not have appeared earlier since the next operation we do is, bit wise OR it with 1 &lt;&lt; val, meaning 0000 | 0100 = 0100, so 3rd bit is set on checker.
-Method 2: There are many other methods in removeDuplicatesWithTail(String word) method in StringManipulations class under com.datastructures.string package but tail based method is the best! Takes least amount of time as compared to Set, Map based and other methods. See approach of tail based method with String algorithms mentioned above.
-I call the best method as tail based method, which performed best for me so far!
-A) Do null / empty checks for input string and log message / error accordingly.
-B) str.toCharArray() to get a char array.
-C) Define a variable "tail" and initialize it to 1.
-D) Iterate from i=0 to len-1.
-E) Beginining of every iteration, define a new variable as int j = 0;
-F) Do a while loop as while (j &lt; tail) and check if arr[j] == arr[i]. If yes break the while loop, else, increment j by one.
-G) After while loop, check if j could reach all the way to tail (meaning no dups found till i so far). If so, move arr content at i to at tail and increment the tail.
-Once for loop finishes, return the string as new String.valueOf(arr, 0, tail). Note that last increment to tail helped us here as tail points to 'index till we need it' + 1.</t>
   </si>
   <si>
     <t>BinarySearchTree</t>
@@ -1914,6 +1891,167 @@
         <scheme val="minor"/>
       </rPr>
       <t>Note:: Solution 1 is abiout 16 times faster than 2, about 2.7 times faster than 3 in my code.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">a) Create an char array from string
+b) Capitalize the first element (if it is not a space)
+c) Iterate through the array from 2nd element, look for character for which there's space on its left of it
+d) Replace that element with its capitalized form
+e) Once all done, create a new String from resulting array as new String(arr) and return it
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> WordUtils.capitalize(str) will do the trick for you for entire string! Also preserves the white spaces in it!</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Character.toUpperCase(char)
+StringUtils.join(arr, " ") will join elements of an array using provided delilimiter.
+WordUtils.capitalize(string) will do everything needed in this problem, i.e.,
+   will capitalize entire string (first char of each word before space). G39 also will 
+  preserve any white F39spaces present in the string. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Declare an int variable, checker = 0. iterate through string. Get int val = ch - 'a'. Then check if (checker &amp; (1 &lt;&lt; val) == 0) is true, add this char to StringBuffer, else continue. Here with 1 &lt;&lt; val, we are left shifting 0001 by val, say for char c, 1 &lt;&lt; 2 gives 0100, so 3rd bit is set. This when bit wise anded (&amp;) with checker, must give 0 for c to not have appeared earlier since the next operation we do is, bit wise OR it with 1 &lt;&lt; val, meaning 0000 | 0100 = 0100, so 3rd bit is set on checker.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) Define a boolean array of size 128 or 256 depending on if string has only ASCII or non-ASCII characters.
+2) Iterate through chars of the string and use character itself as index of array to keep checking if arr[ch] (meaning it is true) and return false in that case. Very next line of code in same iteration of the loop needs to be: arr[ch] = true.
+3) Once the loop ends, return false since loop survived all the way and no where in the array a position was already holding true.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> boolean array elements get initialized with false by Java by default.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Method 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> There are many other methods in removeDuplicatesWithTail(String word) method in StringManipulations class under com.datastructures.string package but tail based method is the best! Takes least amount of time as compared to Set, Map based and other methods. See approach of tail based method with String algorithms mentioned above.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tail-based Method:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+I call the best method as tail based method, which performed best for me so far!
+A) Do null / empty checks for input string and log message / error accordingly.
+B) str.toCharArray() to get a char array.
+C) Define a variable "tail" and initialize it to 1.
+D) Iterate from i=0 to len-1.
+E) Beginining of every iteration, define a new variable as int j = 0;
+F) Do a while loop as while (j &lt; tail) and check if arr[j] == arr[i]. If yes break the while loop, else, increment j by one.
+G) After while loop, check if j could reach all the way to tail (meaning no dups found till i so far). If so, move arr content at i to at tail and increment the tail.
+Once for loop finishes, return the string as new String.valueOf(arr, 0, tail). Note that last increment to tail helped us here as tail points to 'index till we need it' + 1.</t>
     </r>
   </si>
 </sst>
@@ -2415,8 +2553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="E44" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2497,7 +2635,7 @@
         <v>153</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>8</v>
@@ -2532,10 +2670,10 @@
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -2748,13 +2886,13 @@
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>138</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="187" x14ac:dyDescent="0.2">
@@ -2767,10 +2905,10 @@
         <v>140</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G21" s="2"/>
     </row>
@@ -2778,16 +2916,16 @@
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>298</v>
       </c>
       <c r="G22" s="2"/>
     </row>
@@ -2795,19 +2933,19 @@
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -2842,7 +2980,7 @@
         <v>145</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>155</v>
@@ -2852,16 +2990,16 @@
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>308</v>
       </c>
       <c r="G26" s="2"/>
     </row>
@@ -2869,19 +3007,19 @@
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -2991,11 +3129,11 @@
         <v>53</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G34" s="2"/>
     </row>
@@ -3009,10 +3147,10 @@
         <v>129</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G35" s="2"/>
     </row>
@@ -3022,7 +3160,7 @@
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>31</v>
@@ -3031,7 +3169,7 @@
         <v>154</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>156</v>
@@ -3041,20 +3179,20 @@
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>4</v>
       </c>
@@ -3069,26 +3207,26 @@
         <v>168</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>169</v>
+        <v>317</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>170</v>
+        <v>318</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="388" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>316</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>319</v>
       </c>
       <c r="G39" s="2"/>
     </row>
@@ -3102,29 +3240,29 @@
         <v>119</v>
       </c>
       <c r="E40" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G41" s="2"/>
     </row>
@@ -3160,7 +3298,7 @@
       </c>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" ht="340" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
@@ -3170,10 +3308,10 @@
         <v>58</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>177</v>
+        <v>319</v>
       </c>
       <c r="G44" s="2"/>
     </row>
@@ -3183,7 +3321,7 @@
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>31</v>
@@ -3192,7 +3330,7 @@
         <v>154</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>156</v>
@@ -3204,16 +3342,16 @@
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G46" s="2"/>
     </row>
@@ -3251,16 +3389,16 @@
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="G49" s="2"/>
     </row>
@@ -3270,16 +3408,16 @@
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="G50" s="2"/>
     </row>
@@ -3295,10 +3433,10 @@
         <v>45</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G51" s="2"/>
     </row>
@@ -3308,16 +3446,16 @@
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="G52" s="2"/>
     </row>
@@ -3327,19 +3465,19 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="255" x14ac:dyDescent="0.2">
@@ -3348,16 +3486,16 @@
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G54" s="3"/>
     </row>
@@ -3367,16 +3505,16 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>219</v>
       </c>
       <c r="G55" s="2"/>
     </row>
@@ -3422,16 +3560,16 @@
       <c r="A58" s="8"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G58" s="2"/>
     </row>
@@ -3445,10 +3583,10 @@
         <v>46</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G59" s="2"/>
     </row>
@@ -3456,16 +3594,16 @@
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G60" s="2"/>
     </row>
@@ -3567,7 +3705,7 @@
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>103</v>
@@ -3632,16 +3770,16 @@
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>110</v>
@@ -3651,16 +3789,16 @@
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>258</v>
-      </c>
       <c r="E76" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G76" s="2"/>
     </row>
@@ -3668,16 +3806,16 @@
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G77" s="2"/>
     </row>
@@ -3685,16 +3823,16 @@
       <c r="A78" s="8"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G78" s="2"/>
     </row>
@@ -3713,39 +3851,39 @@
     </row>
     <row r="80" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G81" s="2"/>
     </row>
@@ -3753,16 +3891,16 @@
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G82" s="2"/>
     </row>
@@ -3770,16 +3908,16 @@
       <c r="A83" s="8"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="E83" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G83" s="2"/>
     </row>
@@ -3787,35 +3925,35 @@
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:7" s="4" customFormat="1" ht="306" x14ac:dyDescent="0.2">
       <c r="A85" s="8"/>
       <c r="B85" s="3"/>
       <c r="C85" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G85" s="3"/>
     </row>
@@ -3823,16 +3961,16 @@
       <c r="A86" s="8"/>
       <c r="B86" s="3"/>
       <c r="C86" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G86" s="3"/>
     </row>
@@ -3840,16 +3978,16 @@
       <c r="A87" s="8"/>
       <c r="B87" s="3"/>
       <c r="C87" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G87" s="3"/>
     </row>
@@ -3857,16 +3995,16 @@
       <c r="A88" s="8"/>
       <c r="B88" s="3"/>
       <c r="C88" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G88" s="3"/>
     </row>
@@ -3874,37 +4012,37 @@
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G90" s="2"/>
     </row>
@@ -3928,20 +4066,20 @@
     </row>
     <row r="93" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F93" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>293</v>
       </c>
       <c r="G93" s="2"/>
     </row>
@@ -3949,10 +4087,10 @@
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
@@ -3963,7 +4101,7 @@
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
@@ -4043,10 +4181,10 @@
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="19" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated PracticedAlgorithms.xlsx and some code refactoring
</commit_message>
<xml_diff>
--- a/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
+++ b/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asheshsingh/Documents/workspace-sts-3.9.6.RELEASE/java-projects/DataStructures/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80180214-3D4C-154B-90A6-5B2DA7FD466C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729F71D6-8F6E-CF4C-801A-FA9D0AA6695A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="460" windowWidth="33600" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="333">
   <si>
     <t>Data Structure</t>
   </si>
@@ -440,9 +440,6 @@
     <t>Given an input string and ordering string, need to return true if the ordering string is present in Input string. Example: Input: "hello world!", ordering: "hlo!", result: false, since 'l' comes after o (as well) in string. Another example: Input: "hello world!", ordering: "!od", result: false, since "!" appears after 'o' and 'd' in string. Last example: Input: "hello world", ordering: "he!", result true</t>
   </si>
   <si>
-    <t>1) Since ordering string is small, interate through it backwards, for every character, have another loop beginning from index before the first index till 0 and check if last first index (str.indexOf()) of main character in given string is less than lastIndexOf (str.lastIndexOf()) characters before main character in inner loop and if condition met, return false. Return true if all of loop survives.</t>
-  </si>
-  <si>
     <t>StringAsSpaceSeparatedSequence</t>
   </si>
   <si>
@@ -550,12 +547,6 @@
 4) Since we also want to return the max substring, add this to map with key as length of StringBuiler and value as one of values of List&lt;String&gt;. You'll have to check if key exists, in that case, get the value(list) and add to it, otherwise create a new list, add StringBuilder in it and add that list as value with key as length of StringBuilder.
 5) With above done, clear the StringBuilder by calling delete(0, &lt;length of StringBuilder&gt;) and then add the String (char) found at i to StringBuilder.
 Once, all done, get the list from map with key as maxSubStringLength and return it.</t>
-  </si>
-  <si>
-    <t>Important Java methods to remember:
-A) char can be converted to string by Character.toString(ch).
-B) StringBuilder has indexOf(String str), returns -1 if not present
-C) String's substring(fromIndex, toIndex), toIndex is not inclusive</t>
   </si>
   <si>
     <t xml:space="preserve">You are given a list of numbers. For each number, find the next bigger number that appears. When not found, print -1.
@@ -1377,18 +1368,6 @@
 5) pop(): </t>
   </si>
   <si>
-    <t>Here, time complexity will be of O(n). We need a storage of 256 characters but that should not be the big deal
- * Solution: 
- a) Define an int array of size 256. It can be 128 if pure ascii is contained by strings 
- b) Initialize first element of this array by -1. Rest of them by default will have 0 and we are good with them.
- c) loop through each chars of str1 and store their indices in array. Index of array will be ascii values of str1 chars: 
-     arr[str1.charAt(i)] = i
- d) Loop through str2 chars, check if a char is present in str1 by checking arr[ch] &lt;= 0, if not continue checking.
- e) If chars match, save the position of char position and define another variable (beginIndex = j) to check subsequent substrings. Define a new variable endIndex as beginIndex + 1. 
- f) Do a while loop with condition as endIndex should be &lt;= length of str2 to keep checking if str1 contans the substring from str2 begining from beginIndex to endIndex and each time this true, increment the endIndex. See how far we can go, i.e., how large of substring is common from position we saved earlier as beginIndex. Break from while loop whenever there is no match.
- g) when while loop exits, check length of substring found, compare the maxLength of the result we got so far, same the new max, if bigger one is found and store the resulting string to return finally.</t>
-  </si>
-  <si>
     <t>ArrayCommonElements</t>
   </si>
   <si>
@@ -2054,12 +2033,323 @@
 Once for loop finishes, return the string as new String.valueOf(arr, 0, tail). Note that last increment to tail helped us here as tail points to 'index till we need it' + 1.</t>
     </r>
   </si>
+  <si>
+    <t>1) Do null and empty checks using StringUtils.isEmpty(str) for input and ordering strings.
+2) Iterate through ordering string from index 1, check on input string if first index of current char of ordering string is less than last idex of previous char of ordering string in the input string, i.e., str.indexOf(ordering.charAt(i) &lt; str.lastIndexOf(ordering.charAt(i-1))). If so, return false.
+3) After the loop, return true (since it survied till now).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+1) There is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>not</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> firstIndexOf in String class. It is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>str.indexOf()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+2) There is indeed</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lastIndexOf() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in String class.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Important Java methods to remember:
+A) char can be converted to string by Character.toString(ch).
+B) StringBuilder has indexOf(String str), returns -1 if not present
+C) String's substring(fromIndex, toIndex), toIndex is not inclusive
+D) You can use map.getOrDefault(key, default), e.g.:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>List&lt;String&gt; list = map.getOrDefault(tempLen, new ArrayList&lt;&gt;());
+list.add(sb.toString());
+map.put(tempLen, list);</t>
+    </r>
+  </si>
+  <si>
+    <t>Here, time complexity will be of O(n). We need a storage of 256 characters but that should not be the big deal
+ * Solution: 
+ a) Define an int array of size 256. It can be 128 if pure ascii is contained by strings 
+ b) Initialize each element of this array by -1 iinstead of going with default whcih is 0. We're going to store indices of string characters in arr elements so -1 will help not contradict with 0 index for strings.
+ c) Loop through each chars of str1 and store their indices in array. Index of array will be ascii values of str1 chars: 
+     arr[str1.charAt(i)] = i
+ d) Loop through str2 chars, check if a char is present in str1 by checking arr[ch] &gt;= 0, chars match here, if not, continue checking.
+ e) If chars match, save the position of char position and define another variable (beginIndex = j) to check subsequent substrings. Define a new variable endIndex as beginIndex + 1. 
+ f) Do a while loop with condition as endIndex should be &lt;= length of str2 to keep checking if str1 contans the substring from str2 begining from beginIndex to endIndex and each time this true, increment the endIndex. See how far we can go, i.e., how large of substring is common from position we saved earlier as beginIndex. Break from while loop whenever there is no match.
+ g) when while loop exits, check length of substring found, compare the maxLength of the result we got so far, save the new max, if bigger one is found and store the resulting string to return finally.</t>
+  </si>
+  <si>
+    <t>ReplaceSpacesByPercent20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">replaceSpacesByPercent20StringUtils(String str) </t>
+  </si>
+  <si>
+    <t>Given a string, replace the spaces in between by %20. Used in URL Encoding.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Solution:
+You can do it manually by calculating number of spaces, creating a new array with length of string + (3-1) characters of each space replaced by %20 and then reading string and populating the new array with results, finally return new String(arr).
+There is an easier way. I would create an array arr, by splitting the string by space as delimiter (str.split(" ")), then use org.apache.commons.lang3 package's </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">StringUtils </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">method: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>StringUtils.join(arr, "%20")</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to return the string we need!</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">StringUtils.join(arr, "%20") </t>
+  </si>
+  <si>
+    <t>ReverseString</t>
+  </si>
+  <si>
+    <t>reverse(String word)
+reverse2(String word)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) Strings are immutable, so we create a char array out of it, reverse the characteres and then create a new string from that array.
+2) Read the char array both ways till indices match and swap characters. This way you're doing it by O(n/2) insteaf of O(n).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method2: Recursion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) The problem comes down to Get reverse of string: str.substring(1) and append str.substring(0) with it. (.substring(1) means take all the chars begining from index 1).
+2) So, use the breaking condition as</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if (str.length() == 1) return str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and return:
+r</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>eturn reverse2(str.substring(1)) + str.substring(0);</t>
+    </r>
+  </si>
+  <si>
+    <t>ReverseStringButSpecialChars</t>
+  </si>
+  <si>
+    <t>String reverse(String str)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Solution:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) It is like reversing string with swapping two ends of the char array method, except here, we take a while loop with (i&lt;j) where i and j are two ends of the indices.
+2) Within the loop, move i and j by a while loop right and left respectively for as many characters whihc are not Special Chars, Character.isAlphabetic(char) method can help here.
+3) Finally within the loop, do i++ and j--.
+4) Once loop done, return new String(arr).</t>
+    </r>
+  </si>
+  <si>
+    <t>Character.isAlphabetic(char)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2120,6 +2410,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2551,23 +2846,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E44" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.5" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" customWidth="1"/>
+    <col min="5" max="5" width="63.1640625" customWidth="1"/>
     <col min="6" max="6" width="105.1640625" customWidth="1"/>
     <col min="7" max="7" width="67.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="25" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -2578,12 +2873,12 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="21">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
@@ -2592,24 +2887,24 @@
         <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="33" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -2619,29 +2914,29 @@
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="272" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="272">
       <c r="A4" s="8"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="83" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -2651,7 +2946,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>13</v>
@@ -2660,7 +2955,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="83" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -2670,33 +2965,33 @@
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="238" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="187">
       <c r="A7" s="8"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>151</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="51">
       <c r="A8" s="8"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -2713,7 +3008,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="51">
       <c r="A9" s="8"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -2726,7 +3021,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="19">
       <c r="A10" s="8"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2739,7 +3034,7 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="34">
       <c r="A11" s="8"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2754,7 +3049,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="68">
       <c r="A12" s="8"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2769,7 +3064,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="153">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2784,7 +3079,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="51">
       <c r="A14" s="8"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2799,7 +3094,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="51">
       <c r="A15" s="8"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
@@ -2814,7 +3109,7 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="34">
       <c r="A16" s="8"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
@@ -2827,7 +3122,7 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="51">
       <c r="A17" s="8"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
@@ -2842,7 +3137,7 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="119">
       <c r="A18" s="8"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -2851,32 +3146,34 @@
       <c r="D18" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="F18" s="2" t="s">
-        <v>121</v>
+        <v>317</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="221" x14ac:dyDescent="0.2">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="221">
       <c r="A19" s="8"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="85">
       <c r="A20" s="8"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -2886,69 +3183,69 @@
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="187">
       <c r="A21" s="8"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>140</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="136">
       <c r="A22" s="8"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>295</v>
-      </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="238" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="238">
       <c r="A23" s="8"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" ht="34">
       <c r="A24" s="8"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -2958,7 +3255,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>18</v>
@@ -2967,62 +3264,62 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="153">
       <c r="A25" s="8"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="187">
       <c r="A26" s="8"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>305</v>
-      </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="289">
       <c r="A27" s="8"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="F27" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:7" ht="51">
       <c r="A28" s="8"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
@@ -3039,14 +3336,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="34">
       <c r="A29" s="8"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
@@ -3054,7 +3351,7 @@
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" ht="299" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="299" customHeight="1">
       <c r="A30" s="8"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
@@ -3064,16 +3361,16 @@
         <v>28</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="293" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="293" customHeight="1">
       <c r="A31" s="8"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
@@ -3083,7 +3380,7 @@
         <v>35</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>36</v>
@@ -3092,7 +3389,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="19">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
@@ -3107,7 +3404,7 @@
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="19">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
@@ -3122,115 +3419,115 @@
       </c>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="136">
       <c r="A34" s="8"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="85">
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="372" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="372">
       <c r="A36" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="323" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:7" ht="323">
       <c r="A37" s="8"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="119">
       <c r="A38" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="388" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="388">
       <c r="A39" s="8"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>316</v>
-      </c>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="204">
       <c r="A40" s="8"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
@@ -3240,33 +3537,33 @@
         <v>119</v>
       </c>
       <c r="E40" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:7" ht="409.6">
       <c r="A41" s="8"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>291</v>
+        <v>320</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="19">
       <c r="A42" s="8"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
@@ -3275,15 +3572,15 @@
       <c r="D42" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E42" s="2"/>
+      <c r="E42" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="F42" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" ht="102">
       <c r="A43" s="8"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
@@ -3298,7 +3595,7 @@
       </c>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="409.6">
       <c r="A44" s="8"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
@@ -3308,367 +3605,391 @@
         <v>58</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" ht="372" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
-        <v>30</v>
-      </c>
+    <row r="45" spans="1:7" ht="119">
+      <c r="A45" s="8"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>190</v>
+        <v>321</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>31</v>
+        <v>322</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>154</v>
+        <v>323</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>299</v>
+        <v>324</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="323" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>30</v>
-      </c>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="221">
+      <c r="A46" s="8"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>191</v>
+        <v>326</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>192</v>
+        <v>327</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>300</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="153">
       <c r="A47" s="8"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>159</v>
+        <v>329</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>160</v>
+        <v>330</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>161</v>
+        <v>331</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
+        <v>332</v>
+      </c>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" ht="372">
+      <c r="A48" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-    </row>
-    <row r="49" spans="1:7" ht="356" x14ac:dyDescent="0.2">
+      <c r="C48" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="323">
       <c r="A49" s="8" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>236</v>
+        <v>189</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>237</v>
+        <v>190</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>238</v>
+        <v>191</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>239</v>
+        <v>297</v>
       </c>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" ht="255" x14ac:dyDescent="0.2">
-      <c r="A50" s="8" t="s">
-        <v>43</v>
-      </c>
+    <row r="50" spans="1:7" ht="102">
+      <c r="A50" s="8"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>224</v>
+        <v>157</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>225</v>
+        <v>158</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>226</v>
+        <v>159</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="G50" s="2"/>
-    </row>
-    <row r="51" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
-        <v>43</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="19">
+      <c r="A51" s="8"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>229</v>
-      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
       <c r="G51" s="2"/>
     </row>
-    <row r="52" spans="1:7" s="4" customFormat="1" ht="323" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="356">
       <c r="A52" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>201</v>
+        <v>234</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>202</v>
+        <v>235</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>203</v>
+        <v>236</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>204</v>
+        <v>237</v>
       </c>
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="255">
       <c r="A53" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="255" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="1:7" ht="153">
       <c r="A54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3" t="s">
-        <v>210</v>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="G54" s="3"/>
-    </row>
-    <row r="55" spans="1:7" ht="121" customHeight="1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="1:7" s="4" customFormat="1" ht="323">
       <c r="A55" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:7" ht="215" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="409.6">
       <c r="A56" s="8" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>38</v>
+        <v>203</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>40</v>
+        <v>204</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>39</v>
+        <v>205</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>158</v>
+        <v>206</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="102" x14ac:dyDescent="0.2">
-      <c r="A57" s="8"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2" t="s">
-        <v>41</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="255">
+      <c r="A57" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G57" s="2"/>
-    </row>
-    <row r="58" spans="1:7" ht="221" x14ac:dyDescent="0.2">
-      <c r="A58" s="8"/>
+        <v>204</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" ht="121" customHeight="1">
+      <c r="A58" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>308</v>
+        <v>214</v>
       </c>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A59" s="8"/>
+    <row r="59" spans="1:7" ht="215" customHeight="1">
+      <c r="A59" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>188</v>
+        <v>39</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="G59" s="2"/>
-    </row>
-    <row r="60" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="102">
       <c r="A60" s="8"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>198</v>
+        <v>41</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>196</v>
+        <v>42</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>301</v>
+        <v>163</v>
       </c>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="221">
       <c r="A61" s="8"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>48</v>
+        <v>219</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E61" s="2"/>
+        <v>220</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>221</v>
+      </c>
       <c r="F61" s="2" t="s">
-        <v>50</v>
+        <v>305</v>
       </c>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="153">
       <c r="A62" s="8"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E62" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="F62" s="2" t="s">
-        <v>56</v>
+        <v>306</v>
       </c>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A63" s="9"/>
+    <row r="63" spans="1:7" ht="187">
+      <c r="A63" s="8"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>298</v>
+      </c>
       <c r="G63" s="2"/>
     </row>
-    <row r="64" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="51">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
+      <c r="C64" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
+      <c r="F64" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="G64" s="2"/>
     </row>
-    <row r="65" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="409.6">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
+      <c r="C65" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
+      <c r="F65" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="G65" s="2"/>
     </row>
-    <row r="66" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A66" s="8"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
+    <row r="66" spans="1:7" ht="19">
+      <c r="A66" s="9"/>
       <c r="G66" s="2"/>
     </row>
-    <row r="67" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="19">
       <c r="A67" s="8"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -3677,517 +3998,499 @@
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A68" s="8" t="s">
-        <v>90</v>
-      </c>
+    <row r="68" spans="1:7" ht="19">
+      <c r="A68" s="8"/>
       <c r="B68" s="2"/>
-      <c r="C68" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>92</v>
-      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
       <c r="E68" s="2"/>
-      <c r="F68" s="2" t="s">
-        <v>93</v>
-      </c>
+      <c r="F68" s="2"/>
       <c r="G68" s="2"/>
     </row>
-    <row r="69" spans="1:7" ht="221" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="19">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
-      <c r="C69" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
       <c r="E69" s="2"/>
-      <c r="F69" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" ht="19">
       <c r="A70" s="8"/>
       <c r="B70" s="2"/>
-      <c r="C70" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
       <c r="G70" s="2"/>
     </row>
-    <row r="71" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A71" s="8"/>
+    <row r="71" spans="1:7" ht="20">
+      <c r="A71" s="8" t="s">
+        <v>90</v>
+      </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="2" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="221">
       <c r="A72" s="8"/>
       <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
+      <c r="C72" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
-    </row>
-    <row r="73" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="F72" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="19">
       <c r="A73" s="8"/>
       <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
+      <c r="C73" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="19">
       <c r="A74" s="8"/>
       <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
+      <c r="C74" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
+      <c r="F74" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="1:7" ht="289" x14ac:dyDescent="0.2">
-      <c r="A75" s="8" t="s">
-        <v>107</v>
-      </c>
+    <row r="75" spans="1:7" ht="19">
+      <c r="A75" s="8"/>
       <c r="B75" s="2"/>
-      <c r="C75" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+    </row>
+    <row r="76" spans="1:7" ht="19">
       <c r="A76" s="8"/>
       <c r="B76" s="2"/>
-      <c r="C76" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>256</v>
-      </c>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="19">
       <c r="A77" s="8"/>
       <c r="B77" s="2"/>
-      <c r="C77" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>257</v>
-      </c>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
       <c r="G77" s="2"/>
     </row>
-    <row r="78" spans="1:7" ht="153" x14ac:dyDescent="0.2">
-      <c r="A78" s="8"/>
+    <row r="78" spans="1:7" ht="289">
+      <c r="A78" s="8" t="s">
+        <v>107</v>
+      </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="G78" s="2"/>
-    </row>
-    <row r="79" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="G78" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="153">
       <c r="A79" s="8"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
-        <v>108</v>
+        <v>250</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
+        <v>253</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>254</v>
+      </c>
       <c r="G79" s="2"/>
     </row>
-    <row r="80" spans="1:7" ht="136" x14ac:dyDescent="0.2">
-      <c r="A80" s="8" t="s">
-        <v>175</v>
-      </c>
+    <row r="80" spans="1:7" ht="68">
+      <c r="A80" s="8"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>175</v>
+        <v>250</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+      <c r="G80" s="2"/>
+    </row>
+    <row r="81" spans="1:7" ht="153">
       <c r="A81" s="8"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2" t="s">
-        <v>175</v>
+        <v>250</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="G81" s="2"/>
     </row>
-    <row r="82" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="19">
       <c r="A82" s="8"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
-        <v>175</v>
+        <v>108</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>242</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
       <c r="G82" s="2"/>
     </row>
-    <row r="83" spans="1:7" s="4" customFormat="1" ht="170" x14ac:dyDescent="0.2">
-      <c r="A83" s="8"/>
+    <row r="83" spans="1:7" ht="136">
+      <c r="A83" s="8" t="s">
+        <v>173</v>
+      </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>178</v>
+        <v>267</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="G83" s="2"/>
-    </row>
-    <row r="84" spans="1:7" s="4" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="85">
       <c r="A84" s="8"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G84" s="2"/>
+    </row>
+    <row r="85" spans="1:7" ht="102">
+      <c r="A85" s="8"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="E85" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G85" s="2"/>
+    </row>
+    <row r="86" spans="1:7" s="4" customFormat="1" ht="170">
+      <c r="A86" s="8"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G86" s="2"/>
+    </row>
+    <row r="87" spans="1:7" s="4" customFormat="1" ht="119">
+      <c r="A87" s="8"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G87" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E84" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="4" customFormat="1" ht="306" x14ac:dyDescent="0.2">
-      <c r="A85" s="8"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="G85" s="3"/>
-    </row>
-    <row r="86" spans="1:7" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A86" s="8"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="G86" s="3"/>
-    </row>
-    <row r="87" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="8"/>
-      <c r="B87" s="3"/>
-      <c r="C87" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="E87" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="G87" s="3"/>
-    </row>
-    <row r="88" spans="1:7" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:7" s="4" customFormat="1" ht="306">
       <c r="A88" s="8"/>
       <c r="B88" s="3"/>
       <c r="C88" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>250</v>
+        <v>173</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="G88" s="3"/>
     </row>
-    <row r="89" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" s="4" customFormat="1" ht="34">
       <c r="A89" s="8"/>
-      <c r="B89" s="2"/>
+      <c r="B89" s="3"/>
       <c r="C89" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A90" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="B90" s="2"/>
+        <v>173</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="1:7" ht="22" customHeight="1">
+      <c r="A90" s="8"/>
+      <c r="B90" s="3"/>
       <c r="C90" s="2" t="s">
-        <v>260</v>
+        <v>173</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="G90" s="2"/>
-    </row>
-    <row r="91" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G90" s="3"/>
+    </row>
+    <row r="91" spans="1:7" ht="409" customHeight="1">
       <c r="A91" s="8"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="2"/>
-    </row>
-    <row r="92" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="B91" s="3"/>
+      <c r="C91" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="G91" s="3"/>
+    </row>
+    <row r="92" spans="1:7" ht="34">
       <c r="A92" s="8"/>
       <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
-    </row>
-    <row r="93" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="C92" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="409.6">
       <c r="A93" s="8" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="2" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="G93" s="2"/>
     </row>
-    <row r="94" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" ht="19">
       <c r="A94" s="8"/>
       <c r="B94" s="2"/>
-      <c r="C94" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>286</v>
-      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
     </row>
-    <row r="95" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" ht="19">
       <c r="A95" s="8"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
-      <c r="D95" s="2" t="s">
-        <v>262</v>
-      </c>
+      <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
     </row>
-    <row r="96" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" ht="119">
       <c r="A96" s="8" t="s">
-        <v>59</v>
+        <v>282</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="2" t="s">
-        <v>60</v>
+        <v>285</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E96" s="2"/>
+        <v>286</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>287</v>
+      </c>
       <c r="F96" s="2" t="s">
-        <v>61</v>
+        <v>288</v>
       </c>
       <c r="G96" s="2"/>
     </row>
-    <row r="97" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" ht="19">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
+      <c r="C97" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>284</v>
+      </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
     </row>
-    <row r="98" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" ht="19">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
+      <c r="D98" s="2" t="s">
+        <v>260</v>
+      </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
     </row>
-    <row r="99" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A99" s="8"/>
+    <row r="99" spans="1:7" ht="20">
+      <c r="A99" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
+      <c r="C99" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
+      <c r="F99" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="G99" s="2"/>
     </row>
-    <row r="100" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="A100" s="8" t="s">
-        <v>99</v>
-      </c>
+    <row r="100" spans="1:7" ht="19">
+      <c r="A100" s="8"/>
       <c r="B100" s="2"/>
-      <c r="C100" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
       <c r="E100" s="2"/>
-      <c r="F100" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+    </row>
+    <row r="101" spans="1:7" ht="19">
       <c r="A101" s="8"/>
       <c r="B101" s="2"/>
-      <c r="C101" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>102</v>
-      </c>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
       <c r="E101" s="2"/>
-      <c r="F101" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+    </row>
+    <row r="102" spans="1:7" ht="19">
       <c r="A102" s="8"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -4196,36 +4499,81 @@
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" ht="20">
       <c r="A103" s="8" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
+      <c r="C103" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
-    </row>
-    <row r="104" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="F103" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="187">
       <c r="A104" s="8"/>
       <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
+      <c r="C104" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
-    </row>
-    <row r="105" spans="1:7" ht="40" x14ac:dyDescent="0.2">
-      <c r="A105" s="8" t="s">
-        <v>127</v>
-      </c>
+      <c r="F104" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="19">
+      <c r="A105" s="8"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
+    </row>
+    <row r="106" spans="1:7" ht="20">
+      <c r="A106" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
+    </row>
+    <row r="107" spans="1:7" ht="19">
+      <c r="A107" s="8"/>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
+    </row>
+    <row r="108" spans="1:7" ht="40">
+      <c r="A108" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Some code refactoring. Added some more synchronizers in multithreading package
</commit_message>
<xml_diff>
--- a/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
+++ b/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asheshsingh/Documents/workspace-sts-3.9.6.RELEASE/java-projects/DataStructures/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729F71D6-8F6E-CF4C-801A-FA9D0AA6695A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7922E49F-3601-5F4C-9CBF-493B001822AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="460" windowWidth="33600" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="366">
   <si>
     <t>Data Structure</t>
   </si>
@@ -390,9 +390,6 @@
   </si>
   <si>
     <t>Implemented by recursion, check implementation in STS Project</t>
-  </si>
-  <si>
-    <t>LikedList</t>
   </si>
   <si>
     <t>SumNumberRepresentedAsLinkedList</t>
@@ -2344,6 +2341,472 @@
   <si>
     <t>Character.isAlphabetic(char)</t>
   </si>
+  <si>
+    <t>SortDecimalsAsStrings</t>
+  </si>
+  <si>
+    <t>sortDecimalsAsString(String [] strArr)</t>
+  </si>
+  <si>
+    <t>How would you sort an array of strings containing decimal values while preserving the decimal places
+ including leading or trailing zeros. Also preserving leading zeros before the decimal place.
+ Example:
+ Input: {"-100", "00.12", ".12", "02.340"}
+ Output: {"02.340", "00.12", ".12", "-100"}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>We can convert the string array to Double or BigDecimal array (since they preserves decimal precision)
+ by: Double.parseDouble(str) or new BigDecimal(string) for individual elements, but the catch there will be when we
+ convert BigDecimal back to string, we lose the leading zeros before decimal, like "00.12" when converted to
+ Double or BigDecimal and back to string, it will become "0.12", which is not what we want.
+ Hence, the solution in this case is to go for Arrays.sort with string array itself and provide a comparator there
+ which uses Double or BigDecimal to compare the strings:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Method 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Arrays.sort(strArr, Comparator.comparing((String str) -&gt; {
+            // We can use BigDecimal or Double here to compare strings
+            // BigDecimal decimal = new BigDecimal(str);
+            Double decimal = Double.parseDouble(str);
+            return decimal;
+        }).reversed());
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Arrays.sort(strArr, 0, strArr.length, (a, b) -&gt; -(new Double(a).compareTo(new Double(b))));
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Arrays.sort(strArr, 0, strArr.length, (a, b) -&gt; new BigDecimal(b).compareTo(new BigDecimal(a)));</t>
+    </r>
+  </si>
+  <si>
+    <t>Do not change original strings, convert them only while comparing them using Comparator, to Decimal or BigDecimal. That way original strings will be preserved!</t>
+  </si>
+  <si>
+    <t>UniqueIntegersAmongAllSubarrays</t>
+  </si>
+  <si>
+    <t>Directly solved in main method</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Given an array or Integers, find maximum number of unique elements in contiguous subarrays (e.g., elements on indices 0, 1, 2; 1, 2, 3..and so on) of size m (= 3 in this example):
+Array: {5, 3, 5, 2, 3, 2}, m = 3.
+Result: 3
+Explanation:
+Subarray [5, 3, 5] -&gt; Unique chars: 2
+Subarray [3, 5, 2] -&gt; Unique chars: 3
+Subarray [5, 2, 3] -&gt; Unique chars: 3
+Subarray [2, 3, 2] -&gt; Unique chars: 2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Answer: 3</t>
+    </r>
+  </si>
+  <si>
+    <t>Solution:
+1) Define an ArrayDequeue as Deque&lt;Integer&gt; deque = new ArrayDeque&lt;&gt;() and a Set&lt;Integer&gt; set = new HashSet&lt;&gt;(); Define result as int variable.
+2) Iterate through array. Add the element at index =i to deque and a set.
+3) Check if deque.size() == m, check set.size(), if more than max (result), replace result with this.
+4) Integer first = deque.removeFirst().
+5) if !deque.contains(first), set.remove(first).
+6) Finally, return result.</t>
+  </si>
+  <si>
+    <t>Deque can be deined as ArrayDeque or LinkedDeque. We're using Deque.removeFirst() and Deque.contains() methods here.</t>
+  </si>
+  <si>
+    <t>hackerrank</t>
+  </si>
+  <si>
+    <t>PriorityQueue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can create a min or max PriorityQueue and then poll will remove max / min elements from the Queue respectively. You can also peek or offer (add) to the queue.
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PriorityQueue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;Student&gt; queue = new PriorityQueue(
+            Comparator.comparing(Student::getCgpa).reversed()
+                    .thenComparing(Student::getName)
+                    .thenComparing(Student::getId)</t>
+    </r>
+  </si>
+  <si>
+    <t>Arrays</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hackerrank</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - array</t>
+    </r>
+  </si>
+  <si>
+    <t>hackerrank - string</t>
+  </si>
+  <si>
+    <t>LargestSmallestSubstringLexographicalOrder</t>
+  </si>
+  <si>
+    <t>getLargestSmallestSubstringsLexicographicalOrder(String s, int k)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Solution:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) Define two strings, smallest and largest, but by pulling substring(0, k-1) from given string.
+2) Define a method isGreater(String str1, String str2) which returns a boolean if str1 is greated than str2 or not.
+3) Iterate through input string with i=0, j=i+k-1; j&lt;str.length(); i++, j++.
+4) On each iteration, checked is str.substring(i, j+1) is greater than largest substring, if so, update the result for largest substring. Check also if the substring is smaller than smallest, if so, update the result for smallest substring as well.
+5) Finally, return smallest and largest results as a concatenated string with delimiter as we need it.</t>
+    </r>
+  </si>
+  <si>
+    <t>Regex</t>
+  </si>
+  <si>
+    <t>RegexUserNameValidator</t>
+  </si>
+  <si>
+    <t>Write a regex expression to validate username.</t>
+  </si>
+  <si>
+    <t>The username consists of 8 to 30 characters inclusive. If the username consists of less than 8 or greater than 30
+characters, then it is an invalid username. The username can only contain alphanumeric characters and
+underscores (_). Alphanumeric characters describe the character set consisting of lowercase characters [a-z],
+uppercase characters [A-Z], and digits [0-9].
+The first character of the username must be an alphabetic character, i.e., either lowercase character [a-z] or uppercase
+character [A-Z].</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">String regexUsername = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"[a-zA-Z]{1}\\w{7,29}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;
+        Pattern pattern = Pattern.compile(regexUsername);
+        Matcher matcher = pattern.matcher(username);
+        return matcher.matches();</t>
+    </r>
+  </si>
+  <si>
+    <t>RegexDuplicateWords</t>
+  </si>
+  <si>
+    <t>Remove duplicate words in a sentence, case insensitive way. E.g., Good bye bye Bye world World wOrLD" should become "Good bye world"</t>
+  </si>
+  <si>
+    <t>String regex = "\\b(\\w+)(?:\\W+\\1\\b)+" will do the trick here.</t>
+  </si>
+  <si>
+    <t>RegexIPValidation</t>
+  </si>
+  <si>
+    <t>Write a regex to validate IP Address which follows following rules: IP address is a string in the form "A.B.C.D", where the value of A, B, C, and D may range from 0 to 255.
+Leading zeros are allowed. The length of A, B, C, or D can't be greater than 3.</t>
+  </si>
+  <si>
+    <t>String regex = "([0-9]{1,2}|0[0-9]{1,2}|1[0-9]{1,2}|2[0-4][0-9]|25[0-5])"
+                + "\\.(0?[0-9]{1,2}|1[0-9]{1,2}|2[0-4][0-9]|25[0-5])"
+                + "\\.(0?[0-9]{1,2}|1[0-9]{1,2}|2[0-4][0-9]|25[0-5])"
+                + "\\.(0?[0-9]{1,2}|1[0-9]{1,2}|2[0-4][0-9]|25[0-5])";</t>
+  </si>
+  <si>
+    <t>RegexExtractXmlTagContents</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">From an XML like file, given a line, extract the content between valid tags. Example:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Input:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&lt;h1&gt;Nayeem loves counseling&lt;/h1&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Output:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Nayeem loves counseling,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Input:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&lt;h1&gt;&lt;h1&gt;Sanjay has no watch&lt;/h1&gt;&lt;/h1&gt;&lt;par&gt;So wait for a while&lt;/par&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Output:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Sanjay has no watch
+So wait for a while</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>/* Note: Below regex is the core of this solution!
+     A bracket denotes a group, first bracket (.+) is group1 which means tag name (between &lt; and &gt;). Second group is ([^&lt;]+) which is placed before &lt;/\\1&gt; (meaning &lt;/ then content from group 1 (tag name), then a &gt;). So, second group ([^&lt;]+) means content between tags and we are ensuring no occurrences of &lt; is present for a valid content.
+Beauty of defining groups (by brackets ()) is, we can then refer them and also use while loops to find them all! */
+        String regex =</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "&lt;(.+)&gt;([^&lt;]+)&lt;/\\1&gt;";</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+        Pattern pattern = Pattern.compile(regex);
+        Matcher matcher = pattern.matcher(input);
+        // This is where we say find all the matches
+        while (matcher.find()) {
+            // And we need second group, which is content basically, not tag name (which is first group)
+            result.add(matcher.group(2));
+            matchFound = true;
+        }
+return result;</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -2390,13 +2853,6 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2415,6 +2871,13 @@
       <sz val="12"/>
       <color rgb="FF002060"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2437,7 +2900,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2458,6 +2921,17 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -2502,7 +2976,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2512,21 +2986,29 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="39">
@@ -2846,10 +3328,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2857,54 +3339,54 @@
     <col min="1" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.5" customWidth="1"/>
-    <col min="5" max="5" width="63.1640625" customWidth="1"/>
+    <col min="5" max="5" width="72.83203125" customWidth="1"/>
     <col min="6" max="6" width="105.1640625" customWidth="1"/>
     <col min="7" max="7" width="67.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25" customHeight="1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" ht="21">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="33" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="33" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -2914,30 +3396,34 @@
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="272">
-      <c r="A4" s="8"/>
+      <c r="A4" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="83" customHeight="1">
-      <c r="A5" s="8"/>
+      <c r="A5" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>11</v>
@@ -2946,7 +3432,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>13</v>
@@ -2956,7 +3442,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="83" customHeight="1">
-      <c r="A6" s="8"/>
+      <c r="A6" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -2965,34 +3453,38 @@
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="187">
-      <c r="A7" s="8"/>
+      <c r="A7" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="51">
-      <c r="A8" s="8"/>
+      <c r="A8" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>62</v>
@@ -3008,8 +3500,10 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="51">
-      <c r="A9" s="8"/>
+    <row r="9" spans="1:7" ht="34">
+      <c r="A9" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
@@ -3021,8 +3515,10 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="19">
-      <c r="A10" s="8"/>
+    <row r="10" spans="1:7" ht="20">
+      <c r="A10" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
@@ -3035,7 +3531,9 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="34">
-      <c r="A11" s="8"/>
+      <c r="A11" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
@@ -3050,7 +3548,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="68">
-      <c r="A12" s="8"/>
+      <c r="A12" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
@@ -3064,8 +3564,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="153">
-      <c r="A13" s="8"/>
+    <row r="13" spans="1:7" ht="102">
+      <c r="A13" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
@@ -3079,8 +3581,10 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="51">
-      <c r="A14" s="8"/>
+    <row r="14" spans="1:7" ht="34">
+      <c r="A14" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
@@ -3094,8 +3598,10 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="51">
-      <c r="A15" s="8"/>
+    <row r="15" spans="1:7" ht="34">
+      <c r="A15" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
         <v>82</v>
@@ -3110,7 +3616,9 @@
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="34">
-      <c r="A16" s="8"/>
+      <c r="A16" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
         <v>85</v>
@@ -3122,8 +3630,10 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="51">
-      <c r="A17" s="8"/>
+    <row r="17" spans="1:7" ht="34">
+      <c r="A17" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>87</v>
@@ -3137,44 +3647,50 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="119">
-      <c r="A18" s="8"/>
+    <row r="18" spans="1:7" ht="102">
+      <c r="A18" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="F18" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="19" spans="1:7" ht="221">
-      <c r="A19" s="8"/>
+      <c r="A19" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="85">
-      <c r="A20" s="8"/>
+      <c r="A20" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
         <v>9</v>
@@ -3183,70 +3699,78 @@
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>294</v>
-      </c>
     </row>
     <row r="21" spans="1:7" ht="187">
-      <c r="A21" s="8"/>
+      <c r="A21" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="136">
-      <c r="A22" s="8"/>
+      <c r="A22" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="238">
-      <c r="A23" s="8"/>
+      <c r="A23" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>232</v>
-      </c>
     </row>
     <row r="24" spans="1:7" ht="34">
-      <c r="A24" s="8"/>
+      <c r="A24" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
         <v>15</v>
@@ -3255,7 +3779,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>18</v>
@@ -3265,62 +3789,70 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="153">
-      <c r="A25" s="8"/>
+      <c r="A25" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="187">
-      <c r="A26" s="8"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="170">
+      <c r="A26" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>302</v>
-      </c>
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" ht="289">
-      <c r="A27" s="8"/>
+      <c r="A27" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>218</v>
-      </c>
     </row>
     <row r="28" spans="1:7" ht="51">
-      <c r="A28" s="8"/>
+      <c r="A28" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
         <v>19</v>
@@ -3336,14 +3868,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="34">
-      <c r="A29" s="8"/>
+    <row r="29" spans="1:7" ht="20">
+      <c r="A29" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
@@ -3352,7 +3886,9 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" ht="299" customHeight="1">
-      <c r="A30" s="8"/>
+      <c r="A30" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
         <v>27</v>
@@ -3361,17 +3897,19 @@
         <v>28</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="293" customHeight="1">
-      <c r="A31" s="8"/>
+      <c r="A31" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
         <v>33</v>
@@ -3380,7 +3918,7 @@
         <v>35</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>36</v>
@@ -3389,8 +3927,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="19">
-      <c r="A32" s="8"/>
+    <row r="32" spans="1:7" ht="20">
+      <c r="A32" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
         <v>51</v>
@@ -3404,8 +3944,10 @@
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="19">
-      <c r="A33" s="8"/>
+    <row r="33" spans="1:7" ht="20">
+      <c r="A33" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
         <v>52</v>
@@ -3420,673 +3962,767 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" ht="136">
-      <c r="A34" s="8"/>
+      <c r="A34" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" ht="85">
-      <c r="A35" s="8"/>
+      <c r="A35" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="372">
-      <c r="A36" s="8" t="s">
-        <v>30</v>
+    <row r="36" spans="1:7" ht="221">
+      <c r="A36" s="7" t="s">
+        <v>346</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>31</v>
+        <v>219</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>152</v>
+        <v>220</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="323">
-      <c r="A37" s="8"/>
+        <v>304</v>
+      </c>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" ht="187">
+      <c r="A37" s="7" t="s">
+        <v>346</v>
+      </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>297</v>
       </c>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" ht="119">
-      <c r="A38" s="8" t="s">
-        <v>4</v>
+    <row r="38" spans="1:7" ht="289">
+      <c r="A38" s="9" t="s">
+        <v>347</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>164</v>
+        <v>332</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>165</v>
+        <v>333</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>166</v>
+        <v>334</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>314</v>
+        <v>335</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="388">
-      <c r="A39" s="8"/>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="187">
+      <c r="A39" s="9" t="s">
+        <v>347</v>
+      </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>310</v>
+        <v>337</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>312</v>
+        <v>339</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" ht="204">
-      <c r="A40" s="8"/>
+        <v>340</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="187">
+      <c r="A40" s="9" t="s">
+        <v>347</v>
+      </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>118</v>
+        <v>337</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>119</v>
+        <v>338</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>167</v>
+        <v>339</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>168</v>
+        <v>340</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="409.6">
-      <c r="A41" s="8"/>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="372">
+      <c r="A41" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>171</v>
+        <v>31</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>320</v>
+        <v>151</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" ht="19">
-      <c r="A42" s="8"/>
+        <v>295</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="323">
+      <c r="A42" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>112</v>
+        <v>189</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>113</v>
+        <v>190</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>114</v>
+        <v>296</v>
       </c>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" ht="102">
-      <c r="A43" s="8"/>
+    <row r="43" spans="1:7" ht="372">
+      <c r="A43" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>115</v>
+        <v>187</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E43" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="F43" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" ht="409.6">
-      <c r="A44" s="8"/>
+        <v>295</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="323">
+      <c r="A44" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>58</v>
+        <v>189</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" ht="119">
-      <c r="A45" s="8"/>
+    <row r="45" spans="1:7" ht="102">
+      <c r="A45" s="7"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>321</v>
+        <v>156</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>322</v>
+        <v>157</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>323</v>
+        <v>158</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>324</v>
+        <v>159</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="221">
-      <c r="A46" s="8"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="19">
+      <c r="A46" s="7"/>
       <c r="B46" s="2"/>
-      <c r="C46" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>328</v>
-      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" ht="153">
-      <c r="A47" s="8"/>
+    <row r="47" spans="1:7" ht="356">
+      <c r="A47" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>329</v>
+        <v>233</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>330</v>
+        <v>234</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>331</v>
+        <v>235</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>332</v>
+        <v>236</v>
       </c>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="1:7" ht="372">
-      <c r="A48" s="8" t="s">
-        <v>30</v>
+    <row r="48" spans="1:7" ht="255">
+      <c r="A48" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>31</v>
+        <v>222</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>152</v>
+        <v>223</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="323">
-      <c r="A49" s="8" t="s">
-        <v>30</v>
+        <v>225</v>
+      </c>
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" ht="153">
+      <c r="A49" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>189</v>
+        <v>44</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>190</v>
+        <v>45</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>191</v>
+        <v>224</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>297</v>
+        <v>226</v>
       </c>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" ht="102">
-      <c r="A50" s="8"/>
+    <row r="50" spans="1:7" ht="323">
+      <c r="A50" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>157</v>
+        <v>198</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>158</v>
+        <v>199</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>159</v>
+        <v>200</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="19">
-      <c r="A51" s="8"/>
+        <v>201</v>
+      </c>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" ht="409.6">
+      <c r="A51" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="1:7" ht="356">
-      <c r="A52" s="8" t="s">
+      <c r="C51" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="255">
+      <c r="A52" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2" t="s">
-        <v>234</v>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="G52" s="2"/>
-    </row>
-    <row r="53" spans="1:7" ht="255">
-      <c r="A53" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="1:7" ht="170">
+      <c r="A53" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="1:7" ht="153">
-      <c r="A54" s="8" t="s">
-        <v>43</v>
+    <row r="54" spans="1:7" ht="119">
+      <c r="A54" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
-        <v>44</v>
+        <v>163</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>45</v>
+        <v>164</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>225</v>
+        <v>165</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="1:7" s="4" customFormat="1" ht="323">
-      <c r="A55" s="8" t="s">
-        <v>43</v>
+        <v>313</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="388">
+      <c r="A55" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>199</v>
+        <v>309</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>200</v>
+        <v>310</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>201</v>
+        <v>311</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>202</v>
+        <v>312</v>
       </c>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:7" ht="409.6">
-      <c r="A56" s="8" t="s">
-        <v>43</v>
+    <row r="56" spans="1:7" ht="187">
+      <c r="A56" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>203</v>
+        <v>117</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>204</v>
+        <v>118</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>205</v>
+        <v>166</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>206</v>
+        <v>167</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="255">
-      <c r="A57" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3" t="s">
-        <v>208</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="4" customFormat="1" ht="409.6">
+      <c r="A57" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="G57" s="3"/>
-    </row>
-    <row r="58" spans="1:7" ht="121" customHeight="1">
-      <c r="A58" s="8" t="s">
-        <v>43</v>
+        <v>170</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" ht="20">
+      <c r="A58" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2" t="s">
-        <v>211</v>
+        <v>110</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>212</v>
+        <v>111</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>213</v>
+        <v>112</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>214</v>
+        <v>113</v>
       </c>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:7" ht="215" customHeight="1">
-      <c r="A59" s="8" t="s">
-        <v>37</v>
+    <row r="59" spans="1:7" ht="102">
+      <c r="A59" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E59" s="2"/>
       <c r="F59" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="102">
-      <c r="A60" s="8"/>
+        <v>116</v>
+      </c>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" ht="121" customHeight="1">
+      <c r="A60" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>163</v>
+        <v>315</v>
       </c>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:7" ht="221">
-      <c r="A61" s="8"/>
+    <row r="61" spans="1:7" ht="215" customHeight="1">
+      <c r="A61" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>219</v>
+        <v>320</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>220</v>
+        <v>321</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>221</v>
+        <v>322</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="1:7" ht="153">
-      <c r="A62" s="8"/>
+        <v>323</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="221">
+      <c r="A62" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
-        <v>47</v>
+        <v>325</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>46</v>
+        <v>326</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>306</v>
-      </c>
+        <v>327</v>
+      </c>
+      <c r="F62" s="2"/>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" spans="1:7" ht="187">
-      <c r="A63" s="8"/>
+    <row r="63" spans="1:7" ht="153">
+      <c r="A63" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>196</v>
+        <v>328</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>194</v>
+        <v>329</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>195</v>
+        <v>330</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>298</v>
+        <v>331</v>
       </c>
       <c r="G63" s="2"/>
     </row>
-    <row r="64" spans="1:7" ht="51">
-      <c r="A64" s="8"/>
+    <row r="64" spans="1:7" ht="187">
+      <c r="A64" s="7" t="s">
+        <v>348</v>
+      </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
-        <v>48</v>
+        <v>349</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2" t="s">
-        <v>50</v>
-      </c>
+        <v>350</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F64" s="2"/>
       <c r="G64" s="2"/>
     </row>
-    <row r="65" spans="1:7" ht="409.6">
-      <c r="A65" s="8"/>
+    <row r="65" spans="1:7" ht="68">
+      <c r="A65" s="7" t="s">
+        <v>342</v>
+      </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" ht="85">
+      <c r="A66" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="102">
+      <c r="A67" s="7"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" ht="153">
+      <c r="A68" s="7"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" ht="51">
+      <c r="A69" s="7"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" ht="409.6">
+      <c r="A70" s="7"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2" t="s">
+      <c r="E70" s="2"/>
+      <c r="F70" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G65" s="2"/>
-    </row>
-    <row r="66" spans="1:7" ht="19">
-      <c r="A66" s="9"/>
-      <c r="G66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" ht="19">
-      <c r="A67" s="8"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-    </row>
-    <row r="68" spans="1:7" ht="19">
-      <c r="A68" s="8"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-    </row>
-    <row r="69" spans="1:7" ht="19">
-      <c r="A69" s="8"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-    </row>
-    <row r="70" spans="1:7" ht="19">
-      <c r="A70" s="8"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
       <c r="G70" s="2"/>
     </row>
-    <row r="71" spans="1:7" ht="20">
-      <c r="A71" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2" t="s">
-        <v>93</v>
+    <row r="71" spans="1:7" ht="170">
+      <c r="A71" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>356</v>
       </c>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="1:7" ht="221">
-      <c r="A72" s="8"/>
+    <row r="72" spans="1:7" ht="68">
+      <c r="A72" s="10" t="s">
+        <v>352</v>
+      </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>94</v>
+        <v>357</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="19">
-      <c r="A73" s="8"/>
+        <v>358</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="1:7" ht="102">
+      <c r="A73" s="10" t="s">
+        <v>352</v>
+      </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
+        <v>360</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F73" s="2"/>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="1:7" ht="19">
-      <c r="A74" s="8"/>
+    <row r="74" spans="1:7" ht="356">
+      <c r="A74" s="10" t="s">
+        <v>352</v>
+      </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>104</v>
+        <v>363</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="F74" s="2"/>
       <c r="G74" s="2"/>
     </row>
     <row r="75" spans="1:7" ht="19">
-      <c r="A75" s="8"/>
+      <c r="A75" s="7"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
@@ -4094,386 +4730,386 @@
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="1:7" ht="19">
-      <c r="A76" s="8"/>
+    <row r="76" spans="1:7" ht="20">
+      <c r="A76" s="7" t="s">
+        <v>90</v>
+      </c>
       <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
+      <c r="C76" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
+      <c r="F76" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="1:7" ht="19">
-      <c r="A77" s="8"/>
+    <row r="77" spans="1:7" s="4" customFormat="1" ht="221">
+      <c r="A77" s="7"/>
       <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
+      <c r="C77" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-    </row>
-    <row r="78" spans="1:7" ht="289">
-      <c r="A78" s="8" t="s">
-        <v>107</v>
-      </c>
+      <c r="F77" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" s="4" customFormat="1" ht="19">
+      <c r="A78" s="7"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="153">
-      <c r="A79" s="8"/>
+        <v>96</v>
+      </c>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" spans="1:7" s="4" customFormat="1" ht="19">
+      <c r="A79" s="7"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
-        <v>250</v>
+        <v>104</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>262</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="E79" s="2"/>
       <c r="F79" s="2" t="s">
-        <v>254</v>
+        <v>106</v>
       </c>
       <c r="G79" s="2"/>
     </row>
-    <row r="80" spans="1:7" ht="68">
-      <c r="A80" s="8"/>
+    <row r="80" spans="1:7" s="4" customFormat="1" ht="19">
+      <c r="A80" s="7"/>
       <c r="B80" s="2"/>
-      <c r="C80" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>255</v>
-      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
       <c r="G80" s="2"/>
     </row>
-    <row r="81" spans="1:7" ht="153">
-      <c r="A81" s="8"/>
+    <row r="81" spans="1:7" ht="22" customHeight="1">
+      <c r="A81" s="7"/>
       <c r="B81" s="2"/>
-      <c r="C81" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>257</v>
-      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
       <c r="G81" s="2"/>
     </row>
-    <row r="82" spans="1:7" ht="19">
-      <c r="A82" s="8"/>
+    <row r="82" spans="1:7" ht="409" customHeight="1">
+      <c r="A82" s="7"/>
       <c r="B82" s="2"/>
-      <c r="C82" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
     </row>
-    <row r="83" spans="1:7" ht="136">
-      <c r="A83" s="8" t="s">
-        <v>173</v>
+    <row r="83" spans="1:7" ht="289">
+      <c r="A83" s="7" t="s">
+        <v>249</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
-        <v>173</v>
+        <v>249</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="85">
-      <c r="A84" s="8"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="153">
+      <c r="A84" s="7"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
-        <v>173</v>
+        <v>249</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="G84" s="2"/>
     </row>
-    <row r="85" spans="1:7" ht="102">
-      <c r="A85" s="8"/>
+    <row r="85" spans="1:7" ht="68">
+      <c r="A85" s="7"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2" t="s">
-        <v>173</v>
+        <v>249</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>175</v>
+        <v>262</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="G85" s="2"/>
     </row>
-    <row r="86" spans="1:7" s="4" customFormat="1" ht="170">
-      <c r="A86" s="8"/>
+    <row r="86" spans="1:7" ht="153">
+      <c r="A86" s="7"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
-        <v>173</v>
+        <v>249</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>176</v>
+        <v>255</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="G86" s="2"/>
     </row>
-    <row r="87" spans="1:7" s="4" customFormat="1" ht="119">
-      <c r="A87" s="8"/>
+    <row r="87" spans="1:7" ht="19">
+      <c r="A87" s="7"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+    </row>
+    <row r="88" spans="1:7" ht="136">
+      <c r="A88" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G88" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" s="4" customFormat="1" ht="306">
-      <c r="A88" s="8"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="G88" s="3"/>
-    </row>
-    <row r="89" spans="1:7" s="4" customFormat="1" ht="34">
-      <c r="A89" s="8"/>
-      <c r="B89" s="3"/>
+    </row>
+    <row r="89" spans="1:7" ht="85">
+      <c r="A89" s="7"/>
+      <c r="B89" s="2"/>
       <c r="C89" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="G89" s="3"/>
-    </row>
-    <row r="90" spans="1:7" ht="22" customHeight="1">
-      <c r="A90" s="8"/>
-      <c r="B90" s="3"/>
+        <v>172</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G89" s="2"/>
+    </row>
+    <row r="90" spans="1:7" ht="102">
+      <c r="A90" s="7"/>
+      <c r="B90" s="2"/>
       <c r="C90" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="F90" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G90" s="2"/>
+    </row>
+    <row r="91" spans="1:7" ht="170">
+      <c r="A91" s="7"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="G90" s="3"/>
-    </row>
-    <row r="91" spans="1:7" ht="409" customHeight="1">
-      <c r="A91" s="8"/>
-      <c r="B91" s="3"/>
-      <c r="C91" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="G91" s="3"/>
-    </row>
-    <row r="92" spans="1:7" ht="34">
-      <c r="A92" s="8"/>
+      <c r="G91" s="2"/>
+    </row>
+    <row r="92" spans="1:7" ht="119">
+      <c r="A92" s="7"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>279</v>
+        <v>176</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>281</v>
+        <v>177</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="409.6">
-      <c r="A93" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="B93" s="2"/>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="306">
+      <c r="A93" s="7"/>
+      <c r="B93" s="3"/>
       <c r="C93" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="G93" s="2"/>
-    </row>
-    <row r="94" spans="1:7" ht="19">
-      <c r="A94" s="8"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="2"/>
-    </row>
-    <row r="95" spans="1:7" ht="19">
-      <c r="A95" s="8"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-      <c r="G95" s="2"/>
-    </row>
-    <row r="96" spans="1:7" ht="119">
-      <c r="A96" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="B96" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="G93" s="3"/>
+    </row>
+    <row r="94" spans="1:7" ht="34">
+      <c r="A94" s="7"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G94" s="3"/>
+    </row>
+    <row r="95" spans="1:7" ht="170">
+      <c r="A95" s="7"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="G95" s="3"/>
+    </row>
+    <row r="96" spans="1:7" ht="187">
+      <c r="A96" s="7"/>
+      <c r="B96" s="3"/>
       <c r="C96" s="2" t="s">
-        <v>285</v>
+        <v>172</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="G96" s="2"/>
-    </row>
-    <row r="97" spans="1:7" ht="19">
-      <c r="A97" s="8"/>
+        <v>247</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G96" s="3"/>
+    </row>
+    <row r="97" spans="1:7" ht="34">
+      <c r="A97" s="7"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2" t="s">
-        <v>283</v>
+        <v>180</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-    </row>
-    <row r="98" spans="1:7" ht="19">
-      <c r="A98" s="8"/>
+        <v>278</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="409.6">
+      <c r="A98" s="7" t="s">
+        <v>258</v>
+      </c>
       <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
+      <c r="C98" s="2" t="s">
+        <v>257</v>
+      </c>
       <c r="D98" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
+        <v>275</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>277</v>
+      </c>
       <c r="G98" s="2"/>
     </row>
-    <row r="99" spans="1:7" ht="20">
-      <c r="A99" s="8" t="s">
-        <v>59</v>
-      </c>
+    <row r="99" spans="1:7" ht="19">
+      <c r="A99" s="7"/>
       <c r="B99" s="2"/>
-      <c r="C99" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
       <c r="E99" s="2"/>
-      <c r="F99" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="F99" s="2"/>
       <c r="G99" s="2"/>
     </row>
     <row r="100" spans="1:7" ht="19">
-      <c r="A100" s="8"/>
+      <c r="A100" s="7"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -4481,62 +5117,68 @@
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
     </row>
-    <row r="101" spans="1:7" ht="19">
-      <c r="A101" s="8"/>
+    <row r="101" spans="1:7" ht="102">
+      <c r="A101" s="7" t="s">
+        <v>281</v>
+      </c>
       <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
+      <c r="C101" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>287</v>
+      </c>
       <c r="G101" s="2"/>
     </row>
     <row r="102" spans="1:7" ht="19">
-      <c r="A102" s="8"/>
+      <c r="A102" s="7"/>
       <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
+      <c r="C102" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>283</v>
+      </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" ht="20">
-      <c r="A103" s="8" t="s">
-        <v>99</v>
-      </c>
+    <row r="103" spans="1:7" ht="19">
+      <c r="A103" s="7"/>
       <c r="B103" s="2"/>
-      <c r="C103" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="C103" s="2"/>
       <c r="D103" s="2" t="s">
-        <v>97</v>
+        <v>259</v>
       </c>
       <c r="E103" s="2"/>
-      <c r="F103" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="187">
-      <c r="A104" s="8"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+    </row>
+    <row r="104" spans="1:7" ht="20">
+      <c r="A104" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="B104" s="2"/>
       <c r="C104" s="2" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>198</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="G104" s="2"/>
     </row>
     <row r="105" spans="1:7" ht="19">
-      <c r="A105" s="8"/>
+      <c r="A105" s="7"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
@@ -4544,10 +5186,8 @@
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
     </row>
-    <row r="106" spans="1:7" ht="20">
-      <c r="A106" s="8" t="s">
-        <v>125</v>
-      </c>
+    <row r="106" spans="1:7" ht="19">
+      <c r="A106" s="7"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
@@ -4556,7 +5196,7 @@
       <c r="G106" s="2"/>
     </row>
     <row r="107" spans="1:7" ht="19">
-      <c r="A107" s="8"/>
+      <c r="A107" s="7"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
@@ -4564,16 +5204,81 @@
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
     </row>
-    <row r="108" spans="1:7" ht="40">
-      <c r="A108" s="8" t="s">
-        <v>126</v>
+    <row r="108" spans="1:7" ht="20">
+      <c r="A108" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-      <c r="D108" s="2"/>
+      <c r="C108" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
+      <c r="F108" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="187">
+      <c r="A109" s="7"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="19">
+      <c r="A110" s="7"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+    </row>
+    <row r="111" spans="1:7" ht="20">
+      <c r="A111" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+    </row>
+    <row r="112" spans="1:7" ht="19">
+      <c r="A112" s="7"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+    </row>
+    <row r="113" spans="1:7" ht="40">
+      <c r="A113" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added MaxPathSum algo details on PracticedAlgorithms.xlsx
</commit_message>
<xml_diff>
--- a/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
+++ b/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asheshsingh/Documents/workspace-sts-3.9.6.RELEASE/java-projects/DataStructures/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2111C74-2461-AB4B-9337-0598C09394EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54547E3C-8C7F-6146-92D6-3F92AB1F53ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="460" windowWidth="33600" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="370">
   <si>
     <t>Data Structure</t>
   </si>
@@ -672,9 +672,6 @@
   </si>
   <si>
     <t>MaxPathSum</t>
-  </si>
-  <si>
-    <t>Note: This is similar to print all nodes, except that here we need to return sum and there we just had to print the nodes</t>
   </si>
   <si>
     <t>Solution:
@@ -1147,26 +1144,9 @@
     <t>Count Leaf Nodes</t>
   </si>
   <si>
-    <t>1) Check if root is null, return 0.
-2) Define two methods, isLeaf(Node n) and countLeaves(Node n). isLeaf will check if both the children of a node is null, it will return true, else false.
-3) In countLeaves, first check if n is a leaf node, return 1. We are going to call this method recursively, so this serves as the breaking condition.
-4) Define two variables, numLeftLeafNodes and numRightLeafNodes.
-5) Check if n != null and n.getLeftNode() != null. If so, call the same method with n.getLeftNode() as argument and assign the results to numLeftLeafNodes.
-6) Do the reverse for right node.
-7) Return the sum of numLeftLeafNodes and numRightLeafNodes.</t>
-  </si>
-  <si>
     <t>Add sorted data to a BST: public Node addSorted(int [] data, int start, int end)</t>
   </si>
   <si>
-    <t>1) Create a method addSorted with arguments that take a sorted array, start and end indices. This method returns Node object, which will be the root of the BST formed.
-2) Code everything under a condition if(start &lt;= end). This also serves as breaking condition when this method is called recursively.
-3) Get mid point of start and add that data from array to create root node, call that newNode, which we will return before if loop ends.
-4) Before we return the node, call this method recursively, once with argument: data, start, mid-1, assign that result to leftNode variable of type Node and then with argument data, mid+1, end and assign that resule to rightNode variable.
-5) Above wil allow each node of left and right subtree to be populated and we return root  of main BST formed via newNode variabe.
-6) Outside the if loop, return null since start was sent as more than end, so we can't do anything.</t>
-  </si>
-  <si>
     <t>LinkedList</t>
   </si>
   <si>
@@ -1225,9 +1205,6 @@
   </si>
   <si>
     <t>Count number of nodes in a BST.</t>
-  </si>
-  <si>
-    <t>If you are given an array which is already sorted. How can you most add the data to a BST in a most effifient way?</t>
   </si>
   <si>
     <t>Create a Queue from a Circular Array</t>
@@ -1257,15 +1234,6 @@
 5d) Once while loop is done, assign newCapacity to capacity, head to zero, tail to pos and arr to newArr and you're done!</t>
   </si>
   <si>
-    <t>sum()</t>
-  </si>
-  <si>
-    <t>Get sum of all nodes.</t>
-  </si>
-  <si>
-    <t>Similar to print(), maintain a variable and keep on getting the sum in that variable.</t>
-  </si>
-  <si>
     <t>Stacks</t>
   </si>
   <si>
@@ -3320,6 +3288,287 @@
       </rPr>
       <t xml:space="preserve"> since it goes to extreme left (shortest element of a BST tree), prints that, then goes to parent where this method call stack came from, prints that one, goes to right child, and so on. This is why it is called inOrder traversing.</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Check if root is null, return 0.
+2) Define two methods, isLeaf(Node n) and countLeaves(Node n). isLeaf will check if both the children of a node is null, it will return true, else false.
+3) In countLeaves, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>first check if n is a leaf node, return 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. We are going to call this method recursively, so this serves as the breaking condition.
+4) Define two variables, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>numLeftLeafNodes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>numRightLeafNodes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+5) Check if n != null and n.getLeftNode() != null. If so, call the same method with n.getLeftNode() as argument and assign the results to numLeftLeafNodes.
+6) Do the reverse for right node.
+7) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Return</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sum of numLeftLeafNodes and numRightLeafNodes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>If you are given an array which is already sorted. How can you add the data to a BST in a most effifient way?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) Create a method addSorted inside the Node class itself (which we will call from BST class after doing null / empty checks on input sorted array) with arguments that take a sorted array, start and end indices. This method returns Node object, which will be the root of the BST formed.
+2) Code everything under a condition if(start &lt;= end). This also serves as breaking condition when this method is called recursively.
+3) Get mid point of start and end indices and use the array data at mid to create root node, call that newNode, which we will return before if loop ends.
+4) Before we return the node, call this method recursively, once with argument: data, start, mid-1, assign that result to leftNode variable of type Node and then with argument data, mid+1, end and assign that resule to rightNode variable. E.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>newNode.leftNode = addSorted(data, start, mid-1);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+5) Above wil allow each node of left and right subtree to be populated and we return root  of main BST formed via newNode variabe.
+6) Outside the if loop, return null since start was sent as more than end, so we can't do anything.</t>
+    </r>
+  </si>
+  <si>
+    <t>BinarySearchTree - geeksforgeeks-Top10</t>
+  </si>
+  <si>
+    <t>int maxPathSum(Node n)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Given a binary tree (not BST!), find the maximum path sum. The path may start and end at any node in the tree.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> It is not about computing sum of all the nodes, it is about summing all the nodes with max results, start from where you want and end where you want, as long as you don't bypass a node to get to next one.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :
+	 *        1
+	 *       / \
+	 *      2  -13
+	 *     / \     \
+	 *  -4   3     3
+Output: 3 + 2 + 1 = 6, since you include nodes will -4 or -13 or since 3 comes after -13, your path sum will go lower
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: if we change the right most node from 3 to 14, then the max path will be 3+2+1-13+14 since now the max path of node -13 becomes +1 (-13 + 14), currently it is -10 (-13 + 3)
+Another good test case in above binary tree could be that if for a node, both left and right nodes have negative max paths, then do not take either of the children, just take node's own data as max path for that node. For example, if we replace left child of root, 2 to -4, then for root, max paths of both the children will be negative, so max path of root will be its own data, without considering any child, i.e. 3.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Solution:
+1) Define two methods: a) int maxPathSum(Node n) and b) maxPathSumForNode(Node n). We'll use a) for Root since that is special, we will have to consider the route all the way from left subtree -&gt; root -&gt; right subtree. We will use b) to compute max path sum for left and right subtrees.
+2) For a) int maxPathSum(Node n), check if supplied root is null, return 0. Define two variables, maxPathLeft and maxPathRight. First one will be set by method call (maxPathSumForNode(Node n)) by passing left child of the root. Do similar work to compute max path sum for right subtree.
+3) Check if max path sum from both, the left and right subtrees come negative, return root.getData();
+4) Return root.getData() + maxPathSum from left or right, whichever is bigger + smaller maxPathSum, as long as it is not negative. Following will do the trick for you: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>return maxPathLeft &gt; maxPathRight ?
+				maxPathLeft + n.getData() + (maxPathRight &gt; 0 ? maxPathRight : 0)
+				: maxPathRight + n.getData() + (maxPathLeft &gt; 0 ? maxPathLeft : 0);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+5) For second method:  maxPathSumForNode(Node n), which we need to compute max path sums for left and right subtrees, we are going to call it recursively and return bigger of max path sum for left and right children. For breaking condition, it will if (n == null), return 0. Here as well we define two variables, like method a) as int maxPathLeft (= maxPathSumForNode(n.getLeftNode());) and maxPathRight. Finally, one check, if both sides of max path sum are negative, return 0, and then </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>return Math.max(maxPathLeft, maxPathRight) + n.getData();</t>
+    </r>
+  </si>
+  <si>
+    <t>Important part to note here, is Root is special, route can go all the way from left subtree -&gt; root -&gt; right subtree, so we need to include the lower max path sum among two subtrees too, as long as positive, but while computing max path sum for left or right subtree, we will have only one path, either left or right subtree of that child node.</t>
   </si>
 </sst>
 </file>
@@ -3844,8 +4093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C93" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3915,7 +4164,7 @@
     </row>
     <row r="4" spans="1:7" ht="272">
       <c r="A4" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -3928,7 +4177,7 @@
         <v>150</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>8</v>
@@ -3936,7 +4185,7 @@
     </row>
     <row r="5" spans="1:7" ht="83" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -3957,7 +4206,7 @@
     </row>
     <row r="6" spans="1:7" ht="83" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -3967,16 +4216,16 @@
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="187">
       <c r="A7" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -3992,12 +4241,12 @@
         <v>149</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="51">
       <c r="A8" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -4016,7 +4265,7 @@
     </row>
     <row r="9" spans="1:7" ht="34">
       <c r="A9" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4031,7 +4280,7 @@
     </row>
     <row r="10" spans="1:7" ht="20">
       <c r="A10" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4046,7 +4295,7 @@
     </row>
     <row r="11" spans="1:7" ht="34">
       <c r="A11" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -4063,7 +4312,7 @@
     </row>
     <row r="12" spans="1:7" ht="68">
       <c r="A12" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4080,7 +4329,7 @@
     </row>
     <row r="13" spans="1:7" ht="102">
       <c r="A13" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4097,7 +4346,7 @@
     </row>
     <row r="14" spans="1:7" ht="34">
       <c r="A14" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -4114,7 +4363,7 @@
     </row>
     <row r="15" spans="1:7" ht="34">
       <c r="A15" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
@@ -4131,7 +4380,7 @@
     </row>
     <row r="16" spans="1:7" ht="34">
       <c r="A16" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
@@ -4146,7 +4395,7 @@
     </row>
     <row r="17" spans="1:7" ht="34">
       <c r="A17" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
@@ -4163,7 +4412,7 @@
     </row>
     <row r="18" spans="1:7" ht="102">
       <c r="A18" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -4176,15 +4425,15 @@
         <v>119</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="221">
       <c r="A19" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
@@ -4203,7 +4452,7 @@
     </row>
     <row r="20" spans="1:7" ht="85">
       <c r="A20" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -4213,18 +4462,18 @@
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>136</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="187">
       <c r="A21" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
@@ -4234,56 +4483,56 @@
         <v>138</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="136">
       <c r="A22" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="238">
       <c r="A23" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="34">
       <c r="A24" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -4304,7 +4553,7 @@
     </row>
     <row r="25" spans="1:7" ht="153">
       <c r="A25" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
@@ -4317,7 +4566,7 @@
         <v>143</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>152</v>
@@ -4325,47 +4574,47 @@
     </row>
     <row r="26" spans="1:7" ht="170">
       <c r="A26" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" ht="289">
       <c r="A27" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="51">
       <c r="A28" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
@@ -4384,7 +4633,7 @@
     </row>
     <row r="29" spans="1:7" ht="20">
       <c r="A29" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
@@ -4401,7 +4650,7 @@
     </row>
     <row r="30" spans="1:7" ht="299" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
@@ -4422,7 +4671,7 @@
     </row>
     <row r="31" spans="1:7" ht="293" customHeight="1">
       <c r="A31" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
@@ -4443,7 +4692,7 @@
     </row>
     <row r="32" spans="1:7" ht="20">
       <c r="A32" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
@@ -4460,7 +4709,7 @@
     </row>
     <row r="33" spans="1:7" ht="20">
       <c r="A33" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
@@ -4477,24 +4726,24 @@
     </row>
     <row r="34" spans="1:7" ht="136">
       <c r="A34" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" ht="85">
       <c r="A35" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
@@ -4504,112 +4753,112 @@
         <v>127</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" ht="221">
       <c r="A36" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" ht="187">
       <c r="A37" s="7" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" ht="289">
       <c r="A38" s="9" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="187">
       <c r="A39" s="9" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="187">
       <c r="A40" s="9" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="372">
@@ -4618,7 +4867,7 @@
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>31</v>
@@ -4627,7 +4876,7 @@
         <v>151</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>153</v>
@@ -4639,16 +4888,16 @@
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="F42" s="2" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="G42" s="2"/>
     </row>
@@ -4658,7 +4907,7 @@
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>31</v>
@@ -4667,7 +4916,7 @@
         <v>151</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>153</v>
@@ -4679,16 +4928,16 @@
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="F44" s="2" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="G44" s="2"/>
     </row>
@@ -4726,16 +4975,16 @@
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="G47" s="2"/>
     </row>
@@ -4745,16 +4994,16 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="F48" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G48" s="2"/>
     </row>
@@ -4770,10 +5019,10 @@
         <v>45</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G49" s="2"/>
     </row>
@@ -4783,16 +5032,16 @@
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="G50" s="2"/>
     </row>
@@ -4802,19 +5051,19 @@
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="255">
@@ -4823,16 +5072,16 @@
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="G52" s="3"/>
     </row>
@@ -4842,16 +5091,16 @@
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="G53" s="2"/>
     </row>
@@ -4870,10 +5119,10 @@
         <v>165</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="388">
@@ -4882,16 +5131,16 @@
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="G55" s="2"/>
     </row>
@@ -4928,10 +5177,10 @@
         <v>170</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G57" s="2"/>
     </row>
@@ -4986,7 +5235,7 @@
         <v>171</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G60" s="2"/>
     </row>
@@ -4996,19 +5245,19 @@
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="221">
@@ -5017,13 +5266,13 @@
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
@@ -5034,50 +5283,50 @@
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="G63" s="2"/>
     </row>
     <row r="64" spans="1:7" ht="187">
       <c r="A64" s="7" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
     </row>
     <row r="65" spans="1:7" ht="68">
       <c r="A65" s="7" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="G65" s="2"/>
     </row>
@@ -5129,10 +5378,10 @@
         <v>46</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="G68" s="2"/>
     </row>
@@ -5168,69 +5417,69 @@
     </row>
     <row r="71" spans="1:7" ht="170">
       <c r="A71" s="10" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="F71" s="12" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="G71" s="2"/>
     </row>
     <row r="72" spans="1:7" ht="68">
       <c r="A72" s="10" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
     </row>
     <row r="73" spans="1:7" ht="102">
       <c r="A73" s="10" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
     </row>
     <row r="74" spans="1:7" ht="356">
       <c r="A74" s="10" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
@@ -5272,7 +5521,7 @@
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>103</v>
@@ -5333,20 +5582,20 @@
     </row>
     <row r="83" spans="1:7" ht="289">
       <c r="A83" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>109</v>
@@ -5354,64 +5603,64 @@
     </row>
     <row r="84" spans="1:7" ht="153">
       <c r="A84" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="G84" s="2"/>
     </row>
     <row r="85" spans="1:7" ht="68">
       <c r="A85" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="G85" s="2"/>
     </row>
     <row r="86" spans="1:7" ht="204">
       <c r="A86" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="E86" s="2" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="G86" s="2"/>
     </row>
     <row r="87" spans="1:7" ht="340">
       <c r="A87" s="7" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
@@ -5421,10 +5670,10 @@
         <v>108</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="G87" s="2"/>
     </row>
@@ -5437,16 +5686,16 @@
         <v>172</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="85">
@@ -5458,13 +5707,13 @@
         <v>172</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="G89" s="2"/>
     </row>
@@ -5480,10 +5729,10 @@
         <v>173</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="G90" s="2"/>
     </row>
@@ -5499,10 +5748,10 @@
         <v>174</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="G91" s="2"/>
     </row>
@@ -5518,7 +5767,7 @@
         <v>175</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>176</v>
@@ -5539,10 +5788,10 @@
         <v>178</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G93" s="3"/>
     </row>
@@ -5555,13 +5804,13 @@
         <v>172</v>
       </c>
       <c r="D94" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="F94" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="G94" s="3"/>
     </row>
@@ -5574,17 +5823,17 @@
         <v>172</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>241</v>
+        <v>362</v>
       </c>
       <c r="G95" s="3"/>
     </row>
-    <row r="96" spans="1:7" ht="187">
+    <row r="96" spans="1:7" ht="221">
       <c r="A96" s="7" t="s">
         <v>172</v>
       </c>
@@ -5593,53 +5842,53 @@
         <v>172</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>264</v>
+        <v>363</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>243</v>
+        <v>364</v>
       </c>
       <c r="G96" s="3"/>
     </row>
-    <row r="97" spans="1:7" ht="40">
+    <row r="97" spans="1:7" ht="388">
       <c r="A97" s="7" t="s">
-        <v>172</v>
+        <v>365</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2" t="s">
         <v>179</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>268</v>
+        <v>366</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>269</v>
+        <v>367</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>270</v>
+        <v>368</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>180</v>
+        <v>369</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="409.6">
       <c r="A98" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="G98" s="2"/>
     </row>
@@ -5663,20 +5912,20 @@
     </row>
     <row r="101" spans="1:7" ht="102">
       <c r="A101" s="7" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="G101" s="2"/>
     </row>
@@ -5684,10 +5933,10 @@
       <c r="A102" s="7"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
@@ -5698,7 +5947,7 @@
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
@@ -5778,10 +6027,10 @@
       </c>
       <c r="E109" s="2"/>
       <c r="F109" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G109" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="G109" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="19">

</xml_diff>

<commit_message>
Added some more practiced algorithms
</commit_message>
<xml_diff>
--- a/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
+++ b/DataStructures/src/main/resources/PracticedAlgorithms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asheshsingh/Documents/workspace-sts-3.9.6.RELEASE/java-projects/DataStructures/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashesh/Documents/workspace-sts-3.9.6.RELEASE/java-projects/DataStructures/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54547E3C-8C7F-6146-92D6-3F92AB1F53ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686EAEF8-1E13-2149-A25D-0828910D597E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="371">
   <si>
     <t>Data Structure</t>
   </si>
@@ -686,12 +686,6 @@
   </si>
   <si>
     <t>Given an integer array with range of data, find all elements which are less than both its neighbors. For 1st element, it has to less than next element and for last element that has to be less then the previous element.</t>
-  </si>
-  <si>
-    <t>This is a very simple algorithm. Only trick here is boundary conditions on both ends of the array. Following if statement can help get along with it in clean way:
-if ((i == 0) || (arr[i] &lt; arr[i-1]) &amp;&amp; ((I == len-1) || (arr[i] &lt; arr[i+1] ))) {
-    // increment count or populate your result with this array element
-}</t>
   </si>
   <si>
     <t>Reverse a given integer.</t>
@@ -3570,12 +3564,21 @@
   <si>
     <t>Important part to note here, is Root is special, route can go all the way from left subtree -&gt; root -&gt; right subtree, so we need to include the lower max path sum among two subtrees too, as long as positive, but while computing max path sum for left or right subtree, we will have only one path, either left or right subtree of that child node.</t>
   </si>
+  <si>
+    <t>Given a number as string, convert it to integer</t>
+  </si>
+  <si>
+    <t>This is a very simple algorithm. Only trick here is boundary conditions on both ends of the array. Following if statement can help get along with it in clean way:
+if ((i == 0) || (arr[i] &lt; arr[i-1]) &amp;&amp; ((i == len-1) || (arr[i] &lt; arr[i+1] ))) {
+    // increment count or populate your result with this array element
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3588,6 +3591,7 @@
       <sz val="18"/>
       <color rgb="FF002060"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3758,9 +3762,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3772,6 +3773,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="39">
@@ -4093,11 +4097,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="32.83203125" bestFit="1" customWidth="1"/>
@@ -4107,18 +4111,18 @@
     <col min="7" max="7" width="67.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" ht="21">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4141,7 +4145,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="33" customHeight="1">
+    <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>135</v>
       </c>
@@ -4154,7 +4158,9 @@
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>369</v>
+      </c>
       <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
@@ -4162,9 +4168,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="272">
+    <row r="4" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -4177,15 +4183,15 @@
         <v>150</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="83" customHeight="1">
+    <row r="5" spans="1:7" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -4204,9 +4210,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="83" customHeight="1">
+    <row r="6" spans="1:7" ht="83" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -4219,13 +4225,13 @@
         <v>181</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>182</v>
+        <v>370</v>
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="187">
+    <row r="7" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -4241,12 +4247,12 @@
         <v>149</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="51">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -4263,9 +4269,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="34">
+    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4278,9 +4284,9 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="20">
+    <row r="10" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4293,9 +4299,9 @@
       </c>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="34">
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -4310,9 +4316,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="68">
+    <row r="12" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4327,9 +4333,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="102">
+    <row r="13" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4344,9 +4350,9 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="34">
+    <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -4361,9 +4367,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="34">
+    <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
@@ -4378,9 +4384,9 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="34">
+    <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
@@ -4393,9 +4399,9 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="34">
+    <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
@@ -4410,9 +4416,9 @@
       </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="102">
+    <row r="18" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -4425,15 +4431,15 @@
         <v>119</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="221">
+    </row>
+    <row r="19" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
@@ -4450,9 +4456,9 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="85">
+    <row r="20" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -4462,18 +4468,18 @@
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>136</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="187">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
@@ -4483,56 +4489,56 @@
         <v>138</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>180</v>
       </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="136">
+    <row r="22" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="238">
+    <row r="23" spans="1:7" ht="238" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="34">
+    </row>
+    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -4551,9 +4557,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="153">
+    <row r="25" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
@@ -4566,55 +4572,55 @@
         <v>143</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="170">
+    <row r="26" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>284</v>
-      </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="289">
+    <row r="27" spans="1:7" ht="289" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="51">
+    </row>
+    <row r="28" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
@@ -4631,9 +4637,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="20">
+    <row r="29" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
@@ -4648,9 +4654,9 @@
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" ht="299" customHeight="1">
+    <row r="30" spans="1:7" ht="299" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
@@ -4669,9 +4675,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="293" customHeight="1">
+    <row r="31" spans="1:7" ht="293" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
@@ -4690,9 +4696,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="20">
+    <row r="32" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
@@ -4707,9 +4713,9 @@
       </c>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="20">
+    <row r="33" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
@@ -4724,26 +4730,26 @@
       </c>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" ht="136">
+    <row r="34" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" ht="85">
+    <row r="35" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
@@ -4753,121 +4759,121 @@
         <v>127</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="221">
+    <row r="36" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>218</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" ht="187">
+    <row r="37" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" ht="289">
-      <c r="A38" s="9" t="s">
-        <v>330</v>
+    <row r="38" spans="1:7" ht="289" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>329</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="187">
-      <c r="A39" s="9" t="s">
-        <v>330</v>
+    </row>
+    <row r="39" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>329</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="187">
-      <c r="A40" s="9" t="s">
-        <v>330</v>
+    </row>
+    <row r="40" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>329</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="372">
+    </row>
+    <row r="41" spans="1:7" ht="372" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>31</v>
@@ -4876,38 +4882,38 @@
         <v>151</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="323">
+    <row r="42" spans="1:7" ht="323" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="F42" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" ht="372">
+    <row r="43" spans="1:7" ht="372" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>31</v>
@@ -4916,32 +4922,32 @@
         <v>151</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="323">
+    <row r="44" spans="1:7" ht="323" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>188</v>
-      </c>
       <c r="F44" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="1:7" ht="102">
+    <row r="45" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
@@ -4960,7 +4966,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="19">
+    <row r="46" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -4969,45 +4975,45 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="1:7" ht="356">
+    <row r="47" spans="1:7" ht="356" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="1:7" ht="255">
+    <row r="48" spans="1:7" ht="255" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="F48" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="1:7" ht="153">
+    <row r="49" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>43</v>
       </c>
@@ -5019,92 +5025,92 @@
         <v>45</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="1:7" ht="323">
+    <row r="50" spans="1:7" ht="306" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F50" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="1:7" ht="409.6">
+    <row r="51" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="255">
+    </row>
+    <row r="52" spans="1:7" ht="255" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E52" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="F52" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:7" ht="170">
+    <row r="53" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>211</v>
-      </c>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="1:7" ht="119">
+    <row r="54" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>4</v>
       </c>
@@ -5119,32 +5125,32 @@
         <v>165</v>
       </c>
       <c r="F54" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G54" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="G54" s="2" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="388">
+    </row>
+    <row r="55" spans="1:7" ht="388" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="F55" s="2" t="s">
-        <v>295</v>
-      </c>
       <c r="G55" s="2"/>
     </row>
-    <row r="56" spans="1:7" ht="187">
+    <row r="56" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>4</v>
       </c>
@@ -5165,7 +5171,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="4" customFormat="1" ht="409.6">
+    <row r="57" spans="1:7" s="4" customFormat="1" ht="388" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>4</v>
       </c>
@@ -5177,14 +5183,14 @@
         <v>170</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="1:7" ht="20">
+    <row r="58" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>4</v>
       </c>
@@ -5203,7 +5209,7 @@
       </c>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="1:7" ht="102">
+    <row r="59" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>4</v>
       </c>
@@ -5220,7 +5226,7 @@
       </c>
       <c r="G59" s="2"/>
     </row>
-    <row r="60" spans="1:7" ht="121" customHeight="1">
+    <row r="60" spans="1:7" ht="121" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>4</v>
       </c>
@@ -5235,102 +5241,102 @@
         <v>171</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="1:7" ht="215" customHeight="1">
+    <row r="61" spans="1:7" ht="215" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="G61" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="G61" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="221">
+    </row>
+    <row r="62" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>310</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
     </row>
-    <row r="63" spans="1:7" ht="153">
+    <row r="63" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F63" s="2" t="s">
-        <v>314</v>
-      </c>
       <c r="G63" s="2"/>
     </row>
-    <row r="64" spans="1:7" ht="187">
+    <row r="64" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>334</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
     </row>
-    <row r="65" spans="1:7" ht="68">
+    <row r="65" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>328</v>
-      </c>
       <c r="G65" s="2"/>
     </row>
-    <row r="66" spans="1:7" ht="85">
+    <row r="66" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>37</v>
       </c>
@@ -5351,7 +5357,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="102">
+    <row r="67" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A67" s="7"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2" t="s">
@@ -5368,7 +5374,7 @@
       </c>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="1:7" ht="153">
+    <row r="68" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A68" s="7"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
@@ -5378,14 +5384,14 @@
         <v>46</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G68" s="2"/>
     </row>
-    <row r="69" spans="1:7" ht="51">
+    <row r="69" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
@@ -5400,7 +5406,7 @@
       </c>
       <c r="G69" s="2"/>
     </row>
-    <row r="70" spans="1:7" ht="409.6">
+    <row r="70" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
@@ -5415,76 +5421,76 @@
       </c>
       <c r="G70" s="2"/>
     </row>
-    <row r="71" spans="1:7" ht="170">
-      <c r="A71" s="10" t="s">
+    <row r="71" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="C71" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="D71" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="D71" s="11" t="s">
+      <c r="E71" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="E71" s="12" t="s">
+      <c r="F71" s="11" t="s">
         <v>338</v>
       </c>
-      <c r="F71" s="12" t="s">
-        <v>339</v>
-      </c>
       <c r="G71" s="2"/>
     </row>
-    <row r="72" spans="1:7" ht="68">
-      <c r="A72" s="10" t="s">
-        <v>335</v>
+    <row r="72" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A72" s="9" t="s">
+        <v>334</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="E72" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>342</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
     </row>
-    <row r="73" spans="1:7" ht="102">
-      <c r="A73" s="10" t="s">
-        <v>335</v>
+    <row r="73" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A73" s="9" t="s">
+        <v>334</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="E73" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>345</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="1:7" ht="356">
-      <c r="A74" s="10" t="s">
-        <v>335</v>
+    <row r="74" spans="1:7" ht="356" x14ac:dyDescent="0.2">
+      <c r="A74" s="9" t="s">
+        <v>334</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>348</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="1:7" ht="19">
+    <row r="75" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A75" s="7"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -5493,7 +5499,7 @@
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="1:7" ht="20">
+    <row r="76" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
         <v>90</v>
       </c>
@@ -5510,7 +5516,7 @@
       </c>
       <c r="G76" s="2"/>
     </row>
-    <row r="77" spans="1:7" s="4" customFormat="1" ht="221">
+    <row r="77" spans="1:7" s="4" customFormat="1" ht="221" x14ac:dyDescent="0.2">
       <c r="A77" s="7"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2" t="s">
@@ -5521,13 +5527,13 @@
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="78" spans="1:7" s="4" customFormat="1" ht="19">
+    <row r="78" spans="1:7" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A78" s="7"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
@@ -5538,7 +5544,7 @@
       <c r="F78" s="6"/>
       <c r="G78" s="2"/>
     </row>
-    <row r="79" spans="1:7" s="4" customFormat="1" ht="19">
+    <row r="79" spans="1:7" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A79" s="7"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
@@ -5553,7 +5559,7 @@
       </c>
       <c r="G79" s="2"/>
     </row>
-    <row r="80" spans="1:7" s="4" customFormat="1" ht="19">
+    <row r="80" spans="1:7" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A80" s="7"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -5562,7 +5568,7 @@
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
     </row>
-    <row r="81" spans="1:7" ht="22" customHeight="1">
+    <row r="81" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="7"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -5571,7 +5577,7 @@
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
     </row>
-    <row r="82" spans="1:7" ht="409" customHeight="1">
+    <row r="82" spans="1:7" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="7"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -5580,87 +5586,87 @@
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
     </row>
-    <row r="83" spans="1:7" ht="289">
+    <row r="83" spans="1:7" ht="289" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D83" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>242</v>
-      </c>
       <c r="E83" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="153">
+    <row r="84" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G84" s="2"/>
     </row>
-    <row r="85" spans="1:7" ht="68">
+    <row r="85" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D85" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="E85" s="2" t="s">
-        <v>251</v>
-      </c>
       <c r="F85" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G85" s="2"/>
     </row>
-    <row r="86" spans="1:7" ht="204">
+    <row r="86" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E86" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="G86" s="2"/>
+    </row>
+    <row r="87" spans="1:7" ht="340" x14ac:dyDescent="0.2">
+      <c r="A87" s="7" t="s">
         <v>353</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="G86" s="2"/>
-    </row>
-    <row r="87" spans="1:7" ht="340">
-      <c r="A87" s="7" t="s">
-        <v>354</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
@@ -5670,14 +5676,14 @@
         <v>108</v>
       </c>
       <c r="E87" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="F87" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="F87" s="2" t="s">
-        <v>356</v>
-      </c>
       <c r="G87" s="2"/>
     </row>
-    <row r="88" spans="1:7" ht="136">
+    <row r="88" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>172</v>
       </c>
@@ -5686,19 +5692,19 @@
         <v>172</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F88" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="G88" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="G88" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="85">
+    </row>
+    <row r="89" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>172</v>
       </c>
@@ -5707,17 +5713,17 @@
         <v>172</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G89" s="2"/>
     </row>
-    <row r="90" spans="1:7" ht="102">
+    <row r="90" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
         <v>172</v>
       </c>
@@ -5729,14 +5735,14 @@
         <v>173</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G90" s="2"/>
     </row>
-    <row r="91" spans="1:7" ht="187">
+    <row r="91" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>172</v>
       </c>
@@ -5748,14 +5754,14 @@
         <v>174</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G91" s="2"/>
     </row>
-    <row r="92" spans="1:7" ht="119">
+    <row r="92" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
         <v>172</v>
       </c>
@@ -5767,7 +5773,7 @@
         <v>175</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>176</v>
@@ -5776,7 +5782,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="306">
+    <row r="93" spans="1:7" ht="306" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>172</v>
       </c>
@@ -5788,14 +5794,14 @@
         <v>178</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G93" s="3"/>
     </row>
-    <row r="94" spans="1:7" ht="34">
+    <row r="94" spans="1:7" ht="40" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>172</v>
       </c>
@@ -5804,17 +5810,17 @@
         <v>172</v>
       </c>
       <c r="D94" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="F94" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E94" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>238</v>
-      </c>
       <c r="G94" s="3"/>
     </row>
-    <row r="95" spans="1:7" ht="170">
+    <row r="95" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>172</v>
       </c>
@@ -5823,17 +5829,17 @@
         <v>172</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G95" s="3"/>
     </row>
-    <row r="96" spans="1:7" ht="221">
+    <row r="96" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>172</v>
       </c>
@@ -5842,57 +5848,57 @@
         <v>172</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E96" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="F96" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="F96" s="3" t="s">
+      <c r="G96" s="3"/>
+    </row>
+    <row r="97" spans="1:7" ht="388" x14ac:dyDescent="0.2">
+      <c r="A97" s="7" t="s">
         <v>364</v>
-      </c>
-      <c r="G96" s="3"/>
-    </row>
-    <row r="97" spans="1:7" ht="388">
-      <c r="A97" s="7" t="s">
-        <v>365</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2" t="s">
         <v>179</v>
       </c>
       <c r="D97" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E97" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E97" s="2" t="s">
+      <c r="F97" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="G97" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="G97" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="409.6">
+    </row>
+    <row r="98" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D98" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E98" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="E98" s="2" t="s">
+      <c r="F98" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="F98" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="G98" s="2"/>
     </row>
-    <row r="99" spans="1:7" ht="19">
+    <row r="99" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A99" s="7"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -5901,7 +5907,7 @@
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
     </row>
-    <row r="100" spans="1:7" ht="19">
+    <row r="100" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A100" s="7"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -5910,50 +5916,50 @@
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
     </row>
-    <row r="101" spans="1:7" ht="102">
+    <row r="101" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D101" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="E101" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="E101" s="2" t="s">
+      <c r="F101" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F101" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="G101" s="2"/>
     </row>
-    <row r="102" spans="1:7" ht="19">
+    <row r="102" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A102" s="7"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D102" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
     </row>
-    <row r="103" spans="1:7" ht="19">
+    <row r="103" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A103" s="7"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
       <c r="D103" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
     </row>
-    <row r="104" spans="1:7" ht="20">
+    <row r="104" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
         <v>59</v>
       </c>
@@ -5970,7 +5976,7 @@
       </c>
       <c r="G104" s="2"/>
     </row>
-    <row r="105" spans="1:7" ht="19">
+    <row r="105" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A105" s="7"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -5979,7 +5985,7 @@
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>
     </row>
-    <row r="106" spans="1:7" ht="19">
+    <row r="106" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A106" s="7"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -5988,7 +5994,7 @@
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
     </row>
-    <row r="107" spans="1:7" ht="19">
+    <row r="107" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A107" s="7"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -5997,7 +6003,7 @@
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
     </row>
-    <row r="108" spans="1:7" ht="20">
+    <row r="108" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
         <v>99</v>
       </c>
@@ -6016,7 +6022,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="187">
+    <row r="109" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A109" s="7"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2" t="s">
@@ -6027,13 +6033,13 @@
       </c>
       <c r="E109" s="2"/>
       <c r="F109" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G109" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="G109" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="19">
+    </row>
+    <row r="110" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A110" s="7"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -6042,7 +6048,7 @@
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
     </row>
-    <row r="111" spans="1:7" ht="20">
+    <row r="111" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
         <v>124</v>
       </c>
@@ -6053,7 +6059,7 @@
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
     </row>
-    <row r="112" spans="1:7" ht="19">
+    <row r="112" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A112" s="7"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -6062,7 +6068,7 @@
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
     </row>
-    <row r="113" spans="1:7" ht="40">
+    <row r="113" spans="1:7" ht="40" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
         <v>125</v>
       </c>

</xml_diff>